<commit_message>
feat: add null check for Excel cell modifications in cost processing
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BC909F-B7DE-4C75-88B8-A93E24467B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FA3B0-684B-43AB-9198-52AD0AC5392A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="2" r:id="rId1"/>
@@ -1789,92 +1789,113 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1882,60 +1903,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1946,12 +1913,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1963,82 +1924,121 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2612,8 +2612,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="59" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2638,55 +2638,55 @@
       <c r="A1" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="182" t="s">
+      <c r="B1" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="182"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="134"/>
+      <c r="E1" s="134"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="184" t="s">
+      <c r="C2" s="133"/>
+      <c r="D2" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="182" t="s">
+      <c r="B3" s="133" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="184"/>
+      <c r="C3" s="133"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
+      <c r="C4" s="131"/>
+      <c r="D4" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
+      <c r="E4" s="132"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2711,22 +2711,22 @@
       <c r="G6" s="106"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="116" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="186"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="187" t="s">
+      <c r="D7" s="118" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="186"/>
-      <c r="F7" s="188"/>
-      <c r="G7" s="189"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="120"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
-      <c r="C8" s="192"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="76" t="s">
         <v>58</v>
       </c>
@@ -2739,32 +2739,34 @@
       <c r="G8" s="107"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="124" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="195"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="196" t="s">
+      <c r="A10" s="127" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="197"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="71"/>
-      <c r="D10" s="113"/>
+      <c r="D10" s="113">
+        <v>0</v>
+      </c>
       <c r="E10" s="30"/>
       <c r="F10" s="70"/>
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2772,21 +2774,23 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="69"/>
-      <c r="D12" s="30"/>
+      <c r="D12" s="30">
+        <v>0</v>
+      </c>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="176" t="s">
+      <c r="A13" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="177"/>
+      <c r="B13" s="130"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2794,10 +2798,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="176" t="s">
+      <c r="A14" s="129" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="177"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2805,10 +2809,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="176" t="s">
+      <c r="A15" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="177"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2816,10 +2820,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="157" t="s">
+      <c r="A16" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="158"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
@@ -2829,10 +2833,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="167" t="s">
+      <c r="A17" s="136" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="168"/>
+      <c r="B17" s="137"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16+D15+D14+D13+D12+D11+D10</f>
@@ -2858,21 +2862,21 @@
       <c r="G18" s="108"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="172" t="s">
+      <c r="A19" s="138" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="173"/>
-      <c r="C19" s="173"/>
+      <c r="B19" s="139"/>
+      <c r="C19" s="139"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="174" t="s">
+      <c r="A20" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="175"/>
+      <c r="B20" s="141"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2882,12 +2886,14 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="178" t="s">
+      <c r="A21" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="179"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="55"/>
-      <c r="D21" s="30"/>
+      <c r="D21" s="30">
+        <v>0</v>
+      </c>
       <c r="E21" s="54"/>
       <c r="F21" s="54"/>
       <c r="G21" s="94">
@@ -2895,12 +2901,14 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="177"/>
+      <c r="B22" s="130"/>
       <c r="C22" s="86"/>
-      <c r="D22" s="30"/>
+      <c r="D22" s="30">
+        <v>0</v>
+      </c>
       <c r="E22" s="54"/>
       <c r="F22" s="54"/>
       <c r="G22" s="93">
@@ -2908,10 +2916,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="177"/>
+      <c r="B23" s="130"/>
       <c r="C23" s="53"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
@@ -2921,10 +2929,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="176" t="s">
+      <c r="A24" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="177"/>
+      <c r="B24" s="130"/>
       <c r="C24" s="53"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -2934,10 +2942,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="176" t="s">
+      <c r="A25" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="177"/>
+      <c r="B25" s="130"/>
       <c r="C25" s="104" t="s">
         <v>76</v>
       </c>
@@ -2949,10 +2957,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="157" t="s">
+      <c r="A26" s="114" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="158"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="52"/>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
@@ -2962,12 +2970,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="159" t="s">
+      <c r="A27" s="144" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="160"/>
+      <c r="B27" s="145"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="25"/>
+      <c r="D27" s="25">
+        <f>D20+D21+D22+D23-D24+D25-D26</f>
+        <v>0</v>
+      </c>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
       <c r="G27" s="95">
@@ -2975,10 +2986,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="151" t="s">
+      <c r="A28" s="146" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="152"/>
+      <c r="B28" s="147"/>
       <c r="C28" s="50"/>
       <c r="D28" s="49"/>
       <c r="E28" s="48"/>
@@ -2988,10 +2999,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="161" t="s">
+      <c r="A29" s="148" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="162"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="47"/>
       <c r="D29" s="46"/>
       <c r="E29" s="45"/>
@@ -3001,10 +3012,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="163" t="s">
+      <c r="A30" s="152" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="164"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="44"/>
       <c r="D30" s="43"/>
       <c r="E30" s="42"/>
@@ -3014,10 +3025,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="165" t="s">
+      <c r="A31" s="154" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="166"/>
+      <c r="B31" s="155"/>
       <c r="C31" s="41" t="s">
         <v>40</v>
       </c>
@@ -3031,10 +3042,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="167" t="s">
+      <c r="A32" s="136" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="168"/>
+      <c r="B32" s="137"/>
       <c r="C32" s="39"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -3053,21 +3064,21 @@
       <c r="G33" s="109"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="169" t="s">
+      <c r="A34" s="156" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="171"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="158"/>
       <c r="D34" s="36"/>
       <c r="E34" s="35"/>
       <c r="F34" s="34"/>
       <c r="G34" s="100"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="143" t="s">
+      <c r="A35" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="144"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="33"/>
       <c r="D35" s="87" t="s">
         <v>75</v>
@@ -3079,10 +3090,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="143" t="s">
+      <c r="A36" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="144"/>
+      <c r="B36" s="151"/>
       <c r="C36" s="33"/>
       <c r="D36" s="31"/>
       <c r="E36" s="30"/>
@@ -3092,10 +3103,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="143" t="s">
+      <c r="A37" s="150" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="144"/>
+      <c r="B37" s="151"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -3105,10 +3116,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="145" t="s">
+      <c r="A38" s="162" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="146"/>
+      <c r="B38" s="163"/>
       <c r="C38" s="32"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -3118,10 +3129,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="145" t="s">
+      <c r="A39" s="162" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="146"/>
+      <c r="B39" s="163"/>
       <c r="C39" s="32" t="s">
         <v>32</v>
       </c>
@@ -3133,10 +3144,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="147" t="s">
+      <c r="A40" s="164" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="148"/>
+      <c r="B40" s="165"/>
       <c r="C40" s="29"/>
       <c r="D40" s="28"/>
       <c r="E40" s="19"/>
@@ -3146,10 +3157,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="149" t="s">
+      <c r="A41" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="150"/>
+      <c r="B41" s="167"/>
       <c r="C41" s="27"/>
       <c r="D41" s="26"/>
       <c r="E41" s="25"/>
@@ -3179,10 +3190,10 @@
       <c r="G43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="151" t="s">
+      <c r="A44" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="152"/>
+      <c r="B44" s="147"/>
       <c r="C44" s="22">
         <v>2</v>
       </c>
@@ -3194,10 +3205,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="153" t="s">
+      <c r="A45" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="154"/>
+      <c r="B45" s="169"/>
       <c r="C45" s="20">
         <f>C44-1</f>
         <v>1</v>
@@ -3210,10 +3221,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="155" t="s">
+      <c r="A46" s="170" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="156"/>
+      <c r="B46" s="171"/>
       <c r="C46" s="18"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -3232,164 +3243,164 @@
       <c r="G47" s="112"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="140" t="s">
+      <c r="A48" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="141"/>
-      <c r="C48" s="141"/>
-      <c r="D48" s="141"/>
-      <c r="E48" s="141"/>
-      <c r="F48" s="141"/>
-      <c r="G48" s="142"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="161"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="114" t="s">
+      <c r="A49" s="172" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="117" t="s">
+      <c r="B49" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="119"/>
-      <c r="D49" s="131" t="s">
+      <c r="C49" s="176"/>
+      <c r="D49" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="133"/>
-      <c r="F49" s="132" t="s">
+      <c r="E49" s="178"/>
+      <c r="F49" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="133"/>
+      <c r="G49" s="178"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="115"/>
-      <c r="B50" s="135" t="s">
+      <c r="A50" s="173"/>
+      <c r="B50" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="137"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="137"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="137"/>
+      <c r="C50" s="181"/>
+      <c r="D50" s="180"/>
+      <c r="E50" s="181"/>
+      <c r="F50" s="182"/>
+      <c r="G50" s="181"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="116"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="130"/>
-      <c r="D51" s="129"/>
-      <c r="E51" s="130"/>
-      <c r="F51" s="138"/>
-      <c r="G51" s="139"/>
+      <c r="A51" s="174"/>
+      <c r="B51" s="183"/>
+      <c r="C51" s="184"/>
+      <c r="D51" s="183"/>
+      <c r="E51" s="184"/>
+      <c r="F51" s="185"/>
+      <c r="G51" s="186"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="125" t="s">
+      <c r="A52" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="126"/>
-      <c r="C52" s="126"/>
-      <c r="D52" s="126"/>
-      <c r="E52" s="126"/>
-      <c r="F52" s="126"/>
-      <c r="G52" s="127"/>
+      <c r="B52" s="188"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="188"/>
+      <c r="E52" s="188"/>
+      <c r="F52" s="188"/>
+      <c r="G52" s="189"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="114" t="s">
+      <c r="A53" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="131" t="s">
+      <c r="B53" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="132"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="132" t="s">
+      <c r="C53" s="179"/>
+      <c r="D53" s="178"/>
+      <c r="E53" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="132"/>
-      <c r="G53" s="133"/>
+      <c r="F53" s="179"/>
+      <c r="G53" s="178"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="115"/>
-      <c r="B54" s="135"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="137"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="137"/>
+      <c r="A54" s="173"/>
+      <c r="B54" s="180"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="181"/>
+      <c r="E54" s="182"/>
+      <c r="F54" s="182"/>
+      <c r="G54" s="181"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="116"/>
-      <c r="B55" s="129"/>
-      <c r="C55" s="134"/>
-      <c r="D55" s="130"/>
-      <c r="E55" s="138"/>
-      <c r="F55" s="138"/>
-      <c r="G55" s="139"/>
+      <c r="A55" s="174"/>
+      <c r="B55" s="183"/>
+      <c r="C55" s="190"/>
+      <c r="D55" s="184"/>
+      <c r="E55" s="185"/>
+      <c r="F55" s="185"/>
+      <c r="G55" s="186"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="125" t="s">
+      <c r="A56" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="126"/>
-      <c r="C56" s="126"/>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="126"/>
-      <c r="G56" s="127"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="188"/>
+      <c r="D56" s="188"/>
+      <c r="E56" s="188"/>
+      <c r="F56" s="188"/>
+      <c r="G56" s="189"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="114" t="s">
+      <c r="A57" s="172" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="117" t="s">
+      <c r="B57" s="175" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="119"/>
-      <c r="D57" s="117" t="s">
+      <c r="C57" s="176"/>
+      <c r="D57" s="175" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="119"/>
-      <c r="F57" s="117" t="s">
+      <c r="E57" s="176"/>
+      <c r="F57" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="119"/>
+      <c r="G57" s="176"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="115"/>
+      <c r="A58" s="173"/>
       <c r="B58" s="13"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="128"/>
-      <c r="E58" s="121"/>
+      <c r="D58" s="191"/>
+      <c r="E58" s="192"/>
       <c r="F58" s="12"/>
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="115"/>
-      <c r="B59" s="129" t="s">
+      <c r="A59" s="173"/>
+      <c r="B59" s="183" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="130"/>
-      <c r="D59" s="122" t="s">
+      <c r="C59" s="184"/>
+      <c r="D59" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="124"/>
-      <c r="F59" s="123" t="s">
+      <c r="E59" s="194"/>
+      <c r="F59" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="124"/>
+      <c r="G59" s="194"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="115"/>
-      <c r="B60" s="131" t="s">
+      <c r="A60" s="173"/>
+      <c r="B60" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="132"/>
-      <c r="D60" s="133"/>
-      <c r="E60" s="117" t="s">
+      <c r="C60" s="179"/>
+      <c r="D60" s="178"/>
+      <c r="E60" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="118"/>
-      <c r="G60" s="119"/>
+      <c r="F60" s="196"/>
+      <c r="G60" s="176"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="115"/>
+      <c r="A61" s="173"/>
       <c r="B61" s="10"/>
       <c r="C61" s="9"/>
       <c r="D61" s="6"/>
@@ -3398,121 +3409,63 @@
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="116"/>
-      <c r="B62" s="129" t="s">
+      <c r="A62" s="174"/>
+      <c r="B62" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="134"/>
-      <c r="D62" s="130"/>
-      <c r="E62" s="122" t="s">
+      <c r="C62" s="190"/>
+      <c r="D62" s="184"/>
+      <c r="E62" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="123"/>
-      <c r="G62" s="124"/>
+      <c r="F62" s="195"/>
+      <c r="G62" s="194"/>
     </row>
     <row r="63" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="114" t="s">
+      <c r="A63" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="117" t="s">
+      <c r="B63" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="118"/>
-      <c r="D63" s="119"/>
-      <c r="E63" s="117" t="s">
+      <c r="C63" s="196"/>
+      <c r="D63" s="176"/>
+      <c r="E63" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="118"/>
-      <c r="G63" s="119"/>
+      <c r="F63" s="196"/>
+      <c r="G63" s="176"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="115"/>
+      <c r="A64" s="173"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="4"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="120"/>
-      <c r="G64" s="121"/>
+      <c r="F64" s="197"/>
+      <c r="G64" s="192"/>
     </row>
     <row r="65" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="116"/>
-      <c r="B65" s="122" t="s">
+      <c r="A65" s="174"/>
+      <c r="B65" s="193" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="123"/>
-      <c r="D65" s="124"/>
-      <c r="E65" s="122" t="s">
+      <c r="C65" s="195"/>
+      <c r="D65" s="194"/>
+      <c r="E65" s="193" t="s">
         <v>0</v>
       </c>
-      <c r="F65" s="123"/>
-      <c r="G65" s="124"/>
+      <c r="F65" s="195"/>
+      <c r="G65" s="194"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
     <mergeCell ref="A56:G56"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="B57:C57"/>
@@ -3526,12 +3479,70 @@
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: add property filtering for payment items in cost.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38FA3B0-684B-43AB-9198-52AD0AC5392A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D198A14-A418-4537-8A4C-C383FB793CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="2" r:id="rId1"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -612,9 +612,6 @@
   </si>
   <si>
     <t>ملحوظة قيمة التضخم بالحد الاقصي المذكور بالعقد</t>
-  </si>
-  <si>
-    <t>ملحوظة قيمة الدفعة المقدمة بحد اقصي القيمة الاصلية من العقد</t>
   </si>
   <si>
     <t>اعمال إعادة قياس</t>
@@ -1789,11 +1786,218 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
@@ -1832,213 +2036,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2612,8 +2609,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="C1" zoomScale="59" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:G4"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="31" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2638,55 +2635,55 @@
       <c r="A1" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="133" t="s">
+      <c r="B1" s="182" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="133"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
+      <c r="C1" s="182"/>
+      <c r="D1" s="183"/>
+      <c r="E1" s="183"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="133" t="s">
+      <c r="B2" s="182" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="133"/>
-      <c r="D2" s="135" t="s">
+      <c r="C2" s="182"/>
+      <c r="D2" s="184" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="135"/>
-      <c r="F2" s="135"/>
-      <c r="G2" s="135"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="182" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="133"/>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
+      <c r="C3" s="182"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="131" t="s">
+      <c r="B4" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="131"/>
-      <c r="D4" s="132" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="181" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2711,22 +2708,22 @@
       <c r="G6" s="106"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="185" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="117"/>
+      <c r="B7" s="186"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="118" t="s">
+      <c r="D7" s="187" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="117"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="120"/>
+      <c r="E7" s="186"/>
+      <c r="F7" s="188"/>
+      <c r="G7" s="189"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="121"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="123"/>
+      <c r="A8" s="190"/>
+      <c r="B8" s="191"/>
+      <c r="C8" s="192"/>
       <c r="D8" s="76" t="s">
         <v>58</v>
       </c>
@@ -2739,21 +2736,21 @@
       <c r="G8" s="107"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="124" t="s">
+      <c r="A9" s="193" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="125"/>
-      <c r="C9" s="126"/>
+      <c r="B9" s="194"/>
+      <c r="C9" s="195"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="127" t="s">
+      <c r="A10" s="196" t="s">
         <v>69</v>
       </c>
-      <c r="B10" s="128"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="71"/>
       <c r="D10" s="113">
         <v>0</v>
@@ -2763,10 +2760,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="129" t="s">
+      <c r="A11" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="130"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2774,10 +2771,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="129" t="s">
+      <c r="A12" s="176" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="130"/>
+      <c r="B12" s="177"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30">
         <v>0</v>
@@ -2787,10 +2784,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="129" t="s">
+      <c r="A13" s="176" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="130"/>
+      <c r="B13" s="177"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2798,10 +2795,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="129" t="s">
+      <c r="A14" s="176" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="130"/>
+      <c r="B14" s="177"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2809,10 +2806,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="129" t="s">
+      <c r="A15" s="176" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="130"/>
+      <c r="B15" s="177"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2820,10 +2817,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="157" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="115"/>
+      <c r="B16" s="158"/>
       <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
@@ -2833,10 +2830,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="136" t="s">
+      <c r="A17" s="167" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="137"/>
+      <c r="B17" s="168"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16+D15+D14+D13+D12+D11+D10</f>
@@ -2862,21 +2859,21 @@
       <c r="G18" s="108"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="138" t="s">
+      <c r="A19" s="172" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="139"/>
-      <c r="C19" s="139"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="173"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="92"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="140" t="s">
+      <c r="A20" s="174" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="175"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2886,10 +2883,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="142" t="s">
+      <c r="A21" s="178" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="143"/>
+      <c r="B21" s="179"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30">
         <v>0</v>
@@ -2901,10 +2898,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="176" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="130"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30">
         <v>0</v>
@@ -2916,10 +2913,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="129" t="s">
+      <c r="A23" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="130"/>
+      <c r="B23" s="177"/>
       <c r="C23" s="53"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
@@ -2929,10 +2926,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="129" t="s">
+      <c r="A24" s="176" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="130"/>
+      <c r="B24" s="177"/>
       <c r="C24" s="53"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -2942,12 +2939,12 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="129" t="s">
+      <c r="A25" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="130"/>
+      <c r="B25" s="177"/>
       <c r="C25" s="104" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2957,10 +2954,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="114" t="s">
+      <c r="A26" s="157" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="115"/>
+      <c r="B26" s="158"/>
       <c r="C26" s="52"/>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
@@ -2970,10 +2967,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="144" t="s">
+      <c r="A27" s="159" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="145"/>
+      <c r="B27" s="160"/>
       <c r="C27" s="39"/>
       <c r="D27" s="25">
         <f>D20+D21+D22+D23-D24+D25-D26</f>
@@ -2986,10 +2983,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="146" t="s">
+      <c r="A28" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="147"/>
+      <c r="B28" s="152"/>
       <c r="C28" s="50"/>
       <c r="D28" s="49"/>
       <c r="E28" s="48"/>
@@ -2999,10 +2996,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="148" t="s">
+      <c r="A29" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="149"/>
+      <c r="B29" s="162"/>
       <c r="C29" s="47"/>
       <c r="D29" s="46"/>
       <c r="E29" s="45"/>
@@ -3012,10 +3009,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="152" t="s">
+      <c r="A30" s="163" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="153"/>
+      <c r="B30" s="164"/>
       <c r="C30" s="44"/>
       <c r="D30" s="43"/>
       <c r="E30" s="42"/>
@@ -3025,10 +3022,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="154" t="s">
+      <c r="A31" s="165" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="155"/>
+      <c r="B31" s="166"/>
       <c r="C31" s="41" t="s">
         <v>40</v>
       </c>
@@ -3042,10 +3039,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="136" t="s">
+      <c r="A32" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="137"/>
+      <c r="B32" s="168"/>
       <c r="C32" s="39"/>
       <c r="D32" s="25"/>
       <c r="E32" s="25"/>
@@ -3064,25 +3061,23 @@
       <c r="G33" s="109"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="156" t="s">
+      <c r="A34" s="169" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="157"/>
-      <c r="C34" s="158"/>
+      <c r="B34" s="170"/>
+      <c r="C34" s="171"/>
       <c r="D34" s="36"/>
       <c r="E34" s="35"/>
       <c r="F34" s="34"/>
       <c r="G34" s="100"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="150" t="s">
+      <c r="A35" s="143" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="151"/>
+      <c r="B35" s="144"/>
       <c r="C35" s="33"/>
-      <c r="D35" s="87" t="s">
-        <v>75</v>
-      </c>
+      <c r="D35" s="87"/>
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
       <c r="G35" s="101">
@@ -3090,10 +3085,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="150" t="s">
+      <c r="A36" s="143" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="151"/>
+      <c r="B36" s="144"/>
       <c r="C36" s="33"/>
       <c r="D36" s="31"/>
       <c r="E36" s="30"/>
@@ -3103,10 +3098,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="150" t="s">
+      <c r="A37" s="143" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="151"/>
+      <c r="B37" s="144"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -3116,10 +3111,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="162" t="s">
+      <c r="A38" s="145" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="163"/>
+      <c r="B38" s="146"/>
       <c r="C38" s="32"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -3129,10 +3124,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="162" t="s">
+      <c r="A39" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="163"/>
+      <c r="B39" s="146"/>
       <c r="C39" s="32" t="s">
         <v>32</v>
       </c>
@@ -3144,10 +3139,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="164" t="s">
+      <c r="A40" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="165"/>
+      <c r="B40" s="148"/>
       <c r="C40" s="29"/>
       <c r="D40" s="28"/>
       <c r="E40" s="19"/>
@@ -3157,12 +3152,15 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="166" t="s">
+      <c r="A41" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="167"/>
+      <c r="B41" s="150"/>
       <c r="C41" s="27"/>
-      <c r="D41" s="26"/>
+      <c r="D41" s="26">
+        <f>D34+D35+D36+D37+D38+D39+D40</f>
+        <v>0</v>
+      </c>
       <c r="E41" s="25"/>
       <c r="F41" s="25"/>
       <c r="G41" s="102">
@@ -3190,10 +3188,10 @@
       <c r="G43" s="111"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="146" t="s">
+      <c r="A44" s="151" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="147"/>
+      <c r="B44" s="152"/>
       <c r="C44" s="22">
         <v>2</v>
       </c>
@@ -3205,10 +3203,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="168" t="s">
+      <c r="A45" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="169"/>
+      <c r="B45" s="154"/>
       <c r="C45" s="20">
         <f>C44-1</f>
         <v>1</v>
@@ -3221,10 +3219,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="170" t="s">
+      <c r="A46" s="155" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="171"/>
+      <c r="B46" s="156"/>
       <c r="C46" s="18"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -3243,164 +3241,164 @@
       <c r="G47" s="112"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="159" t="s">
+      <c r="A48" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="160"/>
-      <c r="C48" s="160"/>
-      <c r="D48" s="160"/>
-      <c r="E48" s="160"/>
-      <c r="F48" s="160"/>
-      <c r="G48" s="161"/>
+      <c r="B48" s="141"/>
+      <c r="C48" s="141"/>
+      <c r="D48" s="141"/>
+      <c r="E48" s="141"/>
+      <c r="F48" s="141"/>
+      <c r="G48" s="142"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="172" t="s">
+      <c r="A49" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="175" t="s">
+      <c r="B49" s="117" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="176"/>
-      <c r="D49" s="177" t="s">
+      <c r="C49" s="119"/>
+      <c r="D49" s="131" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="178"/>
-      <c r="F49" s="179" t="s">
+      <c r="E49" s="133"/>
+      <c r="F49" s="132" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="178"/>
+      <c r="G49" s="133"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="173"/>
-      <c r="B50" s="180" t="s">
+      <c r="A50" s="115"/>
+      <c r="B50" s="135" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="181"/>
-      <c r="D50" s="180"/>
-      <c r="E50" s="181"/>
-      <c r="F50" s="182"/>
-      <c r="G50" s="181"/>
+      <c r="C50" s="137"/>
+      <c r="D50" s="135"/>
+      <c r="E50" s="137"/>
+      <c r="F50" s="136"/>
+      <c r="G50" s="137"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="174"/>
-      <c r="B51" s="183"/>
-      <c r="C51" s="184"/>
-      <c r="D51" s="183"/>
-      <c r="E51" s="184"/>
-      <c r="F51" s="185"/>
-      <c r="G51" s="186"/>
+      <c r="A51" s="116"/>
+      <c r="B51" s="129"/>
+      <c r="C51" s="130"/>
+      <c r="D51" s="129"/>
+      <c r="E51" s="130"/>
+      <c r="F51" s="138"/>
+      <c r="G51" s="139"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="187" t="s">
+      <c r="A52" s="125" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="188"/>
-      <c r="C52" s="188"/>
-      <c r="D52" s="188"/>
-      <c r="E52" s="188"/>
-      <c r="F52" s="188"/>
-      <c r="G52" s="189"/>
+      <c r="B52" s="126"/>
+      <c r="C52" s="126"/>
+      <c r="D52" s="126"/>
+      <c r="E52" s="126"/>
+      <c r="F52" s="126"/>
+      <c r="G52" s="127"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="172" t="s">
+      <c r="A53" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="177" t="s">
+      <c r="B53" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="179"/>
-      <c r="D53" s="178"/>
-      <c r="E53" s="179" t="s">
+      <c r="C53" s="132"/>
+      <c r="D53" s="133"/>
+      <c r="E53" s="132" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="179"/>
-      <c r="G53" s="178"/>
+      <c r="F53" s="132"/>
+      <c r="G53" s="133"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="173"/>
-      <c r="B54" s="180"/>
-      <c r="C54" s="182"/>
-      <c r="D54" s="181"/>
-      <c r="E54" s="182"/>
-      <c r="F54" s="182"/>
-      <c r="G54" s="181"/>
+      <c r="A54" s="115"/>
+      <c r="B54" s="135"/>
+      <c r="C54" s="136"/>
+      <c r="D54" s="137"/>
+      <c r="E54" s="136"/>
+      <c r="F54" s="136"/>
+      <c r="G54" s="137"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="174"/>
-      <c r="B55" s="183"/>
-      <c r="C55" s="190"/>
-      <c r="D55" s="184"/>
-      <c r="E55" s="185"/>
-      <c r="F55" s="185"/>
-      <c r="G55" s="186"/>
+      <c r="A55" s="116"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="134"/>
+      <c r="D55" s="130"/>
+      <c r="E55" s="138"/>
+      <c r="F55" s="138"/>
+      <c r="G55" s="139"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="187" t="s">
+      <c r="A56" s="125" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="188"/>
-      <c r="C56" s="188"/>
-      <c r="D56" s="188"/>
-      <c r="E56" s="188"/>
-      <c r="F56" s="188"/>
-      <c r="G56" s="189"/>
+      <c r="B56" s="126"/>
+      <c r="C56" s="126"/>
+      <c r="D56" s="126"/>
+      <c r="E56" s="126"/>
+      <c r="F56" s="126"/>
+      <c r="G56" s="127"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="172" t="s">
+      <c r="A57" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="175" t="s">
+      <c r="B57" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="176"/>
-      <c r="D57" s="175" t="s">
+      <c r="C57" s="119"/>
+      <c r="D57" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="176"/>
-      <c r="F57" s="175" t="s">
+      <c r="E57" s="119"/>
+      <c r="F57" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="176"/>
+      <c r="G57" s="119"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="173"/>
+      <c r="A58" s="115"/>
       <c r="B58" s="13"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="191"/>
-      <c r="E58" s="192"/>
+      <c r="D58" s="128"/>
+      <c r="E58" s="121"/>
       <c r="F58" s="12"/>
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="173"/>
-      <c r="B59" s="183" t="s">
+      <c r="A59" s="115"/>
+      <c r="B59" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="184"/>
-      <c r="D59" s="193" t="s">
+      <c r="C59" s="130"/>
+      <c r="D59" s="122" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="194"/>
-      <c r="F59" s="195" t="s">
+      <c r="E59" s="124"/>
+      <c r="F59" s="123" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="194"/>
+      <c r="G59" s="124"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="173"/>
-      <c r="B60" s="177" t="s">
+      <c r="A60" s="115"/>
+      <c r="B60" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="179"/>
-      <c r="D60" s="178"/>
-      <c r="E60" s="175" t="s">
+      <c r="C60" s="132"/>
+      <c r="D60" s="133"/>
+      <c r="E60" s="117" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="196"/>
-      <c r="G60" s="176"/>
+      <c r="F60" s="118"/>
+      <c r="G60" s="119"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="173"/>
+      <c r="A61" s="115"/>
       <c r="B61" s="10"/>
       <c r="C61" s="9"/>
       <c r="D61" s="6"/>
@@ -3409,63 +3407,121 @@
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="174"/>
-      <c r="B62" s="183" t="s">
+      <c r="A62" s="116"/>
+      <c r="B62" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="190"/>
-      <c r="D62" s="184"/>
-      <c r="E62" s="193" t="s">
+      <c r="C62" s="134"/>
+      <c r="D62" s="130"/>
+      <c r="E62" s="122" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="195"/>
-      <c r="G62" s="194"/>
+      <c r="F62" s="123"/>
+      <c r="G62" s="124"/>
     </row>
     <row r="63" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="172" t="s">
+      <c r="A63" s="114" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="175" t="s">
+      <c r="B63" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="196"/>
-      <c r="D63" s="176"/>
-      <c r="E63" s="175" t="s">
+      <c r="C63" s="118"/>
+      <c r="D63" s="119"/>
+      <c r="E63" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="196"/>
-      <c r="G63" s="176"/>
+      <c r="F63" s="118"/>
+      <c r="G63" s="119"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="173"/>
+      <c r="A64" s="115"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="4"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="197"/>
-      <c r="G64" s="192"/>
+      <c r="F64" s="120"/>
+      <c r="G64" s="121"/>
     </row>
     <row r="65" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="174"/>
-      <c r="B65" s="193" t="s">
+      <c r="A65" s="116"/>
+      <c r="B65" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="195"/>
-      <c r="D65" s="194"/>
-      <c r="E65" s="193" t="s">
+      <c r="C65" s="123"/>
+      <c r="D65" s="124"/>
+      <c r="E65" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="F65" s="195"/>
-      <c r="G65" s="194"/>
+      <c r="F65" s="123"/>
+      <c r="G65" s="124"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
     <mergeCell ref="A56:G56"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="B57:C57"/>
@@ -3479,70 +3535,12 @@
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: optimize property filtering logic in cost.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D198A14-A418-4537-8A4C-C383FB793CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EE5B94-5469-45FA-8867-01CD4AA96687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -2610,7 +2610,7 @@
   <dimension ref="A1:G65"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="31" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
feat: add inflation rate and remeasured calculations in cost.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EE5B94-5469-45FA-8867-01CD4AA96687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B903265D-8C41-4EA8-A6D9-022EDBBB126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <definedName name="PPP" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PRAYER" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PrevDate">[1]Summary!$L$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$67</definedName>
     <definedName name="qeewq" hidden="1">{"offequipsch",#N/A,FALSE,"GTC_Schedule";"onconstsch",#N/A,FALSE,"GTC_Schedule";"techsch",#N/A,FALSE,"GTC_Schedule";"totsch",#N/A,FALSE,"GTC_Schedule"}</definedName>
     <definedName name="qp" hidden="1">#REF!</definedName>
     <definedName name="qqq" hidden="1">#REF!</definedName>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -574,19 +574,12 @@
     <t>عن الأعمال حتى:</t>
   </si>
   <si>
-    <t>مستخلص جاري رقم 2 من بداية العمل حتى شهر نوفمبر 2024</t>
-  </si>
-  <si>
     <t xml:space="preserve">المقــــاول </t>
   </si>
   <si>
     <t xml:space="preserve">الاستـــشارى  </t>
   </si>
   <si>
-    <t xml:space="preserve">مشــروع : عقد تنفيذ وتشطيب عدد 40 عمارة مجموعة 88 
-وعدد 44 عمارة مجموعة 89 منطقة B8 </t>
-  </si>
-  <si>
     <t xml:space="preserve">رب العمــــــل     </t>
   </si>
   <si>
@@ -615,6 +608,19 @@
   </si>
   <si>
     <t>اعمال إعادة قياس</t>
+  </si>
+  <si>
+    <t>إجمالي قيمة الزيادة لأعمال معادة القياس (إضافة )</t>
+  </si>
+  <si>
+    <t>إجمالى قيمة الزيادة لأعمال معادة القياس (حذف )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">مستخلص جاري رقم (2) </t>
+  </si>
+  <si>
+    <t>عقد تنفيذ فيلات منطقة V35 -مدينتى
+عن أعمال حتى 31 يناير 2025</t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1453,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1704,9 +1710,6 @@
     </xf>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="4" fontId="15" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -2061,20 +2064,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2784693</xdr:colOff>
+      <xdr:colOff>2496950</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>89579</xdr:rowOff>
+      <xdr:rowOff>279831</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="994169" cy="720586"/>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>781728</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>266983</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 5" descr="Logo_Arabian_Co">
+        <xdr:cNvPr id="18" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F155AFF-AD52-4BB7-BD43-9DB1978903BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2680F00-AA91-4D17-B8DF-AF48EE746B1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2091,113 +2099,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="9983031238" y="89579"/>
-          <a:ext cx="994169" cy="720586"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2039471</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>85645</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="733487" cy="651042"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="ALEXLOGO_SMALL">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E5F380-BD1E-41F7-AF27-B49B74D017A4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9983294192" y="85645"/>
-          <a:ext cx="733487" cy="651042"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 8594"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF">
-            <a:shade val="85000"/>
-          </a:srgbClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:reflection blurRad="12700" stA="38000" endPos="28000" dist="5000" dir="5400000" sy="-100000" algn="bl" rotWithShape="0"/>
-        </a:effectLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>2267530</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>40820</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1058156</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>243226</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B5390B-F1C0-4443-9208-7DD9B0CAAEAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9985856719" y="517070"/>
-          <a:ext cx="609901" cy="431006"/>
+          <a:off x="10586497933" y="279831"/>
+          <a:ext cx="1545880" cy="536050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2222,54 +2125,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>187300</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>64374</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="954201" cy="575728"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="\\CVL_HABASHY\4 share\ISLAM\2021\3-1-2021\IMG-20210103-WA0000.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C638EDC-BEE5-4E6B-BC4D-1E57AB18F711}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9984716099" y="540624"/>
-          <a:ext cx="954201" cy="575728"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2607,10 +2462,10 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="31" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2633,57 +2488,57 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="85" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="182" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="182"/>
-      <c r="D1" s="183"/>
-      <c r="E1" s="183"/>
+        <v>66</v>
+      </c>
+      <c r="B1" s="181" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="182" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="182"/>
-      <c r="D2" s="184" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="184"/>
-      <c r="F2" s="184"/>
-      <c r="G2" s="184"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="183" t="s">
+        <v>77</v>
+      </c>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="182" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="182"/>
-      <c r="D3" s="184"/>
-      <c r="E3" s="184"/>
-      <c r="F3" s="184"/>
-      <c r="G3" s="184"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4" s="180" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="181" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2692,7 +2547,7 @@
       <c r="D5" s="83"/>
       <c r="E5" s="83"/>
       <c r="F5" s="82"/>
-      <c r="G5" s="105"/>
+      <c r="G5" s="104"/>
     </row>
     <row r="6" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="81"/>
@@ -2702,28 +2557,26 @@
       <c r="E6" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="78">
-        <v>45610</v>
-      </c>
-      <c r="G6" s="106"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="185" t="s">
+      <c r="A7" s="184" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="186"/>
+      <c r="B7" s="185"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="187" t="s">
+      <c r="D7" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="186"/>
-      <c r="F7" s="188"/>
-      <c r="G7" s="189"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="187"/>
+      <c r="G7" s="188"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="190"/>
-      <c r="B8" s="191"/>
-      <c r="C8" s="192"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="190"/>
+      <c r="C8" s="191"/>
       <c r="D8" s="76" t="s">
         <v>58</v>
       </c>
@@ -2733,37 +2586,35 @@
       <c r="F8" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="107"/>
+      <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="195"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="196" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10" s="197"/>
+      <c r="A10" s="195" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="196"/>
       <c r="C10" s="71"/>
-      <c r="D10" s="113">
-        <v>0</v>
-      </c>
+      <c r="D10" s="112"/>
       <c r="E10" s="30"/>
       <c r="F10" s="70"/>
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="176" t="s">
+      <c r="A11" s="175" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="177"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2771,23 +2622,21 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="176" t="s">
+      <c r="A12" s="175" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="177"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="69"/>
-      <c r="D12" s="30">
-        <v>0</v>
-      </c>
+      <c r="D12" s="30"/>
       <c r="E12" s="30"/>
       <c r="F12" s="30"/>
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="176" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="177"/>
+      <c r="A13" s="175" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="176"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2795,10 +2644,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="176" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="177"/>
+      <c r="A14" s="175" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="176"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2806,10 +2655,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="176" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="177"/>
+      <c r="A15" s="175" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" s="176"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2817,10 +2666,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="157" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="158"/>
+      <c r="A16" s="156" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="157"/>
       <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
@@ -2830,10 +2679,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="167" t="s">
+      <c r="A17" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="168"/>
+      <c r="B17" s="167"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16+D15+D14+D13+D12+D11+D10</f>
@@ -2856,608 +2705,629 @@
       <c r="D18" s="59"/>
       <c r="E18" s="59"/>
       <c r="F18" s="59"/>
-      <c r="G18" s="108"/>
+      <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="172" t="s">
+      <c r="A19" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="173"/>
-      <c r="C19" s="173"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="172"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
-      <c r="G19" s="92"/>
+      <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="174" t="s">
+      <c r="A20" s="173" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="175"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
-      <c r="G20" s="93">
+      <c r="G20" s="92">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="178" t="s">
+      <c r="A21" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="179"/>
+      <c r="B21" s="178"/>
       <c r="C21" s="55"/>
-      <c r="D21" s="30">
-        <v>0</v>
-      </c>
+      <c r="D21" s="30"/>
       <c r="E21" s="54"/>
       <c r="F21" s="54"/>
-      <c r="G21" s="94">
+      <c r="G21" s="93">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="176" t="s">
+      <c r="A22" s="175" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="177"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="86"/>
-      <c r="D22" s="30">
-        <v>0</v>
-      </c>
+      <c r="D22" s="30"/>
       <c r="E22" s="54"/>
       <c r="F22" s="54"/>
-      <c r="G22" s="93">
+      <c r="G22" s="92">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="176" t="s">
+      <c r="A23" s="175" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="176"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="92"/>
+    </row>
+    <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="175" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" s="176"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="92"/>
+    </row>
+    <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="175" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="176" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="177"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="93">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="176" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="177"/>
-      <c r="C25" s="104" t="s">
-        <v>75</v>
-      </c>
+      <c r="B25" s="176"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
-      <c r="G25" s="94">
+      <c r="G25" s="93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="175" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="176"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="175" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="176"/>
+      <c r="C27" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="93">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="157" t="s">
+    <row r="28" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="158"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="94">
+      <c r="B28" s="157"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="93">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="159" t="s">
+    <row r="29" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="160"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="25">
-        <f>D20+D21+D22+D23-D24+D25-D26</f>
+      <c r="B29" s="159"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="25">
+        <f>D20+D21+D22+D25-D26+D27-D28</f>
         <v>0</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="95">
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="94">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="151" t="s">
+    <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="150" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="152"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="96">
+      <c r="B30" s="151"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="95">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="161" t="s">
+    <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="162"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="97">
+      <c r="B31" s="161"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="96">
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="163" t="s">
+    <row r="32" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="164"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="98">
+      <c r="B32" s="163"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="97">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="165" t="s">
+    <row r="33" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="166"/>
-      <c r="C31" s="41" t="s">
+      <c r="B33" s="165"/>
+      <c r="C33" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D31" s="88" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="89"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="99">
+      <c r="D33" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="88"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="98">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="167" t="s">
+    <row r="34" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A34" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="168"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="95">
+      <c r="B34" s="167"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="94">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="38"/>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="109"/>
-    </row>
-    <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="169" t="s">
+    <row r="35" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="38"/>
+      <c r="B35" s="37"/>
+      <c r="C35" s="37"/>
+      <c r="D35" s="37"/>
+      <c r="E35" s="37"/>
+      <c r="F35" s="37"/>
+      <c r="G35" s="108"/>
+    </row>
+    <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="170"/>
-      <c r="C34" s="171"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="100"/>
-    </row>
-    <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="143" t="s">
+      <c r="B36" s="169"/>
+      <c r="C36" s="170"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="99"/>
+    </row>
+    <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="144"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="101">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="143" t="s">
-        <v>36</v>
-      </c>
-      <c r="B36" s="144"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="101">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="143" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="144"/>
+      <c r="B37" s="143"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
-      <c r="G37" s="101">
-        <v>16</v>
+      <c r="G37" s="100">
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="145" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="146"/>
-      <c r="C38" s="32"/>
+      <c r="A38" s="142" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="143"/>
+      <c r="C38" s="33"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="101">
-        <v>17</v>
+      <c r="G38" s="100">
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="145" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="146"/>
-      <c r="C39" s="32" t="s">
-        <v>32</v>
-      </c>
+      <c r="A39" s="142" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="143"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
-      <c r="G39" s="101">
+      <c r="G39" s="100">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A40" s="144" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" s="145"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="100">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="144" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="145"/>
+      <c r="C41" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="100">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="147" t="s">
+    <row r="42" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="148"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="101">
+      <c r="B42" s="147"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="100">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="149" t="s">
+    <row r="43" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="150"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="26">
-        <f>D34+D35+D36+D37+D38+D39+D40</f>
+      <c r="B43" s="149"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="26">
+        <f>D36+D37+D38+D39+D40+D41+D42</f>
         <v>0</v>
       </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="102">
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="101">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="24"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="23"/>
-      <c r="G42" s="110"/>
-    </row>
-    <row r="43" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="90" t="s">
+    <row r="44" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="24"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="109"/>
+    </row>
+    <row r="45" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="91"/>
-      <c r="D43" s="91"/>
-      <c r="E43" s="91"/>
-      <c r="F43" s="91"/>
-      <c r="G43" s="111"/>
-    </row>
-    <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="151" t="s">
+      <c r="B45" s="90"/>
+      <c r="C45" s="90"/>
+      <c r="D45" s="90"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="90"/>
+      <c r="G45" s="110"/>
+    </row>
+    <row r="46" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="152"/>
-      <c r="C44" s="22">
+      <c r="B46" s="151"/>
+      <c r="C46" s="22">
         <v>2</v>
       </c>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="96">
+      <c r="D46" s="21">
+        <f>D34-D43</f>
+        <v>0</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="95">
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="153" t="s">
+    <row r="47" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="154"/>
-      <c r="C45" s="20">
-        <f>C44-1</f>
+      <c r="B47" s="153"/>
+      <c r="C47" s="20">
+        <f>C46-1</f>
         <v>1</v>
       </c>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="103">
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="102">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="155" t="s">
+    <row r="48" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="156"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="95">
+      <c r="B48" s="155"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17"/>
+      <c r="F48" s="17"/>
+      <c r="G48" s="94">
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="16"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="112"/>
-    </row>
-    <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="140" t="s">
+    <row r="49" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A49" s="16"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="111"/>
+    </row>
+    <row r="50" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A50" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="141"/>
-      <c r="C48" s="141"/>
-      <c r="D48" s="141"/>
-      <c r="E48" s="141"/>
-      <c r="F48" s="141"/>
-      <c r="G48" s="142"/>
-    </row>
-    <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="114" t="s">
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="141"/>
+    </row>
+    <row r="51" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A51" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="117" t="s">
+      <c r="B51" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="119"/>
-      <c r="D49" s="131" t="s">
+      <c r="C51" s="118"/>
+      <c r="D51" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="133"/>
-      <c r="F49" s="132" t="s">
+      <c r="E51" s="132"/>
+      <c r="F51" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="133"/>
-    </row>
-    <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="115"/>
-      <c r="B50" s="135" t="s">
+      <c r="G51" s="132"/>
+    </row>
+    <row r="52" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A52" s="114"/>
+      <c r="B52" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="137"/>
-      <c r="D50" s="135"/>
-      <c r="E50" s="137"/>
-      <c r="F50" s="136"/>
-      <c r="G50" s="137"/>
-    </row>
-    <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="116"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="130"/>
-      <c r="D51" s="129"/>
-      <c r="E51" s="130"/>
-      <c r="F51" s="138"/>
-      <c r="G51" s="139"/>
-    </row>
-    <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="125" t="s">
+      <c r="C52" s="136"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="136"/>
+    </row>
+    <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A53" s="115"/>
+      <c r="B53" s="128"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="129"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="138"/>
+    </row>
+    <row r="54" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A54" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="126"/>
-      <c r="C52" s="126"/>
-      <c r="D52" s="126"/>
-      <c r="E52" s="126"/>
-      <c r="F52" s="126"/>
-      <c r="G52" s="127"/>
-    </row>
-    <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="114" t="s">
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="125"/>
+      <c r="F54" s="125"/>
+      <c r="G54" s="126"/>
+    </row>
+    <row r="55" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="131" t="s">
+      <c r="B55" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="132"/>
-      <c r="D53" s="133"/>
-      <c r="E53" s="132" t="s">
+      <c r="C55" s="131"/>
+      <c r="D55" s="132"/>
+      <c r="E55" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="132"/>
-      <c r="G53" s="133"/>
-    </row>
-    <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="115"/>
-      <c r="B54" s="135"/>
-      <c r="C54" s="136"/>
-      <c r="D54" s="137"/>
-      <c r="E54" s="136"/>
-      <c r="F54" s="136"/>
-      <c r="G54" s="137"/>
-    </row>
-    <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="116"/>
-      <c r="B55" s="129"/>
-      <c r="C55" s="134"/>
-      <c r="D55" s="130"/>
-      <c r="E55" s="138"/>
-      <c r="F55" s="138"/>
-      <c r="G55" s="139"/>
-    </row>
-    <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="125" t="s">
+      <c r="F55" s="131"/>
+      <c r="G55" s="132"/>
+    </row>
+    <row r="56" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A56" s="114"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="135"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="135"/>
+      <c r="F56" s="135"/>
+      <c r="G56" s="136"/>
+    </row>
+    <row r="57" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A57" s="115"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="129"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="137"/>
+      <c r="G57" s="138"/>
+    </row>
+    <row r="58" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A58" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="126"/>
-      <c r="C56" s="126"/>
-      <c r="D56" s="126"/>
-      <c r="E56" s="126"/>
-      <c r="F56" s="126"/>
-      <c r="G56" s="127"/>
-    </row>
-    <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="114" t="s">
+      <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
+      <c r="D58" s="125"/>
+      <c r="E58" s="125"/>
+      <c r="F58" s="125"/>
+      <c r="G58" s="126"/>
+    </row>
+    <row r="59" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="117" t="s">
+      <c r="B59" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="119"/>
-      <c r="D57" s="117" t="s">
+      <c r="C59" s="118"/>
+      <c r="D59" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="119"/>
-      <c r="F57" s="117" t="s">
+      <c r="E59" s="118"/>
+      <c r="F59" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="119"/>
-    </row>
-    <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="115"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="128"/>
-      <c r="E58" s="121"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="11"/>
-    </row>
-    <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="115"/>
-      <c r="B59" s="129" t="s">
+      <c r="G59" s="118"/>
+    </row>
+    <row r="60" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="114"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="127"/>
+      <c r="E60" s="120"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="114"/>
+      <c r="B61" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="130"/>
-      <c r="D59" s="122" t="s">
+      <c r="C61" s="129"/>
+      <c r="D61" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="124"/>
-      <c r="F59" s="123" t="s">
+      <c r="E61" s="123"/>
+      <c r="F61" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="124"/>
-    </row>
-    <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="115"/>
-      <c r="B60" s="131" t="s">
+      <c r="G61" s="123"/>
+    </row>
+    <row r="62" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A62" s="114"/>
+      <c r="B62" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="132"/>
-      <c r="D60" s="133"/>
-      <c r="E60" s="117" t="s">
+      <c r="C62" s="131"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="118"/>
-      <c r="G60" s="119"/>
-    </row>
-    <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="115"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="6"/>
-    </row>
-    <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="116"/>
-      <c r="B62" s="129" t="s">
+      <c r="F62" s="117"/>
+      <c r="G62" s="118"/>
+    </row>
+    <row r="63" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="114"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="115"/>
+      <c r="B64" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="134"/>
-      <c r="D62" s="130"/>
-      <c r="E62" s="122" t="s">
+      <c r="C64" s="133"/>
+      <c r="D64" s="129"/>
+      <c r="E64" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="123"/>
-      <c r="G62" s="124"/>
-    </row>
-    <row r="63" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="114" t="s">
+      <c r="F64" s="122"/>
+      <c r="G64" s="123"/>
+    </row>
+    <row r="65" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A65" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="117" t="s">
+      <c r="B65" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="118"/>
-      <c r="D63" s="119"/>
-      <c r="E63" s="117" t="s">
+      <c r="C65" s="117"/>
+      <c r="D65" s="118"/>
+      <c r="E65" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="118"/>
-      <c r="G63" s="119"/>
-    </row>
-    <row r="64" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="115"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="120"/>
-      <c r="G64" s="121"/>
-    </row>
-    <row r="65" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="116"/>
-      <c r="B65" s="122" t="s">
+      <c r="F65" s="117"/>
+      <c r="G65" s="118"/>
+    </row>
+    <row r="66" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="114"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="119"/>
+      <c r="G66" s="120"/>
+    </row>
+    <row r="67" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A67" s="115"/>
+      <c r="B67" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="123"/>
-      <c r="D65" s="124"/>
-      <c r="E65" s="122" t="s">
+      <c r="C67" s="122"/>
+      <c r="D67" s="123"/>
+      <c r="E67" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="F65" s="123"/>
-      <c r="G65" s="124"/>
+      <c r="F67" s="122"/>
+      <c r="G67" s="123"/>
     </row>
   </sheetData>
-  <mergeCells count="83">
+  <mergeCells count="85">
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D7:E7"/>
@@ -3480,67 +3350,69 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
     <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A50:G50"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:A53"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="D51:E51"/>
     <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A55:A57"/>
     <mergeCell ref="B55:D55"/>
     <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A58:G58"/>
+    <mergeCell ref="A59:A64"/>
     <mergeCell ref="B59:C59"/>
     <mergeCell ref="D59:E59"/>
     <mergeCell ref="F59:G59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="A65:A67"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: correct date format in cost.py for current and last date
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B903265D-8C41-4EA8-A6D9-022EDBBB126E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AAC9C3-13AC-427A-80E2-848D36BF9ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -602,12 +602,6 @@
   </si>
   <si>
     <t xml:space="preserve">صافي الأوامر التغييرية إعادة قياس  </t>
-  </si>
-  <si>
-    <t>ملحوظة قيمة التضخم بالحد الاقصي المذكور بالعقد</t>
-  </si>
-  <si>
-    <t>اعمال إعادة قياس</t>
   </si>
   <si>
     <t>إجمالي قيمة الزيادة لأعمال معادة القياس (إضافة )</t>
@@ -1789,92 +1783,113 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1882,60 +1897,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1946,12 +1907,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1963,82 +1918,121 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2464,8 +2458,8 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2490,55 +2484,55 @@
       <c r="A1" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="181"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="183" t="s">
-        <v>77</v>
-      </c>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="134" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2561,22 +2555,22 @@
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="115" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="185"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="186" t="s">
+      <c r="D7" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="185"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="188"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="119"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="189"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="191"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="76" t="s">
         <v>58</v>
       </c>
@@ -2589,21 +2583,21 @@
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="192" t="s">
+      <c r="A9" s="123" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="195" t="s">
+      <c r="A10" s="126" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="196"/>
+      <c r="B10" s="127"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2611,10 +2605,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="175" t="s">
+      <c r="A11" s="128" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="176"/>
+      <c r="B11" s="129"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2622,10 +2616,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="176"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2633,10 +2627,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="175" t="s">
+      <c r="A13" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="176"/>
+      <c r="B13" s="129"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2644,10 +2638,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="175" t="s">
+      <c r="A14" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="176"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2655,10 +2649,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="175" t="s">
+      <c r="A15" s="128" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="176"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2666,10 +2660,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="113" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="157"/>
+      <c r="B16" s="114"/>
       <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
@@ -2679,13 +2673,13 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="166" t="s">
+      <c r="A17" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="167"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
-        <f>D16+D15+D14+D13+D12+D11+D10</f>
+        <f>D16-D15-D14+D13+D12+D11+D10</f>
         <v>0</v>
       </c>
       <c r="E17" s="62">
@@ -2708,21 +2702,21 @@
       <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="171" t="s">
+      <c r="A19" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="173" t="s">
+      <c r="A20" s="139" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="174"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2732,10 +2726,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="177" t="s">
+      <c r="A21" s="141" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="178"/>
+      <c r="B21" s="142"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30"/>
       <c r="E21" s="54"/>
@@ -2745,10 +2739,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="128" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="176"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2758,10 +2752,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="175" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" s="176"/>
+      <c r="A23" s="128" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="129"/>
       <c r="C23" s="86"/>
       <c r="D23" s="30"/>
       <c r="E23" s="54"/>
@@ -2769,10 +2763,10 @@
       <c r="G23" s="92"/>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="175" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="176"/>
+      <c r="A24" s="128" t="s">
+        <v>73</v>
+      </c>
+      <c r="B24" s="129"/>
       <c r="C24" s="86"/>
       <c r="D24" s="30"/>
       <c r="E24" s="54"/>
@@ -2780,10 +2774,10 @@
       <c r="G24" s="92"/>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="175" t="s">
+      <c r="A25" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="176"/>
+      <c r="B25" s="129"/>
       <c r="C25" s="53"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2793,10 +2787,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="175" t="s">
+      <c r="A26" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="176"/>
+      <c r="B26" s="129"/>
       <c r="C26" s="53"/>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -2806,13 +2800,11 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="175" t="s">
+      <c r="A27" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="176"/>
-      <c r="C27" s="103" t="s">
-        <v>73</v>
-      </c>
+      <c r="B27" s="129"/>
+      <c r="C27" s="103"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
@@ -2821,10 +2813,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="156" t="s">
+      <c r="A28" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="157"/>
+      <c r="B28" s="114"/>
       <c r="C28" s="52"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
@@ -2834,10 +2826,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="158" t="s">
+      <c r="A29" s="143" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="159"/>
+      <c r="B29" s="144"/>
       <c r="C29" s="39"/>
       <c r="D29" s="25">
         <f>D20+D21+D22+D25-D26+D27-D28</f>
@@ -2850,10 +2842,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="150" t="s">
+      <c r="A30" s="145" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="151"/>
+      <c r="B30" s="146"/>
       <c r="C30" s="50"/>
       <c r="D30" s="49"/>
       <c r="E30" s="48"/>
@@ -2863,10 +2855,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="160" t="s">
+      <c r="A31" s="147" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="161"/>
+      <c r="B31" s="148"/>
       <c r="C31" s="47"/>
       <c r="D31" s="46"/>
       <c r="E31" s="45"/>
@@ -2876,10 +2868,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="162" t="s">
+      <c r="A32" s="151" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="163"/>
+      <c r="B32" s="152"/>
       <c r="C32" s="44"/>
       <c r="D32" s="43"/>
       <c r="E32" s="42"/>
@@ -2889,16 +2881,14 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="164" t="s">
+      <c r="A33" s="153" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="165"/>
+      <c r="B33" s="154"/>
       <c r="C33" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="87" t="s">
-        <v>72</v>
-      </c>
+      <c r="D33" s="87"/>
       <c r="E33" s="88"/>
       <c r="F33" s="40"/>
       <c r="G33" s="98">
@@ -2906,12 +2896,15 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="166" t="s">
+      <c r="A34" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="167"/>
+      <c r="B34" s="136"/>
       <c r="C34" s="39"/>
-      <c r="D34" s="25"/>
+      <c r="D34" s="25">
+        <f>D29+D30+D31+D32+D33</f>
+        <v>0</v>
+      </c>
       <c r="E34" s="25"/>
       <c r="F34" s="25"/>
       <c r="G34" s="94">
@@ -2928,21 +2921,21 @@
       <c r="G35" s="108"/>
     </row>
     <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="168" t="s">
+      <c r="A36" s="155" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="169"/>
-      <c r="C36" s="170"/>
+      <c r="B36" s="156"/>
+      <c r="C36" s="157"/>
       <c r="D36" s="36"/>
       <c r="E36" s="35"/>
       <c r="F36" s="34"/>
       <c r="G36" s="99"/>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="142" t="s">
+      <c r="A37" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="143"/>
+      <c r="B37" s="150"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -2952,10 +2945,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="142" t="s">
+      <c r="A38" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="143"/>
+      <c r="B38" s="150"/>
       <c r="C38" s="33"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -2965,10 +2958,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="142" t="s">
+      <c r="A39" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="143"/>
+      <c r="B39" s="150"/>
       <c r="C39" s="33"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
@@ -2978,10 +2971,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="144" t="s">
+      <c r="A40" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="145"/>
+      <c r="B40" s="162"/>
       <c r="C40" s="32"/>
       <c r="D40" s="31"/>
       <c r="E40" s="30"/>
@@ -2991,10 +2984,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="145"/>
+      <c r="B41" s="162"/>
       <c r="C41" s="32" t="s">
         <v>32</v>
       </c>
@@ -3006,10 +2999,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="146" t="s">
+      <c r="A42" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="147"/>
+      <c r="B42" s="164"/>
       <c r="C42" s="29"/>
       <c r="D42" s="28"/>
       <c r="E42" s="19"/>
@@ -3019,10 +3012,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="149"/>
+      <c r="B43" s="166"/>
       <c r="C43" s="27"/>
       <c r="D43" s="26">
         <f>D36+D37+D38+D39+D40+D41+D42</f>
@@ -3055,10 +3048,10 @@
       <c r="G45" s="110"/>
     </row>
     <row r="46" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="150" t="s">
+      <c r="A46" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="151"/>
+      <c r="B46" s="146"/>
       <c r="C46" s="22">
         <v>2</v>
       </c>
@@ -3073,10 +3066,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="152" t="s">
+      <c r="A47" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="153"/>
+      <c r="B47" s="168"/>
       <c r="C47" s="20">
         <f>C46-1</f>
         <v>1</v>
@@ -3089,10 +3082,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="154" t="s">
+      <c r="A48" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="155"/>
+      <c r="B48" s="170"/>
       <c r="C48" s="18"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -3111,164 +3104,164 @@
       <c r="G49" s="111"/>
     </row>
     <row r="50" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="139" t="s">
+      <c r="A50" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="140"/>
-      <c r="F50" s="140"/>
-      <c r="G50" s="141"/>
+      <c r="B50" s="159"/>
+      <c r="C50" s="159"/>
+      <c r="D50" s="159"/>
+      <c r="E50" s="159"/>
+      <c r="F50" s="159"/>
+      <c r="G50" s="160"/>
     </row>
     <row r="51" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="113" t="s">
+      <c r="A51" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="116" t="s">
+      <c r="B51" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="118"/>
-      <c r="D51" s="130" t="s">
+      <c r="C51" s="175"/>
+      <c r="D51" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="132"/>
-      <c r="F51" s="131" t="s">
+      <c r="E51" s="177"/>
+      <c r="F51" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="132"/>
+      <c r="G51" s="177"/>
     </row>
     <row r="52" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="114"/>
-      <c r="B52" s="134" t="s">
+      <c r="A52" s="172"/>
+      <c r="B52" s="179" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="134"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="136"/>
+      <c r="C52" s="180"/>
+      <c r="D52" s="179"/>
+      <c r="E52" s="180"/>
+      <c r="F52" s="181"/>
+      <c r="G52" s="180"/>
     </row>
     <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="115"/>
-      <c r="B53" s="128"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="129"/>
-      <c r="F53" s="137"/>
-      <c r="G53" s="138"/>
+      <c r="A53" s="173"/>
+      <c r="B53" s="182"/>
+      <c r="C53" s="183"/>
+      <c r="D53" s="182"/>
+      <c r="E53" s="183"/>
+      <c r="F53" s="184"/>
+      <c r="G53" s="185"/>
     </row>
     <row r="54" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="124" t="s">
+      <c r="A54" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="125"/>
-      <c r="C54" s="125"/>
-      <c r="D54" s="125"/>
-      <c r="E54" s="125"/>
-      <c r="F54" s="125"/>
-      <c r="G54" s="126"/>
+      <c r="B54" s="187"/>
+      <c r="C54" s="187"/>
+      <c r="D54" s="187"/>
+      <c r="E54" s="187"/>
+      <c r="F54" s="187"/>
+      <c r="G54" s="188"/>
     </row>
     <row r="55" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="113" t="s">
+      <c r="A55" s="171" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="130" t="s">
+      <c r="B55" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="131"/>
-      <c r="D55" s="132"/>
-      <c r="E55" s="131" t="s">
+      <c r="C55" s="178"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="F55" s="131"/>
-      <c r="G55" s="132"/>
+      <c r="F55" s="178"/>
+      <c r="G55" s="177"/>
     </row>
     <row r="56" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="114"/>
-      <c r="B56" s="134"/>
-      <c r="C56" s="135"/>
-      <c r="D56" s="136"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="136"/>
+      <c r="A56" s="172"/>
+      <c r="B56" s="179"/>
+      <c r="C56" s="181"/>
+      <c r="D56" s="180"/>
+      <c r="E56" s="181"/>
+      <c r="F56" s="181"/>
+      <c r="G56" s="180"/>
     </row>
     <row r="57" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="115"/>
-      <c r="B57" s="128"/>
-      <c r="C57" s="133"/>
-      <c r="D57" s="129"/>
-      <c r="E57" s="137"/>
-      <c r="F57" s="137"/>
-      <c r="G57" s="138"/>
+      <c r="A57" s="173"/>
+      <c r="B57" s="182"/>
+      <c r="C57" s="189"/>
+      <c r="D57" s="183"/>
+      <c r="E57" s="184"/>
+      <c r="F57" s="184"/>
+      <c r="G57" s="185"/>
     </row>
     <row r="58" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="124" t="s">
+      <c r="A58" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="125"/>
-      <c r="C58" s="125"/>
-      <c r="D58" s="125"/>
-      <c r="E58" s="125"/>
-      <c r="F58" s="125"/>
-      <c r="G58" s="126"/>
+      <c r="B58" s="187"/>
+      <c r="C58" s="187"/>
+      <c r="D58" s="187"/>
+      <c r="E58" s="187"/>
+      <c r="F58" s="187"/>
+      <c r="G58" s="188"/>
     </row>
     <row r="59" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="113" t="s">
+      <c r="A59" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="116" t="s">
+      <c r="B59" s="174" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="118"/>
-      <c r="D59" s="116" t="s">
+      <c r="C59" s="175"/>
+      <c r="D59" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="118"/>
-      <c r="F59" s="116" t="s">
+      <c r="E59" s="175"/>
+      <c r="F59" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="118"/>
+      <c r="G59" s="175"/>
     </row>
     <row r="60" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="114"/>
+      <c r="A60" s="172"/>
       <c r="B60" s="13"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="127"/>
-      <c r="E60" s="120"/>
+      <c r="D60" s="190"/>
+      <c r="E60" s="191"/>
       <c r="F60" s="12"/>
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="114"/>
-      <c r="B61" s="128" t="s">
+      <c r="A61" s="172"/>
+      <c r="B61" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="129"/>
-      <c r="D61" s="121" t="s">
+      <c r="C61" s="183"/>
+      <c r="D61" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="123"/>
-      <c r="F61" s="122" t="s">
+      <c r="E61" s="193"/>
+      <c r="F61" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="123"/>
+      <c r="G61" s="193"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="114"/>
-      <c r="B62" s="130" t="s">
+      <c r="A62" s="172"/>
+      <c r="B62" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="131"/>
-      <c r="D62" s="132"/>
-      <c r="E62" s="116" t="s">
+      <c r="C62" s="178"/>
+      <c r="D62" s="177"/>
+      <c r="E62" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="117"/>
-      <c r="G62" s="118"/>
+      <c r="F62" s="195"/>
+      <c r="G62" s="175"/>
     </row>
     <row r="63" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="114"/>
+      <c r="A63" s="172"/>
       <c r="B63" s="10"/>
       <c r="C63" s="9"/>
       <c r="D63" s="6"/>
@@ -3277,123 +3270,63 @@
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="115"/>
-      <c r="B64" s="128" t="s">
+      <c r="A64" s="173"/>
+      <c r="B64" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="133"/>
-      <c r="D64" s="129"/>
-      <c r="E64" s="121" t="s">
+      <c r="C64" s="189"/>
+      <c r="D64" s="183"/>
+      <c r="E64" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="122"/>
-      <c r="G64" s="123"/>
+      <c r="F64" s="194"/>
+      <c r="G64" s="193"/>
     </row>
     <row r="65" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="113" t="s">
+      <c r="A65" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="116" t="s">
+      <c r="B65" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="117"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="116" t="s">
+      <c r="C65" s="195"/>
+      <c r="D65" s="175"/>
+      <c r="E65" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="117"/>
-      <c r="G65" s="118"/>
+      <c r="F65" s="195"/>
+      <c r="G65" s="175"/>
     </row>
     <row r="66" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="114"/>
+      <c r="A66" s="172"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="4"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="119"/>
-      <c r="G66" s="120"/>
+      <c r="F66" s="196"/>
+      <c r="G66" s="191"/>
     </row>
     <row r="67" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="115"/>
-      <c r="B67" s="121" t="s">
+      <c r="A67" s="173"/>
+      <c r="B67" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="122"/>
-      <c r="D67" s="123"/>
-      <c r="E67" s="121" t="s">
+      <c r="C67" s="194"/>
+      <c r="D67" s="193"/>
+      <c r="E67" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="F67" s="122"/>
-      <c r="G67" s="123"/>
+      <c r="F67" s="194"/>
+      <c r="G67" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A59:A64"/>
     <mergeCell ref="B59:C59"/>
@@ -3407,12 +3340,72 @@
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="E64:G64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to improve inflation rate and remeasured calculations; add PDF extension in ExcelModifier.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AAC9C3-13AC-427A-80E2-848D36BF9ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2FF4D-B614-4F14-A48D-F5052FC8FB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="2" r:id="rId1"/>
@@ -1783,11 +1783,218 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
@@ -1826,213 +2033,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2458,8 +2458,8 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A11" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2484,55 +2484,55 @@
       <c r="A1" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="181" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="134" t="s">
+      <c r="C2" s="181"/>
+      <c r="D2" s="183" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>74</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2555,22 +2555,22 @@
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="184" t="s">
         <v>60</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="185"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="186" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="116"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="119"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="187"/>
+      <c r="G7" s="188"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="120"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="190"/>
+      <c r="C8" s="191"/>
       <c r="D8" s="76" t="s">
         <v>58</v>
       </c>
@@ -2583,21 +2583,21 @@
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="192" t="s">
         <v>55</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="125"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="195" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="127"/>
+      <c r="B10" s="196"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2605,10 +2605,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="175" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="129"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2616,10 +2616,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="175" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="129"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2627,10 +2627,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="175" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="129"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2638,10 +2638,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="128" t="s">
+      <c r="A14" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="129"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2649,10 +2649,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="175" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="129"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2660,10 +2660,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="157"/>
       <c r="C16" s="65" t="s">
         <v>40</v>
       </c>
@@ -2673,10 +2673,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="135" t="s">
+      <c r="A17" s="166" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="136"/>
+      <c r="B17" s="167"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16-D15-D14+D13+D12+D11+D10</f>
@@ -2702,21 +2702,21 @@
       <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="137" t="s">
+      <c r="A19" s="171" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="172"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="139" t="s">
+      <c r="A20" s="173" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="140"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2726,10 +2726,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="141" t="s">
+      <c r="A21" s="177" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="142"/>
+      <c r="B21" s="178"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30"/>
       <c r="E21" s="54"/>
@@ -2739,10 +2739,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="128" t="s">
+      <c r="A22" s="175" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="129"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2752,10 +2752,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="128" t="s">
+      <c r="A23" s="175" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="129"/>
+      <c r="B23" s="176"/>
       <c r="C23" s="86"/>
       <c r="D23" s="30"/>
       <c r="E23" s="54"/>
@@ -2763,10 +2763,10 @@
       <c r="G23" s="92"/>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="175" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="129"/>
+      <c r="B24" s="176"/>
       <c r="C24" s="86"/>
       <c r="D24" s="30"/>
       <c r="E24" s="54"/>
@@ -2774,10 +2774,10 @@
       <c r="G24" s="92"/>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="128" t="s">
+      <c r="A25" s="175" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="129"/>
+      <c r="B25" s="176"/>
       <c r="C25" s="53"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2787,10 +2787,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="128" t="s">
+      <c r="A26" s="175" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="129"/>
+      <c r="B26" s="176"/>
       <c r="C26" s="53"/>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -2800,10 +2800,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="128" t="s">
+      <c r="A27" s="175" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="129"/>
+      <c r="B27" s="176"/>
       <c r="C27" s="103"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
@@ -2813,10 +2813,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="113" t="s">
+      <c r="A28" s="156" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="114"/>
+      <c r="B28" s="157"/>
       <c r="C28" s="52"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
@@ -2826,26 +2826,32 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="143" t="s">
+      <c r="A29" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="B29" s="144"/>
+      <c r="B29" s="159"/>
       <c r="C29" s="39"/>
       <c r="D29" s="25">
         <f>D20+D21+D22+D25-D26+D27-D28</f>
         <v>0</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
+      <c r="E29" s="25">
+        <f t="shared" ref="E29:F29" si="1">E20+E21+E22+E25-E26+E27-E28</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="G29" s="94">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="145" t="s">
+      <c r="A30" s="150" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="146"/>
+      <c r="B30" s="151"/>
       <c r="C30" s="50"/>
       <c r="D30" s="49"/>
       <c r="E30" s="48"/>
@@ -2855,10 +2861,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="147" t="s">
+      <c r="A31" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="148"/>
+      <c r="B31" s="161"/>
       <c r="C31" s="47"/>
       <c r="D31" s="46"/>
       <c r="E31" s="45"/>
@@ -2868,10 +2874,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="151" t="s">
+      <c r="A32" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="152"/>
+      <c r="B32" s="163"/>
       <c r="C32" s="44"/>
       <c r="D32" s="43"/>
       <c r="E32" s="42"/>
@@ -2881,10 +2887,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="153" t="s">
+      <c r="A33" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="154"/>
+      <c r="B33" s="165"/>
       <c r="C33" s="41" t="s">
         <v>40</v>
       </c>
@@ -2896,17 +2902,23 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="135" t="s">
+      <c r="A34" s="166" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="136"/>
+      <c r="B34" s="167"/>
       <c r="C34" s="39"/>
       <c r="D34" s="25">
         <f>D29+D30+D31+D32+D33</f>
         <v>0</v>
       </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="E34" s="25">
+        <f t="shared" ref="E34:F34" si="2">E29+E30+E31+E32+E33</f>
+        <v>0</v>
+      </c>
+      <c r="F34" s="25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="G34" s="94">
         <v>13</v>
       </c>
@@ -2921,21 +2933,21 @@
       <c r="G35" s="108"/>
     </row>
     <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="155" t="s">
+      <c r="A36" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="B36" s="156"/>
-      <c r="C36" s="157"/>
+      <c r="B36" s="169"/>
+      <c r="C36" s="170"/>
       <c r="D36" s="36"/>
       <c r="E36" s="35"/>
       <c r="F36" s="34"/>
       <c r="G36" s="99"/>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="149" t="s">
+      <c r="A37" s="142" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="150"/>
+      <c r="B37" s="143"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -2945,10 +2957,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="149" t="s">
+      <c r="A38" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="150"/>
+      <c r="B38" s="143"/>
       <c r="C38" s="33"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -2958,10 +2970,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="149" t="s">
+      <c r="A39" s="142" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="150"/>
+      <c r="B39" s="143"/>
       <c r="C39" s="33"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
@@ -2971,10 +2983,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="161" t="s">
+      <c r="A40" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="162"/>
+      <c r="B40" s="145"/>
       <c r="C40" s="32"/>
       <c r="D40" s="31"/>
       <c r="E40" s="30"/>
@@ -2984,10 +2996,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="161" t="s">
+      <c r="A41" s="144" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="162"/>
+      <c r="B41" s="145"/>
       <c r="C41" s="32" t="s">
         <v>32</v>
       </c>
@@ -2999,10 +3011,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="163" t="s">
+      <c r="A42" s="146" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="164"/>
+      <c r="B42" s="147"/>
       <c r="C42" s="29"/>
       <c r="D42" s="28"/>
       <c r="E42" s="19"/>
@@ -3012,17 +3024,23 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="165" t="s">
+      <c r="A43" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="166"/>
+      <c r="B43" s="149"/>
       <c r="C43" s="27"/>
       <c r="D43" s="26">
         <f>D36+D37+D38+D39+D40+D41+D42</f>
         <v>0</v>
       </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
+      <c r="E43" s="26">
+        <f t="shared" ref="E43:F43" si="3">E36+E37+E38+E39+E40+E41+E42</f>
+        <v>0</v>
+      </c>
+      <c r="F43" s="26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="G43" s="101">
         <v>20</v>
       </c>
@@ -3048,10 +3066,10 @@
       <c r="G45" s="110"/>
     </row>
     <row r="46" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="145" t="s">
+      <c r="A46" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="146"/>
+      <c r="B46" s="151"/>
       <c r="C46" s="22">
         <v>2</v>
       </c>
@@ -3059,17 +3077,23 @@
         <f>D34-D43</f>
         <v>0</v>
       </c>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
+      <c r="E46" s="21">
+        <f t="shared" ref="E46:F46" si="4">E34-E43</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G46" s="95">
         <v>21</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="167" t="s">
+      <c r="A47" s="152" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="168"/>
+      <c r="B47" s="153"/>
       <c r="C47" s="20">
         <f>C46-1</f>
         <v>1</v>
@@ -3082,10 +3106,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="169" t="s">
+      <c r="A48" s="154" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="170"/>
+      <c r="B48" s="155"/>
       <c r="C48" s="18"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -3104,164 +3128,164 @@
       <c r="G49" s="111"/>
     </row>
     <row r="50" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="158" t="s">
+      <c r="A50" s="139" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="159"/>
-      <c r="C50" s="159"/>
-      <c r="D50" s="159"/>
-      <c r="E50" s="159"/>
-      <c r="F50" s="159"/>
-      <c r="G50" s="160"/>
+      <c r="B50" s="140"/>
+      <c r="C50" s="140"/>
+      <c r="D50" s="140"/>
+      <c r="E50" s="140"/>
+      <c r="F50" s="140"/>
+      <c r="G50" s="141"/>
     </row>
     <row r="51" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="171" t="s">
+      <c r="A51" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="174" t="s">
+      <c r="B51" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="175"/>
-      <c r="D51" s="176" t="s">
+      <c r="C51" s="118"/>
+      <c r="D51" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="177"/>
-      <c r="F51" s="178" t="s">
+      <c r="E51" s="132"/>
+      <c r="F51" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="177"/>
+      <c r="G51" s="132"/>
     </row>
     <row r="52" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="172"/>
-      <c r="B52" s="179" t="s">
+      <c r="A52" s="114"/>
+      <c r="B52" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="180"/>
-      <c r="D52" s="179"/>
-      <c r="E52" s="180"/>
-      <c r="F52" s="181"/>
-      <c r="G52" s="180"/>
+      <c r="C52" s="136"/>
+      <c r="D52" s="134"/>
+      <c r="E52" s="136"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="136"/>
     </row>
     <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="173"/>
-      <c r="B53" s="182"/>
-      <c r="C53" s="183"/>
-      <c r="D53" s="182"/>
-      <c r="E53" s="183"/>
-      <c r="F53" s="184"/>
-      <c r="G53" s="185"/>
+      <c r="A53" s="115"/>
+      <c r="B53" s="128"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="129"/>
+      <c r="F53" s="137"/>
+      <c r="G53" s="138"/>
     </row>
     <row r="54" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="186" t="s">
+      <c r="A54" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="187"/>
-      <c r="C54" s="187"/>
-      <c r="D54" s="187"/>
-      <c r="E54" s="187"/>
-      <c r="F54" s="187"/>
-      <c r="G54" s="188"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="125"/>
+      <c r="D54" s="125"/>
+      <c r="E54" s="125"/>
+      <c r="F54" s="125"/>
+      <c r="G54" s="126"/>
     </row>
     <row r="55" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="171" t="s">
+      <c r="A55" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="176" t="s">
+      <c r="B55" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="178"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="178" t="s">
+      <c r="C55" s="131"/>
+      <c r="D55" s="132"/>
+      <c r="E55" s="131" t="s">
         <v>16</v>
       </c>
-      <c r="F55" s="178"/>
-      <c r="G55" s="177"/>
+      <c r="F55" s="131"/>
+      <c r="G55" s="132"/>
     </row>
     <row r="56" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="172"/>
-      <c r="B56" s="179"/>
-      <c r="C56" s="181"/>
-      <c r="D56" s="180"/>
-      <c r="E56" s="181"/>
-      <c r="F56" s="181"/>
-      <c r="G56" s="180"/>
+      <c r="A56" s="114"/>
+      <c r="B56" s="134"/>
+      <c r="C56" s="135"/>
+      <c r="D56" s="136"/>
+      <c r="E56" s="135"/>
+      <c r="F56" s="135"/>
+      <c r="G56" s="136"/>
     </row>
     <row r="57" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="173"/>
-      <c r="B57" s="182"/>
-      <c r="C57" s="189"/>
-      <c r="D57" s="183"/>
-      <c r="E57" s="184"/>
-      <c r="F57" s="184"/>
-      <c r="G57" s="185"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="128"/>
+      <c r="C57" s="133"/>
+      <c r="D57" s="129"/>
+      <c r="E57" s="137"/>
+      <c r="F57" s="137"/>
+      <c r="G57" s="138"/>
     </row>
     <row r="58" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="186" t="s">
+      <c r="A58" s="124" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="187"/>
-      <c r="C58" s="187"/>
-      <c r="D58" s="187"/>
-      <c r="E58" s="187"/>
-      <c r="F58" s="187"/>
-      <c r="G58" s="188"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="125"/>
+      <c r="D58" s="125"/>
+      <c r="E58" s="125"/>
+      <c r="F58" s="125"/>
+      <c r="G58" s="126"/>
     </row>
     <row r="59" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="171" t="s">
+      <c r="A59" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="174" t="s">
+      <c r="B59" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="175"/>
-      <c r="D59" s="174" t="s">
+      <c r="C59" s="118"/>
+      <c r="D59" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="175"/>
-      <c r="F59" s="174" t="s">
+      <c r="E59" s="118"/>
+      <c r="F59" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="175"/>
+      <c r="G59" s="118"/>
     </row>
     <row r="60" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="172"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="13"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="190"/>
-      <c r="E60" s="191"/>
+      <c r="D60" s="127"/>
+      <c r="E60" s="120"/>
       <c r="F60" s="12"/>
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="172"/>
-      <c r="B61" s="182" t="s">
+      <c r="A61" s="114"/>
+      <c r="B61" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="183"/>
-      <c r="D61" s="192" t="s">
+      <c r="C61" s="129"/>
+      <c r="D61" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="193"/>
-      <c r="F61" s="194" t="s">
+      <c r="E61" s="123"/>
+      <c r="F61" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="193"/>
+      <c r="G61" s="123"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="172"/>
-      <c r="B62" s="176" t="s">
+      <c r="A62" s="114"/>
+      <c r="B62" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="178"/>
-      <c r="D62" s="177"/>
-      <c r="E62" s="174" t="s">
+      <c r="C62" s="131"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="195"/>
-      <c r="G62" s="175"/>
+      <c r="F62" s="117"/>
+      <c r="G62" s="118"/>
     </row>
     <row r="63" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="172"/>
+      <c r="A63" s="114"/>
       <c r="B63" s="10"/>
       <c r="C63" s="9"/>
       <c r="D63" s="6"/>
@@ -3270,63 +3294,123 @@
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="173"/>
-      <c r="B64" s="182" t="s">
+      <c r="A64" s="115"/>
+      <c r="B64" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="189"/>
-      <c r="D64" s="183"/>
-      <c r="E64" s="192" t="s">
+      <c r="C64" s="133"/>
+      <c r="D64" s="129"/>
+      <c r="E64" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="194"/>
-      <c r="G64" s="193"/>
+      <c r="F64" s="122"/>
+      <c r="G64" s="123"/>
     </row>
     <row r="65" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="171" t="s">
+      <c r="A65" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="174" t="s">
+      <c r="B65" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="195"/>
-      <c r="D65" s="175"/>
-      <c r="E65" s="174" t="s">
+      <c r="C65" s="117"/>
+      <c r="D65" s="118"/>
+      <c r="E65" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="195"/>
-      <c r="G65" s="175"/>
+      <c r="F65" s="117"/>
+      <c r="G65" s="118"/>
     </row>
     <row r="66" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="172"/>
+      <c r="A66" s="114"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="4"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="196"/>
-      <c r="G66" s="191"/>
+      <c r="F66" s="119"/>
+      <c r="G66" s="120"/>
     </row>
     <row r="67" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="173"/>
-      <c r="B67" s="192" t="s">
+      <c r="A67" s="115"/>
+      <c r="B67" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="194"/>
-      <c r="D67" s="193"/>
-      <c r="E67" s="192" t="s">
+      <c r="C67" s="122"/>
+      <c r="D67" s="123"/>
+      <c r="E67" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="F67" s="194"/>
-      <c r="G67" s="193"/>
+      <c r="F67" s="122"/>
+      <c r="G67" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A59:A64"/>
     <mergeCell ref="B59:C59"/>
@@ -3340,72 +3424,12 @@
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="E64:G64"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to handle single recipient case in reviewer name display
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE2FF4D-B614-4F14-A48D-F5052FC8FB2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B29F2D-6A8A-483D-86E3-0985AAEF2684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="75">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -484,9 +484,6 @@
     <t xml:space="preserve">  تعليات الاستلام مرفق بيان </t>
   </si>
   <si>
-    <t>(مرفق بيان)</t>
-  </si>
-  <si>
     <t>تعليات متنوعة</t>
   </si>
   <si>
@@ -602,12 +599,6 @@
   </si>
   <si>
     <t xml:space="preserve">صافي الأوامر التغييرية إعادة قياس  </t>
-  </si>
-  <si>
-    <t>إجمالي قيمة الزيادة لأعمال معادة القياس (إضافة )</t>
-  </si>
-  <si>
-    <t>إجمالى قيمة الزيادة لأعمال معادة القياس (حذف )</t>
   </si>
   <si>
     <t xml:space="preserve">مستخلص جاري رقم (2) </t>
@@ -615,6 +606,12 @@
   <si>
     <t>عقد تنفيذ فيلات منطقة V35 -مدينتى
 عن أعمال حتى 31 يناير 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">إجمالي قيمة الزيادة لأعمال معادة القياس (إضافة )       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">إجمالى قيمة الزيادة لأعمال معادة القياس (حذف )         </t>
   </si>
 </sst>
 </file>
@@ -1447,7 +1444,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1783,92 +1780,113 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1876,60 +1894,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1940,12 +1904,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1957,83 +1915,128 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2458,8 +2461,8 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A9" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScale="43" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2482,57 +2485,57 @@
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="85" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="181" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="181"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="B1" s="132" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="132"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="181" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="183" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="134" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="181" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
-        <v>62</v>
-      </c>
-      <c r="B4" s="179" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
+      <c r="C4" s="130"/>
+      <c r="D4" s="131" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2549,55 +2552,55 @@
       <c r="C6" s="80"/>
       <c r="D6" s="80"/>
       <c r="E6" s="79" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="78"/>
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="184" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="185"/>
+      <c r="A7" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="116"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="186" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="185"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="188"/>
+      <c r="D7" s="117" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="116"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="119"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="189"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="191"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="76" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="192" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
+      <c r="A9" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="124"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="195" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="196"/>
+      <c r="A10" s="126" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="127"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2605,10 +2608,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="175" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="176"/>
+      <c r="A11" s="128" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="129"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2616,10 +2619,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="175" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="176"/>
+      <c r="A12" s="128" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="129"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2627,10 +2630,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="175" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13" s="176"/>
+      <c r="A13" s="128" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="129"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2638,10 +2641,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="175" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="176"/>
+      <c r="A14" s="128" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" s="129"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2649,10 +2652,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="175" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="176"/>
+      <c r="A15" s="128" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="129"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2660,12 +2663,12 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="156" t="s">
-        <v>68</v>
-      </c>
-      <c r="B16" s="157"/>
+      <c r="A16" s="113" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="114"/>
       <c r="C16" s="65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -2673,10 +2676,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="166" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="167"/>
+      <c r="A17" s="135" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="136"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16-D15-D14+D13+D12+D11+D10</f>
@@ -2702,21 +2705,21 @@
       <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="171" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
+      <c r="A19" s="137" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="173" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="174"/>
+      <c r="A20" s="139" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="140"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2726,10 +2729,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="177" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="178"/>
+      <c r="A21" s="141" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="142"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30"/>
       <c r="E21" s="54"/>
@@ -2739,10 +2742,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="175" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="176"/>
+      <c r="A22" s="128" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="129"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2752,10 +2755,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="175" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="176"/>
+      <c r="A23" s="197" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="198"/>
       <c r="C23" s="86"/>
       <c r="D23" s="30"/>
       <c r="E23" s="54"/>
@@ -2763,10 +2766,10 @@
       <c r="G23" s="92"/>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="175" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="176"/>
+      <c r="A24" s="197" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="198"/>
       <c r="C24" s="86"/>
       <c r="D24" s="30"/>
       <c r="E24" s="54"/>
@@ -2774,10 +2777,10 @@
       <c r="G24" s="92"/>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="175" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="176"/>
+      <c r="A25" s="128" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="129"/>
       <c r="C25" s="53"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2787,10 +2790,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="175" t="s">
-        <v>47</v>
-      </c>
-      <c r="B26" s="176"/>
+      <c r="A26" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="129"/>
       <c r="C26" s="53"/>
       <c r="D26" s="30"/>
       <c r="E26" s="30"/>
@@ -2800,10 +2803,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="175" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="176"/>
+      <c r="A27" s="128" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="129"/>
       <c r="C27" s="103"/>
       <c r="D27" s="30"/>
       <c r="E27" s="30"/>
@@ -2813,10 +2816,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="156" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="157"/>
+      <c r="A28" s="113" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="114"/>
       <c r="C28" s="52"/>
       <c r="D28" s="51"/>
       <c r="E28" s="51"/>
@@ -2826,10 +2829,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="158" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" s="159"/>
+      <c r="A29" s="143" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="144"/>
       <c r="C29" s="39"/>
       <c r="D29" s="25">
         <f>D20+D21+D22+D25-D26+D27-D28</f>
@@ -2848,10 +2851,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="150" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="151"/>
+      <c r="A30" s="145" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="146"/>
       <c r="C30" s="50"/>
       <c r="D30" s="49"/>
       <c r="E30" s="48"/>
@@ -2861,10 +2864,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="160" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="161"/>
+      <c r="A31" s="147" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="148"/>
       <c r="C31" s="47"/>
       <c r="D31" s="46"/>
       <c r="E31" s="45"/>
@@ -2874,10 +2877,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="162" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="163"/>
+      <c r="A32" s="151" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="152"/>
       <c r="C32" s="44"/>
       <c r="D32" s="43"/>
       <c r="E32" s="42"/>
@@ -2887,12 +2890,12 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="164" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="165"/>
+      <c r="A33" s="153" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="154"/>
       <c r="C33" s="41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D33" s="87"/>
       <c r="E33" s="88"/>
@@ -2902,10 +2905,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="166" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="167"/>
+      <c r="A34" s="135" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="136"/>
       <c r="C34" s="39"/>
       <c r="D34" s="25">
         <f>D29+D30+D31+D32+D33</f>
@@ -2933,21 +2936,21 @@
       <c r="G35" s="108"/>
     </row>
     <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="168" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="169"/>
-      <c r="C36" s="170"/>
+      <c r="A36" s="155" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="156"/>
+      <c r="C36" s="157"/>
       <c r="D36" s="36"/>
       <c r="E36" s="35"/>
       <c r="F36" s="34"/>
       <c r="G36" s="99"/>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="142" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="143"/>
+      <c r="A37" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="150"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -2957,10 +2960,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="142" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="143"/>
+      <c r="A38" s="149" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="150"/>
       <c r="C38" s="33"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -2970,10 +2973,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="142" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="143"/>
+      <c r="A39" s="149" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="150"/>
       <c r="C39" s="33"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
@@ -2983,10 +2986,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="144" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="145"/>
+      <c r="A40" s="161" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="162"/>
       <c r="C40" s="32"/>
       <c r="D40" s="31"/>
       <c r="E40" s="30"/>
@@ -2996,13 +2999,11 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="144" t="s">
-        <v>33</v>
-      </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="32" t="s">
+      <c r="A41" s="161" t="s">
         <v>32</v>
       </c>
+      <c r="B41" s="162"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="31"/>
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
@@ -3011,10 +3012,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="146" t="s">
+      <c r="A42" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="147"/>
+      <c r="B42" s="164"/>
       <c r="C42" s="29"/>
       <c r="D42" s="28"/>
       <c r="E42" s="19"/>
@@ -3024,10 +3025,10 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="148" t="s">
+      <c r="A43" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="149"/>
+      <c r="B43" s="166"/>
       <c r="C43" s="27"/>
       <c r="D43" s="26">
         <f>D36+D37+D38+D39+D40+D41+D42</f>
@@ -3066,10 +3067,10 @@
       <c r="G45" s="110"/>
     </row>
     <row r="46" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="150" t="s">
+      <c r="A46" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="B46" s="151"/>
+      <c r="B46" s="146"/>
       <c r="C46" s="22">
         <v>2</v>
       </c>
@@ -3090,10 +3091,10 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="152" t="s">
+      <c r="A47" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="B47" s="153"/>
+      <c r="B47" s="168"/>
       <c r="C47" s="20">
         <f>C46-1</f>
         <v>1</v>
@@ -3106,10 +3107,10 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="154" t="s">
+      <c r="A48" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="B48" s="155"/>
+      <c r="B48" s="170"/>
       <c r="C48" s="18"/>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -3128,164 +3129,164 @@
       <c r="G49" s="111"/>
     </row>
     <row r="50" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="139" t="s">
+      <c r="A50" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="140"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="140"/>
-      <c r="E50" s="140"/>
-      <c r="F50" s="140"/>
-      <c r="G50" s="141"/>
+      <c r="B50" s="159"/>
+      <c r="C50" s="159"/>
+      <c r="D50" s="159"/>
+      <c r="E50" s="159"/>
+      <c r="F50" s="159"/>
+      <c r="G50" s="160"/>
     </row>
     <row r="51" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="113" t="s">
+      <c r="A51" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="116" t="s">
+      <c r="B51" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="118"/>
-      <c r="D51" s="130" t="s">
+      <c r="C51" s="175"/>
+      <c r="D51" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="132"/>
-      <c r="F51" s="131" t="s">
+      <c r="E51" s="177"/>
+      <c r="F51" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="G51" s="132"/>
+      <c r="G51" s="177"/>
     </row>
     <row r="52" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="114"/>
-      <c r="B52" s="134" t="s">
+      <c r="A52" s="172"/>
+      <c r="B52" s="179" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="136"/>
-      <c r="D52" s="134"/>
-      <c r="E52" s="136"/>
-      <c r="F52" s="135"/>
-      <c r="G52" s="136"/>
+      <c r="C52" s="180"/>
+      <c r="D52" s="179"/>
+      <c r="E52" s="180"/>
+      <c r="F52" s="181"/>
+      <c r="G52" s="180"/>
     </row>
     <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="115"/>
-      <c r="B53" s="128"/>
-      <c r="C53" s="129"/>
-      <c r="D53" s="128"/>
-      <c r="E53" s="129"/>
-      <c r="F53" s="137"/>
-      <c r="G53" s="138"/>
+      <c r="A53" s="173"/>
+      <c r="B53" s="182"/>
+      <c r="C53" s="183"/>
+      <c r="D53" s="182"/>
+      <c r="E53" s="183"/>
+      <c r="F53" s="184"/>
+      <c r="G53" s="185"/>
     </row>
     <row r="54" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="124" t="s">
+      <c r="A54" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="B54" s="125"/>
-      <c r="C54" s="125"/>
-      <c r="D54" s="125"/>
-      <c r="E54" s="125"/>
-      <c r="F54" s="125"/>
-      <c r="G54" s="126"/>
+      <c r="B54" s="187"/>
+      <c r="C54" s="187"/>
+      <c r="D54" s="187"/>
+      <c r="E54" s="187"/>
+      <c r="F54" s="187"/>
+      <c r="G54" s="188"/>
     </row>
     <row r="55" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="113" t="s">
+      <c r="A55" s="171" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="130" t="s">
+      <c r="B55" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="C55" s="131"/>
-      <c r="D55" s="132"/>
-      <c r="E55" s="131" t="s">
+      <c r="C55" s="178"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="F55" s="131"/>
-      <c r="G55" s="132"/>
+      <c r="F55" s="178"/>
+      <c r="G55" s="177"/>
     </row>
     <row r="56" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="114"/>
-      <c r="B56" s="134"/>
-      <c r="C56" s="135"/>
-      <c r="D56" s="136"/>
-      <c r="E56" s="135"/>
-      <c r="F56" s="135"/>
-      <c r="G56" s="136"/>
+      <c r="A56" s="172"/>
+      <c r="B56" s="179"/>
+      <c r="C56" s="181"/>
+      <c r="D56" s="180"/>
+      <c r="E56" s="181"/>
+      <c r="F56" s="181"/>
+      <c r="G56" s="180"/>
     </row>
     <row r="57" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="115"/>
-      <c r="B57" s="128"/>
-      <c r="C57" s="133"/>
-      <c r="D57" s="129"/>
-      <c r="E57" s="137"/>
-      <c r="F57" s="137"/>
-      <c r="G57" s="138"/>
+      <c r="A57" s="173"/>
+      <c r="B57" s="182"/>
+      <c r="C57" s="189"/>
+      <c r="D57" s="183"/>
+      <c r="E57" s="184"/>
+      <c r="F57" s="184"/>
+      <c r="G57" s="185"/>
     </row>
     <row r="58" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="124" t="s">
+      <c r="A58" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="B58" s="125"/>
-      <c r="C58" s="125"/>
-      <c r="D58" s="125"/>
-      <c r="E58" s="125"/>
-      <c r="F58" s="125"/>
-      <c r="G58" s="126"/>
+      <c r="B58" s="187"/>
+      <c r="C58" s="187"/>
+      <c r="D58" s="187"/>
+      <c r="E58" s="187"/>
+      <c r="F58" s="187"/>
+      <c r="G58" s="188"/>
     </row>
     <row r="59" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="113" t="s">
+      <c r="A59" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="116" t="s">
+      <c r="B59" s="174" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="118"/>
-      <c r="D59" s="116" t="s">
+      <c r="C59" s="175"/>
+      <c r="D59" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="118"/>
-      <c r="F59" s="116" t="s">
+      <c r="E59" s="175"/>
+      <c r="F59" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="118"/>
+      <c r="G59" s="175"/>
     </row>
     <row r="60" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="114"/>
+      <c r="A60" s="172"/>
       <c r="B60" s="13"/>
       <c r="C60" s="6"/>
-      <c r="D60" s="127"/>
-      <c r="E60" s="120"/>
+      <c r="D60" s="190"/>
+      <c r="E60" s="191"/>
       <c r="F60" s="12"/>
       <c r="G60" s="11"/>
     </row>
     <row r="61" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="114"/>
-      <c r="B61" s="128" t="s">
+      <c r="A61" s="172"/>
+      <c r="B61" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="C61" s="129"/>
-      <c r="D61" s="121" t="s">
+      <c r="C61" s="183"/>
+      <c r="D61" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="E61" s="123"/>
-      <c r="F61" s="122" t="s">
+      <c r="E61" s="193"/>
+      <c r="F61" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="G61" s="123"/>
+      <c r="G61" s="193"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="114"/>
-      <c r="B62" s="130" t="s">
+      <c r="A62" s="172"/>
+      <c r="B62" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="131"/>
-      <c r="D62" s="132"/>
-      <c r="E62" s="116" t="s">
+      <c r="C62" s="178"/>
+      <c r="D62" s="177"/>
+      <c r="E62" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="117"/>
-      <c r="G62" s="118"/>
+      <c r="F62" s="195"/>
+      <c r="G62" s="175"/>
     </row>
     <row r="63" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="114"/>
+      <c r="A63" s="172"/>
       <c r="B63" s="10"/>
       <c r="C63" s="9"/>
       <c r="D63" s="6"/>
@@ -3294,123 +3295,63 @@
       <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="115"/>
-      <c r="B64" s="128" t="s">
+      <c r="A64" s="173"/>
+      <c r="B64" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C64" s="133"/>
-      <c r="D64" s="129"/>
-      <c r="E64" s="121" t="s">
+      <c r="C64" s="189"/>
+      <c r="D64" s="183"/>
+      <c r="E64" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="122"/>
-      <c r="G64" s="123"/>
+      <c r="F64" s="194"/>
+      <c r="G64" s="193"/>
     </row>
     <row r="65" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="113" t="s">
+      <c r="A65" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="116" t="s">
+      <c r="B65" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="C65" s="117"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="116" t="s">
+      <c r="C65" s="195"/>
+      <c r="D65" s="175"/>
+      <c r="E65" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="117"/>
-      <c r="G65" s="118"/>
+      <c r="F65" s="195"/>
+      <c r="G65" s="175"/>
     </row>
     <row r="66" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="114"/>
+      <c r="A66" s="172"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
       <c r="D66" s="4"/>
       <c r="E66" s="3"/>
-      <c r="F66" s="119"/>
-      <c r="G66" s="120"/>
+      <c r="F66" s="196"/>
+      <c r="G66" s="191"/>
     </row>
     <row r="67" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="115"/>
-      <c r="B67" s="121" t="s">
+      <c r="A67" s="173"/>
+      <c r="B67" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="C67" s="122"/>
-      <c r="D67" s="123"/>
-      <c r="E67" s="121" t="s">
+      <c r="C67" s="194"/>
+      <c r="D67" s="193"/>
+      <c r="E67" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="F67" s="122"/>
-      <c r="G67" s="123"/>
+      <c r="F67" s="194"/>
+      <c r="G67" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="E67:G67"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="A59:A64"/>
     <mergeCell ref="B59:C59"/>
@@ -3424,12 +3365,72 @@
     <mergeCell ref="E62:G62"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="E64:G64"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="A54:G54"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="E57:G57"/>
+    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="A50:G50"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to add property_006 handling and adjust cell modifications
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34318266-3F6F-46A9-857E-26D1A6C5399B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E3857-703C-4901-B6C7-15D1A6747316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <definedName name="PPP" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PRAYER" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PrevDate">[1]Summary!$L$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$67</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$65</definedName>
     <definedName name="qeewq" hidden="1">{"offequipsch",#N/A,FALSE,"GTC_Schedule";"onconstsch",#N/A,FALSE,"GTC_Schedule";"techsch",#N/A,FALSE,"GTC_Schedule";"totsch",#N/A,FALSE,"GTC_Schedule"}</definedName>
     <definedName name="qp" hidden="1">#REF!</definedName>
     <definedName name="qqq" hidden="1">#REF!</definedName>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -607,18 +607,6 @@
     <t>عقد تنفيذ فيلات منطقة V35 -مدينتى
 عن أعمال حتى 31 يناير 2025</t>
   </si>
-  <si>
-    <t>(إضافة )</t>
-  </si>
-  <si>
-    <t>(حذف )</t>
-  </si>
-  <si>
-    <t>إجمالي قيمة الزيادة لأعمال معادة القياس</t>
-  </si>
-  <si>
-    <t>إجمالى قيمة الزيادة لأعمال معادة القياس</t>
-  </si>
 </sst>
 </file>
 
@@ -632,7 +620,7 @@
     <numFmt numFmtId="168" formatCode="[$-20B0000]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="169" formatCode="\م\س\ت\خ\ل\ص\ \ج\ا\ر\ى\ \ر\ق\م\ \(\ #\ \)"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -850,12 +838,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="20"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1456,7 +1438,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1792,11 +1774,218 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
@@ -1836,216 +2025,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="35" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2468,10 +2447,10 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A19" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2496,55 +2475,55 @@
       <c r="A1" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="132" t="s">
+      <c r="B1" s="181" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
+      <c r="C1" s="181"/>
+      <c r="D1" s="182"/>
+      <c r="E1" s="182"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="181" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="134" t="s">
+      <c r="C2" s="181"/>
+      <c r="D2" s="183" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
+      <c r="E2" s="183"/>
+      <c r="F2" s="183"/>
+      <c r="G2" s="183"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="181" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="132"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
+      <c r="C3" s="181"/>
+      <c r="D3" s="183"/>
+      <c r="E3" s="183"/>
+      <c r="F3" s="183"/>
+      <c r="G3" s="183"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="179" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131" t="s">
+      <c r="C4" s="179"/>
+      <c r="D4" s="180" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2567,22 +2546,22 @@
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="185"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="186" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="116"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="119"/>
+      <c r="E7" s="185"/>
+      <c r="F7" s="187"/>
+      <c r="G7" s="188"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="120"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
+      <c r="A8" s="189"/>
+      <c r="B8" s="190"/>
+      <c r="C8" s="191"/>
       <c r="D8" s="76" t="s">
         <v>57</v>
       </c>
@@ -2595,21 +2574,21 @@
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="192" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="125"/>
+      <c r="B9" s="193"/>
+      <c r="C9" s="194"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="195" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="127"/>
+      <c r="B10" s="196"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2617,10 +2596,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="175" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="129"/>
+      <c r="B11" s="176"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2628,10 +2607,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="175" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="129"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2639,10 +2618,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="175" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="129"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2650,10 +2629,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="128" t="s">
+      <c r="A14" s="175" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="129"/>
+      <c r="B14" s="176"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2661,10 +2640,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="175" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="129"/>
+      <c r="B15" s="176"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2672,10 +2651,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="156" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="157"/>
       <c r="C16" s="65" t="s">
         <v>39</v>
       </c>
@@ -2685,10 +2664,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="135" t="s">
+      <c r="A17" s="166" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="136"/>
+      <c r="B17" s="167"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16-D15-D14+D13+D12+D11+D10</f>
@@ -2714,21 +2693,21 @@
       <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="137" t="s">
+      <c r="A19" s="171" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="138"/>
-      <c r="C19" s="138"/>
+      <c r="B19" s="172"/>
+      <c r="C19" s="172"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="139" t="s">
+      <c r="A20" s="173" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="140"/>
+      <c r="B20" s="174"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2738,10 +2717,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="141" t="s">
+      <c r="A21" s="177" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="142"/>
+      <c r="B21" s="178"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30"/>
       <c r="E21" s="54"/>
@@ -2751,10 +2730,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="128" t="s">
+      <c r="A22" s="175" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="129"/>
+      <c r="B22" s="176"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2764,674 +2743,575 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="143" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="144"/>
-      <c r="C23" s="197" t="s">
-        <v>73</v>
-      </c>
+      <c r="A23" s="175" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="176"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="30"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="92"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="93">
+        <v>4</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="143" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="144"/>
-      <c r="C24" s="197" t="s">
-        <v>74</v>
-      </c>
+      <c r="A24" s="175" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="176"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="30"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="92"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="92">
+        <v>5</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="128" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="129"/>
-      <c r="C25" s="53"/>
+      <c r="A25" s="175" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="176"/>
+      <c r="C25" s="103"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
       <c r="G25" s="93">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="128" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="129"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="92">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="128" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="129"/>
-      <c r="C27" s="103"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="93">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="113" t="s">
+    <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="156" t="s">
         <v>45</v>
       </c>
-      <c r="B28" s="114"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="93">
+      <c r="B26" s="157"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="51"/>
+      <c r="F26" s="51"/>
+      <c r="G26" s="93">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="145" t="s">
+    <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="B29" s="146"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="25">
-        <f>D20+D21+D22+D25-D26+D27-D28</f>
+      <c r="B27" s="159"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="25">
+        <f>D20+D21+D22+D23+D24+D25+D26</f>
         <v>0</v>
       </c>
-      <c r="E29" s="25">
-        <f t="shared" ref="E29:F29" si="1">E20+E21+E22+E25-E26+E27-E28</f>
+      <c r="E27" s="25">
+        <f>E20+E21+E22+E23-E24+E25-E26</f>
         <v>0</v>
       </c>
-      <c r="F29" s="25">
+      <c r="F27" s="25">
+        <f>F20+F21+F22+F23-F24+F25-F26</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="150" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" s="151"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="95">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="160" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="161"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="96">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="162" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="163"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="97">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="164" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="165"/>
+      <c r="C31" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="87"/>
+      <c r="E31" s="88"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="98">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A32" s="166" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" s="167"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="25">
+        <f>D27+D28+D29+D30+D31</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="25">
+        <f t="shared" ref="E32:F32" si="1">E27+E28+E29+E30+E31</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="25">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G29" s="94">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="147" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="148"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="49"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="95">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="143" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="144"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="96">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="151" t="s">
-        <v>41</v>
-      </c>
-      <c r="B32" s="152"/>
-      <c r="C32" s="44"/>
-      <c r="D32" s="43"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="97">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="153" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="154"/>
-      <c r="C33" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="88"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="98">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="135" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="136"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="25">
-        <f>D29+D30+D31+D32+D33</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="25">
-        <f t="shared" ref="E34:F34" si="2">E29+E30+E31+E32+E33</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G34" s="94">
+      <c r="G32" s="94">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="38"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="108"/>
-    </row>
-    <row r="36" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="155" t="s">
+    <row r="33" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A33" s="38"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="37"/>
+      <c r="G33" s="108"/>
+    </row>
+    <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A34" s="168" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="156"/>
-      <c r="C36" s="157"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="99"/>
+      <c r="B34" s="169"/>
+      <c r="C34" s="170"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="99"/>
+    </row>
+    <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="142" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="143"/>
+      <c r="C35" s="33"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="100">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="142" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="143"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="100">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" s="150"/>
+      <c r="A37" s="142" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="143"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
       <c r="G37" s="100">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="149" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="150"/>
-      <c r="C38" s="33"/>
+      <c r="A38" s="144" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="145"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
       <c r="G38" s="100">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="149" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="150"/>
-      <c r="C39" s="33"/>
+      <c r="A39" s="144" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="145"/>
+      <c r="C39" s="32"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
       <c r="G39" s="100">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="161" t="s">
-        <v>33</v>
-      </c>
-      <c r="B40" s="162"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="146" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="147"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="100">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="161" t="s">
-        <v>32</v>
-      </c>
-      <c r="B41" s="162"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="100">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="163" t="s">
-        <v>31</v>
-      </c>
-      <c r="B42" s="164"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="100">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="165" t="s">
+    <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="B43" s="166"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="26">
-        <f>D36+D37+D38+D39+D40+D41+D42</f>
+      <c r="B41" s="149"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="26">
+        <f>D34+D35+D36+D37+D38+D39+D40</f>
         <v>0</v>
       </c>
-      <c r="E43" s="26">
-        <f t="shared" ref="E43:F43" si="3">E36+E37+E38+E39+E40+E41+E42</f>
+      <c r="E41" s="26">
+        <f t="shared" ref="E41:F41" si="2">E34+E35+E36+E37+E38+E39+E40</f>
         <v>0</v>
       </c>
-      <c r="F43" s="26">
+      <c r="F41" s="26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="101">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="24"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="109"/>
+    </row>
+    <row r="43" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="89" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="90"/>
+      <c r="C43" s="90"/>
+      <c r="D43" s="90"/>
+      <c r="E43" s="90"/>
+      <c r="F43" s="90"/>
+      <c r="G43" s="110"/>
+    </row>
+    <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" s="150" t="s">
+        <v>28</v>
+      </c>
+      <c r="B44" s="151"/>
+      <c r="C44" s="22">
+        <v>2</v>
+      </c>
+      <c r="D44" s="21">
+        <f>D32-D41</f>
+        <v>0</v>
+      </c>
+      <c r="E44" s="21">
+        <f t="shared" ref="E44:F44" si="3">E32-E41</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="21">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G43" s="101">
+      <c r="G44" s="95">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="152" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="153"/>
+      <c r="C45" s="20">
+        <f>C44</f>
+        <v>2</v>
+      </c>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="102">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="154" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="155"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="94">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="16"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="111"/>
+    </row>
+    <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="139" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="140"/>
+      <c r="C48" s="140"/>
+      <c r="D48" s="140"/>
+      <c r="E48" s="140"/>
+      <c r="F48" s="140"/>
+      <c r="G48" s="141"/>
+    </row>
+    <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="116" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="118"/>
+      <c r="D49" s="130" t="s">
+        <v>22</v>
+      </c>
+      <c r="E49" s="132"/>
+      <c r="F49" s="131" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="132"/>
+    </row>
+    <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A50" s="114"/>
+      <c r="B50" s="134" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="24"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="23"/>
-      <c r="G44" s="109"/>
-    </row>
-    <row r="45" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="89" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="90"/>
-      <c r="C45" s="90"/>
-      <c r="D45" s="90"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="90"/>
-      <c r="G45" s="110"/>
-    </row>
-    <row r="46" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="147" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="148"/>
-      <c r="C46" s="22">
+      <c r="C50" s="136"/>
+      <c r="D50" s="134"/>
+      <c r="E50" s="136"/>
+      <c r="F50" s="135"/>
+      <c r="G50" s="136"/>
+    </row>
+    <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="115"/>
+      <c r="B51" s="128"/>
+      <c r="C51" s="129"/>
+      <c r="D51" s="128"/>
+      <c r="E51" s="129"/>
+      <c r="F51" s="137"/>
+      <c r="G51" s="138"/>
+    </row>
+    <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A52" s="124" t="s">
+        <v>19</v>
+      </c>
+      <c r="B52" s="125"/>
+      <c r="C52" s="125"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="125"/>
+      <c r="F52" s="125"/>
+      <c r="G52" s="126"/>
+    </row>
+    <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A53" s="113" t="s">
+        <v>18</v>
+      </c>
+      <c r="B53" s="130" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="131"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="131" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="131"/>
+      <c r="G53" s="132"/>
+    </row>
+    <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A54" s="114"/>
+      <c r="B54" s="134"/>
+      <c r="C54" s="135"/>
+      <c r="D54" s="136"/>
+      <c r="E54" s="135"/>
+      <c r="F54" s="135"/>
+      <c r="G54" s="136"/>
+    </row>
+    <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A55" s="115"/>
+      <c r="B55" s="128"/>
+      <c r="C55" s="133"/>
+      <c r="D55" s="129"/>
+      <c r="E55" s="137"/>
+      <c r="F55" s="137"/>
+      <c r="G55" s="138"/>
+    </row>
+    <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="124" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="125"/>
+      <c r="C56" s="125"/>
+      <c r="D56" s="125"/>
+      <c r="E56" s="125"/>
+      <c r="F56" s="125"/>
+      <c r="G56" s="126"/>
+    </row>
+    <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A57" s="113" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="116" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="118"/>
+      <c r="D57" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" s="118"/>
+      <c r="F57" s="116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G57" s="118"/>
+    </row>
+    <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="114"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="127"/>
+      <c r="E58" s="120"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A59" s="114"/>
+      <c r="B59" s="128" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="129"/>
+      <c r="D59" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" s="123"/>
+      <c r="F59" s="122" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="123"/>
+    </row>
+    <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A60" s="114"/>
+      <c r="B60" s="130" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="131"/>
+      <c r="D60" s="132"/>
+      <c r="E60" s="116" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" s="117"/>
+      <c r="G60" s="118"/>
+    </row>
+    <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A61" s="114"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="8"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A62" s="115"/>
+      <c r="B62" s="128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="133"/>
+      <c r="D62" s="129"/>
+      <c r="E62" s="121" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="122"/>
+      <c r="G62" s="123"/>
+    </row>
+    <row r="63" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A63" s="113" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="116" t="s">
+        <v>3</v>
+      </c>
+      <c r="C63" s="117"/>
+      <c r="D63" s="118"/>
+      <c r="E63" s="116" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="21">
-        <f>D34-D43</f>
+      <c r="F63" s="117"/>
+      <c r="G63" s="118"/>
+    </row>
+    <row r="64" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A64" s="114"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="119"/>
+      <c r="G64" s="120"/>
+    </row>
+    <row r="65" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A65" s="115"/>
+      <c r="B65" s="121" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="122"/>
+      <c r="D65" s="123"/>
+      <c r="E65" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="E46" s="21">
-        <f t="shared" ref="E46:F46" si="4">E34-E43</f>
-        <v>0</v>
-      </c>
-      <c r="F46" s="21">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="G46" s="95">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A47" s="167" t="s">
-        <v>27</v>
-      </c>
-      <c r="B47" s="168"/>
-      <c r="C47" s="20">
-        <f>C46-1</f>
-        <v>1</v>
-      </c>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="102">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="169" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="170"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="94">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="16"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="111"/>
-    </row>
-    <row r="50" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A50" s="158" t="s">
-        <v>25</v>
-      </c>
-      <c r="B50" s="159"/>
-      <c r="C50" s="159"/>
-      <c r="D50" s="159"/>
-      <c r="E50" s="159"/>
-      <c r="F50" s="159"/>
-      <c r="G50" s="160"/>
-    </row>
-    <row r="51" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="171" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="174" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="175"/>
-      <c r="D51" s="176" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="177"/>
-      <c r="F51" s="178" t="s">
-        <v>21</v>
-      </c>
-      <c r="G51" s="177"/>
-    </row>
-    <row r="52" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="172"/>
-      <c r="B52" s="179" t="s">
-        <v>20</v>
-      </c>
-      <c r="C52" s="180"/>
-      <c r="D52" s="179"/>
-      <c r="E52" s="180"/>
-      <c r="F52" s="181"/>
-      <c r="G52" s="180"/>
-    </row>
-    <row r="53" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="173"/>
-      <c r="B53" s="182"/>
-      <c r="C53" s="183"/>
-      <c r="D53" s="182"/>
-      <c r="E53" s="183"/>
-      <c r="F53" s="184"/>
-      <c r="G53" s="185"/>
-    </row>
-    <row r="54" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="186" t="s">
-        <v>19</v>
-      </c>
-      <c r="B54" s="187"/>
-      <c r="C54" s="187"/>
-      <c r="D54" s="187"/>
-      <c r="E54" s="187"/>
-      <c r="F54" s="187"/>
-      <c r="G54" s="188"/>
-    </row>
-    <row r="55" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="171" t="s">
-        <v>18</v>
-      </c>
-      <c r="B55" s="176" t="s">
-        <v>17</v>
-      </c>
-      <c r="C55" s="178"/>
-      <c r="D55" s="177"/>
-      <c r="E55" s="178" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" s="178"/>
-      <c r="G55" s="177"/>
-    </row>
-    <row r="56" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="172"/>
-      <c r="B56" s="179"/>
-      <c r="C56" s="181"/>
-      <c r="D56" s="180"/>
-      <c r="E56" s="181"/>
-      <c r="F56" s="181"/>
-      <c r="G56" s="180"/>
-    </row>
-    <row r="57" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="173"/>
-      <c r="B57" s="182"/>
-      <c r="C57" s="189"/>
-      <c r="D57" s="183"/>
-      <c r="E57" s="184"/>
-      <c r="F57" s="184"/>
-      <c r="G57" s="185"/>
-    </row>
-    <row r="58" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="186" t="s">
-        <v>15</v>
-      </c>
-      <c r="B58" s="187"/>
-      <c r="C58" s="187"/>
-      <c r="D58" s="187"/>
-      <c r="E58" s="187"/>
-      <c r="F58" s="187"/>
-      <c r="G58" s="188"/>
-    </row>
-    <row r="59" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="171" t="s">
-        <v>14</v>
-      </c>
-      <c r="B59" s="174" t="s">
-        <v>13</v>
-      </c>
-      <c r="C59" s="175"/>
-      <c r="D59" s="174" t="s">
-        <v>12</v>
-      </c>
-      <c r="E59" s="175"/>
-      <c r="F59" s="174" t="s">
-        <v>11</v>
-      </c>
-      <c r="G59" s="175"/>
-    </row>
-    <row r="60" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="172"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="190"/>
-      <c r="E60" s="191"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="11"/>
-    </row>
-    <row r="61" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="172"/>
-      <c r="B61" s="182" t="s">
-        <v>10</v>
-      </c>
-      <c r="C61" s="183"/>
-      <c r="D61" s="192" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="193"/>
-      <c r="F61" s="194" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" s="193"/>
-    </row>
-    <row r="62" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="172"/>
-      <c r="B62" s="176" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" s="178"/>
-      <c r="D62" s="177"/>
-      <c r="E62" s="174" t="s">
-        <v>7</v>
-      </c>
-      <c r="F62" s="195"/>
-      <c r="G62" s="175"/>
-    </row>
-    <row r="63" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="172"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="9"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="173"/>
-      <c r="B64" s="182" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" s="189"/>
-      <c r="D64" s="183"/>
-      <c r="E64" s="192" t="s">
-        <v>5</v>
-      </c>
-      <c r="F64" s="194"/>
-      <c r="G64" s="193"/>
-    </row>
-    <row r="65" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="171" t="s">
-        <v>4</v>
-      </c>
-      <c r="B65" s="174" t="s">
-        <v>3</v>
-      </c>
-      <c r="C65" s="195"/>
-      <c r="D65" s="175"/>
-      <c r="E65" s="174" t="s">
-        <v>2</v>
-      </c>
-      <c r="F65" s="195"/>
-      <c r="G65" s="175"/>
-    </row>
-    <row r="66" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="172"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="196"/>
-      <c r="G66" s="191"/>
-    </row>
-    <row r="67" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="173"/>
-      <c r="B67" s="192" t="s">
-        <v>1</v>
-      </c>
-      <c r="C67" s="194"/>
-      <c r="D67" s="193"/>
-      <c r="E67" s="192" t="s">
-        <v>0</v>
-      </c>
-      <c r="F67" s="194"/>
-      <c r="G67" s="193"/>
+      <c r="F65" s="122"/>
+      <c r="G65" s="123"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="A58:G58"/>
-    <mergeCell ref="A59:A64"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="A54:G54"/>
-    <mergeCell ref="A55:A57"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="E56:G56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="E57:G57"/>
-    <mergeCell ref="A51:A53"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
+  <mergeCells count="83">
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D7:E7"/>
@@ -3444,6 +3324,77 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to format payment number in Arabic and improve merged cell handling in ExcelModifier.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C75E3857-703C-4901-B6C7-15D1A6747316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1456240A-6FC5-46A8-BFEF-26876212165A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -602,10 +602,6 @@
   </si>
   <si>
     <t xml:space="preserve">مستخلص جاري رقم (2) </t>
-  </si>
-  <si>
-    <t>عقد تنفيذ فيلات منطقة V35 -مدينتى
-عن أعمال حتى 31 يناير 2025</t>
   </si>
 </sst>
 </file>
@@ -1774,92 +1770,113 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1867,60 +1884,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1931,12 +1894,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1948,82 +1905,121 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2449,8 +2445,8 @@
   </sheetPr>
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A28" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2475,55 +2471,53 @@
       <c r="A1" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="181" t="s">
+      <c r="B1" s="132" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="181"/>
-      <c r="D1" s="182"/>
-      <c r="E1" s="182"/>
+      <c r="C1" s="132"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
     </row>
     <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="181" t="s">
+      <c r="B2" s="132" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="183" t="s">
-        <v>72</v>
-      </c>
-      <c r="E2" s="183"/>
-      <c r="F2" s="183"/>
-      <c r="G2" s="183"/>
+      <c r="C2" s="132"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="181" t="s">
+      <c r="B3" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="183"/>
-      <c r="E3" s="183"/>
-      <c r="F3" s="183"/>
-      <c r="G3" s="183"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="134"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="134"/>
+      <c r="G3" s="134"/>
     </row>
     <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="179"/>
-      <c r="D4" s="180" t="s">
+      <c r="C4" s="130"/>
+      <c r="D4" s="131" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="131"/>
+      <c r="G4" s="131"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2546,22 +2540,22 @@
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="115" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="185"/>
+      <c r="B7" s="116"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="186" t="s">
+      <c r="D7" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="185"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="188"/>
+      <c r="E7" s="116"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="119"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="189"/>
-      <c r="B8" s="190"/>
-      <c r="C8" s="191"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="122"/>
       <c r="D8" s="76" t="s">
         <v>57</v>
       </c>
@@ -2574,21 +2568,21 @@
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="192" t="s">
+      <c r="A9" s="123" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="194"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="125"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="195" t="s">
+      <c r="A10" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="196"/>
+      <c r="B10" s="127"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2596,10 +2590,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="175" t="s">
+      <c r="A11" s="128" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="176"/>
+      <c r="B11" s="129"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2607,10 +2601,10 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="175" t="s">
+      <c r="A12" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="176"/>
+      <c r="B12" s="129"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
@@ -2618,10 +2612,10 @@
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="175" t="s">
+      <c r="A13" s="128" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="176"/>
+      <c r="B13" s="129"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2629,10 +2623,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="175" t="s">
+      <c r="A14" s="128" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="176"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2640,10 +2634,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="175" t="s">
+      <c r="A15" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="176"/>
+      <c r="B15" s="129"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2651,10 +2645,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="157"/>
+      <c r="B16" s="114"/>
       <c r="C16" s="65" t="s">
         <v>39</v>
       </c>
@@ -2664,10 +2658,10 @@
       <c r="G16" s="64"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="166" t="s">
+      <c r="A17" s="135" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="167"/>
+      <c r="B17" s="136"/>
       <c r="C17" s="63"/>
       <c r="D17" s="62">
         <f>D16-D15-D14+D13+D12+D11+D10</f>
@@ -2693,21 +2687,21 @@
       <c r="G18" s="107"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="171" t="s">
+      <c r="A19" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="172"/>
-      <c r="C19" s="172"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
       <c r="D19" s="57"/>
       <c r="E19" s="58"/>
       <c r="F19" s="57"/>
       <c r="G19" s="91"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="173" t="s">
+      <c r="A20" s="139" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="174"/>
+      <c r="B20" s="140"/>
       <c r="C20" s="56"/>
       <c r="D20" s="30"/>
       <c r="E20" s="30"/>
@@ -2717,10 +2711,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="177" t="s">
+      <c r="A21" s="141" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="178"/>
+      <c r="B21" s="142"/>
       <c r="C21" s="55"/>
       <c r="D21" s="30"/>
       <c r="E21" s="54"/>
@@ -2730,10 +2724,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="175" t="s">
+      <c r="A22" s="128" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="176"/>
+      <c r="B22" s="129"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2743,10 +2737,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="175" t="s">
+      <c r="A23" s="128" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="176"/>
+      <c r="B23" s="129"/>
       <c r="C23" s="53"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
@@ -2756,10 +2750,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="175" t="s">
+      <c r="A24" s="128" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="176"/>
+      <c r="B24" s="129"/>
       <c r="C24" s="53"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -2769,10 +2763,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="175" t="s">
+      <c r="A25" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="176"/>
+      <c r="B25" s="129"/>
       <c r="C25" s="103"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2782,10 +2776,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="157"/>
+      <c r="B26" s="114"/>
       <c r="C26" s="52"/>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
@@ -2795,10 +2789,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="158" t="s">
+      <c r="A27" s="143" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="159"/>
+      <c r="B27" s="144"/>
       <c r="C27" s="39"/>
       <c r="D27" s="25">
         <f>D20+D21+D22+D23+D24+D25+D26</f>
@@ -2817,10 +2811,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="150" t="s">
+      <c r="A28" s="145" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="151"/>
+      <c r="B28" s="146"/>
       <c r="C28" s="50"/>
       <c r="D28" s="49"/>
       <c r="E28" s="48"/>
@@ -2830,10 +2824,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="160" t="s">
+      <c r="A29" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="161"/>
+      <c r="B29" s="148"/>
       <c r="C29" s="47"/>
       <c r="D29" s="46"/>
       <c r="E29" s="45"/>
@@ -2843,10 +2837,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="162" t="s">
+      <c r="A30" s="151" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="163"/>
+      <c r="B30" s="152"/>
       <c r="C30" s="44"/>
       <c r="D30" s="43"/>
       <c r="E30" s="42"/>
@@ -2856,10 +2850,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="164" t="s">
+      <c r="A31" s="153" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="165"/>
+      <c r="B31" s="154"/>
       <c r="C31" s="41" t="s">
         <v>39</v>
       </c>
@@ -2871,10 +2865,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="166" t="s">
+      <c r="A32" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="167"/>
+      <c r="B32" s="136"/>
       <c r="C32" s="39"/>
       <c r="D32" s="25">
         <f>D27+D28+D29+D30+D31</f>
@@ -2902,21 +2896,21 @@
       <c r="G33" s="108"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="168" t="s">
+      <c r="A34" s="155" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="169"/>
-      <c r="C34" s="170"/>
+      <c r="B34" s="156"/>
+      <c r="C34" s="157"/>
       <c r="D34" s="36"/>
       <c r="E34" s="35"/>
       <c r="F34" s="34"/>
       <c r="G34" s="99"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="142" t="s">
+      <c r="A35" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="143"/>
+      <c r="B35" s="150"/>
       <c r="C35" s="33"/>
       <c r="D35" s="31"/>
       <c r="E35" s="30"/>
@@ -2926,10 +2920,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="142" t="s">
+      <c r="A36" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="143"/>
+      <c r="B36" s="150"/>
       <c r="C36" s="33"/>
       <c r="D36" s="31"/>
       <c r="E36" s="30"/>
@@ -2939,10 +2933,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="142" t="s">
+      <c r="A37" s="149" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="143"/>
+      <c r="B37" s="150"/>
       <c r="C37" s="33"/>
       <c r="D37" s="31"/>
       <c r="E37" s="30"/>
@@ -2952,10 +2946,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="144" t="s">
+      <c r="A38" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="145"/>
+      <c r="B38" s="162"/>
       <c r="C38" s="32"/>
       <c r="D38" s="31"/>
       <c r="E38" s="30"/>
@@ -2965,10 +2959,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="144" t="s">
+      <c r="A39" s="161" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="145"/>
+      <c r="B39" s="162"/>
       <c r="C39" s="32"/>
       <c r="D39" s="31"/>
       <c r="E39" s="30"/>
@@ -2978,10 +2972,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="146" t="s">
+      <c r="A40" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="147"/>
+      <c r="B40" s="164"/>
       <c r="C40" s="29"/>
       <c r="D40" s="28"/>
       <c r="E40" s="19"/>
@@ -2991,10 +2985,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="148" t="s">
+      <c r="A41" s="165" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="149"/>
+      <c r="B41" s="166"/>
       <c r="C41" s="27"/>
       <c r="D41" s="26">
         <f>D34+D35+D36+D37+D38+D39+D40</f>
@@ -3033,10 +3027,10 @@
       <c r="G43" s="110"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="150" t="s">
+      <c r="A44" s="145" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="151"/>
+      <c r="B44" s="146"/>
       <c r="C44" s="22">
         <v>2</v>
       </c>
@@ -3057,10 +3051,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="152" t="s">
+      <c r="A45" s="167" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="153"/>
+      <c r="B45" s="168"/>
       <c r="C45" s="20">
         <f>C44</f>
         <v>2</v>
@@ -3073,10 +3067,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="154" t="s">
+      <c r="A46" s="169" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="155"/>
+      <c r="B46" s="170"/>
       <c r="C46" s="18"/>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -3095,164 +3089,164 @@
       <c r="G47" s="111"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="139" t="s">
+      <c r="A48" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="140"/>
-      <c r="C48" s="140"/>
-      <c r="D48" s="140"/>
-      <c r="E48" s="140"/>
-      <c r="F48" s="140"/>
-      <c r="G48" s="141"/>
+      <c r="B48" s="159"/>
+      <c r="C48" s="159"/>
+      <c r="D48" s="159"/>
+      <c r="E48" s="159"/>
+      <c r="F48" s="159"/>
+      <c r="G48" s="160"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="113" t="s">
+      <c r="A49" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="116" t="s">
+      <c r="B49" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="118"/>
-      <c r="D49" s="130" t="s">
+      <c r="C49" s="175"/>
+      <c r="D49" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="132"/>
-      <c r="F49" s="131" t="s">
+      <c r="E49" s="177"/>
+      <c r="F49" s="178" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="132"/>
+      <c r="G49" s="177"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="114"/>
-      <c r="B50" s="134" t="s">
+      <c r="A50" s="172"/>
+      <c r="B50" s="179" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="136"/>
-      <c r="D50" s="134"/>
-      <c r="E50" s="136"/>
-      <c r="F50" s="135"/>
-      <c r="G50" s="136"/>
+      <c r="C50" s="180"/>
+      <c r="D50" s="179"/>
+      <c r="E50" s="180"/>
+      <c r="F50" s="181"/>
+      <c r="G50" s="180"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="115"/>
-      <c r="B51" s="128"/>
-      <c r="C51" s="129"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="129"/>
-      <c r="F51" s="137"/>
-      <c r="G51" s="138"/>
+      <c r="A51" s="173"/>
+      <c r="B51" s="182"/>
+      <c r="C51" s="183"/>
+      <c r="D51" s="182"/>
+      <c r="E51" s="183"/>
+      <c r="F51" s="184"/>
+      <c r="G51" s="185"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="124" t="s">
+      <c r="A52" s="186" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="125"/>
-      <c r="C52" s="125"/>
-      <c r="D52" s="125"/>
-      <c r="E52" s="125"/>
-      <c r="F52" s="125"/>
-      <c r="G52" s="126"/>
+      <c r="B52" s="187"/>
+      <c r="C52" s="187"/>
+      <c r="D52" s="187"/>
+      <c r="E52" s="187"/>
+      <c r="F52" s="187"/>
+      <c r="G52" s="188"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="113" t="s">
+      <c r="A53" s="171" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="130" t="s">
+      <c r="B53" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="131"/>
-      <c r="D53" s="132"/>
-      <c r="E53" s="131" t="s">
+      <c r="C53" s="178"/>
+      <c r="D53" s="177"/>
+      <c r="E53" s="178" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="131"/>
-      <c r="G53" s="132"/>
+      <c r="F53" s="178"/>
+      <c r="G53" s="177"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="114"/>
-      <c r="B54" s="134"/>
-      <c r="C54" s="135"/>
-      <c r="D54" s="136"/>
-      <c r="E54" s="135"/>
-      <c r="F54" s="135"/>
-      <c r="G54" s="136"/>
+      <c r="A54" s="172"/>
+      <c r="B54" s="179"/>
+      <c r="C54" s="181"/>
+      <c r="D54" s="180"/>
+      <c r="E54" s="181"/>
+      <c r="F54" s="181"/>
+      <c r="G54" s="180"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="115"/>
-      <c r="B55" s="128"/>
-      <c r="C55" s="133"/>
-      <c r="D55" s="129"/>
-      <c r="E55" s="137"/>
-      <c r="F55" s="137"/>
-      <c r="G55" s="138"/>
+      <c r="A55" s="173"/>
+      <c r="B55" s="182"/>
+      <c r="C55" s="189"/>
+      <c r="D55" s="183"/>
+      <c r="E55" s="184"/>
+      <c r="F55" s="184"/>
+      <c r="G55" s="185"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="124" t="s">
+      <c r="A56" s="186" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="125"/>
-      <c r="C56" s="125"/>
-      <c r="D56" s="125"/>
-      <c r="E56" s="125"/>
-      <c r="F56" s="125"/>
-      <c r="G56" s="126"/>
+      <c r="B56" s="187"/>
+      <c r="C56" s="187"/>
+      <c r="D56" s="187"/>
+      <c r="E56" s="187"/>
+      <c r="F56" s="187"/>
+      <c r="G56" s="188"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="113" t="s">
+      <c r="A57" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="116" t="s">
+      <c r="B57" s="174" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="118"/>
-      <c r="D57" s="116" t="s">
+      <c r="C57" s="175"/>
+      <c r="D57" s="174" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="118"/>
-      <c r="F57" s="116" t="s">
+      <c r="E57" s="175"/>
+      <c r="F57" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="118"/>
+      <c r="G57" s="175"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="114"/>
+      <c r="A58" s="172"/>
       <c r="B58" s="13"/>
       <c r="C58" s="6"/>
-      <c r="D58" s="127"/>
-      <c r="E58" s="120"/>
+      <c r="D58" s="190"/>
+      <c r="E58" s="191"/>
       <c r="F58" s="12"/>
       <c r="G58" s="11"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="114"/>
-      <c r="B59" s="128" t="s">
+      <c r="A59" s="172"/>
+      <c r="B59" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="129"/>
-      <c r="D59" s="121" t="s">
+      <c r="C59" s="183"/>
+      <c r="D59" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="123"/>
-      <c r="F59" s="122" t="s">
+      <c r="E59" s="193"/>
+      <c r="F59" s="194" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="123"/>
+      <c r="G59" s="193"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="114"/>
-      <c r="B60" s="130" t="s">
+      <c r="A60" s="172"/>
+      <c r="B60" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="131"/>
-      <c r="D60" s="132"/>
-      <c r="E60" s="116" t="s">
+      <c r="C60" s="178"/>
+      <c r="D60" s="177"/>
+      <c r="E60" s="174" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="117"/>
-      <c r="G60" s="118"/>
+      <c r="F60" s="195"/>
+      <c r="G60" s="175"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="114"/>
+      <c r="A61" s="172"/>
       <c r="B61" s="10"/>
       <c r="C61" s="9"/>
       <c r="D61" s="6"/>
@@ -3261,121 +3255,63 @@
       <c r="G61" s="6"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="115"/>
-      <c r="B62" s="128" t="s">
+      <c r="A62" s="173"/>
+      <c r="B62" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="133"/>
-      <c r="D62" s="129"/>
-      <c r="E62" s="121" t="s">
+      <c r="C62" s="189"/>
+      <c r="D62" s="183"/>
+      <c r="E62" s="192" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="122"/>
-      <c r="G62" s="123"/>
+      <c r="F62" s="194"/>
+      <c r="G62" s="193"/>
     </row>
     <row r="63" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="113" t="s">
+      <c r="A63" s="171" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="116" t="s">
+      <c r="B63" s="174" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="117"/>
-      <c r="D63" s="118"/>
-      <c r="E63" s="116" t="s">
+      <c r="C63" s="195"/>
+      <c r="D63" s="175"/>
+      <c r="E63" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="117"/>
-      <c r="G63" s="118"/>
+      <c r="F63" s="195"/>
+      <c r="G63" s="175"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="114"/>
+      <c r="A64" s="172"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
       <c r="D64" s="4"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="119"/>
-      <c r="G64" s="120"/>
+      <c r="F64" s="196"/>
+      <c r="G64" s="191"/>
     </row>
     <row r="65" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A65" s="115"/>
-      <c r="B65" s="121" t="s">
+      <c r="A65" s="173"/>
+      <c r="B65" s="192" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="122"/>
-      <c r="D65" s="123"/>
-      <c r="E65" s="121" t="s">
+      <c r="C65" s="194"/>
+      <c r="D65" s="193"/>
+      <c r="E65" s="192" t="s">
         <v>0</v>
       </c>
-      <c r="F65" s="122"/>
-      <c r="G65" s="123"/>
+      <c r="F65" s="194"/>
+      <c r="G65" s="193"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="E65:G65"/>
     <mergeCell ref="A56:G56"/>
     <mergeCell ref="A57:A62"/>
     <mergeCell ref="B57:C57"/>
@@ -3389,12 +3325,70 @@
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A63:A65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to change subtitle cell reference from D4 to E4
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1456240A-6FC5-46A8-BFEF-26876212165A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871468E9-E253-4FA9-9C6F-11AA7B74652C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -196,7 +196,7 @@
     <definedName name="PPP" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PRAYER" hidden="1">{#N/A,#N/A,FALSE,"CCTV"}</definedName>
     <definedName name="PrevDate">[1]Summary!$L$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">IPC!$A$1:$G$69</definedName>
     <definedName name="qeewq" hidden="1">{"offequipsch",#N/A,FALSE,"GTC_Schedule";"onconstsch",#N/A,FALSE,"GTC_Schedule";"techsch",#N/A,FALSE,"GTC_Schedule";"totsch",#N/A,FALSE,"GTC_Schedule"}</definedName>
     <definedName name="qp" hidden="1">#REF!</definedName>
     <definedName name="qqq" hidden="1">#REF!</definedName>
@@ -616,7 +616,7 @@
     <numFmt numFmtId="168" formatCode="[$-20B0000]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="169" formatCode="\م\س\ت\خ\ل\ص\ \ج\ا\ر\ى\ \ر\ق\م\ \(\ #\ \)"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -834,6 +834,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1434,7 +1444,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="203">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1770,6 +1780,9 @@
     <xf numFmtId="3" fontId="15" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1824,9 +1837,6 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
@@ -2020,6 +2030,24 @@
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="13" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
@@ -2045,25 +2073,25 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2496950</xdr:colOff>
+      <xdr:colOff>1726890</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>279831</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>781728</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>266983</xdr:rowOff>
+      <xdr:colOff>1023846</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>107022</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 2">
+        <xdr:cNvPr id="3" name="Picture 2" descr="Madinaty-logo – Furniture – Architouch">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2680F00-AA91-4D17-B8DF-AF48EE746B1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDFD3DD9-F1FB-C04D-F0CB-3D446DC2FBA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2072,7 +2100,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
@@ -2080,28 +2114,83 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10586497933" y="279831"/>
-          <a:ext cx="1545880" cy="536050"/>
+          <a:off x="10526905143" y="0"/>
+          <a:ext cx="2557574" cy="1933539"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:srgbClr val="FF3300"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw dist="107763" dir="2700000" algn="ctr" rotWithShape="0">
-            <a:srgbClr val="808080">
-              <a:alpha val="50000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>35674</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>21404</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1016357</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>250114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Autodesk Construction Cloud">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52823F81-5F7D-5AB8-CC05-9CFB5EDE61F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="10526912632" y="21782640"/>
+          <a:ext cx="7501919" cy="999272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -2443,10 +2532,10 @@
     <tabColor theme="9" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A58" zoomScale="89" zoomScaleNormal="100" zoomScaleSheetLayoutView="59" zoomScalePageLayoutView="44" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2467,7 +2556,7 @@
     <col min="22" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="85" t="s">
         <v>65</v>
       </c>
@@ -2478,7 +2567,7 @@
       <c r="D1" s="133"/>
       <c r="E1" s="133"/>
     </row>
-    <row r="2" spans="1:7" ht="20" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="85" t="s">
         <v>63</v>
       </c>
@@ -2489,9 +2578,9 @@
       <c r="D2" s="134"/>
       <c r="E2" s="134"/>
       <c r="F2" s="134"/>
-      <c r="G2" s="134"/>
-    </row>
-    <row r="3" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="G2" s="198"/>
+    </row>
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="85" t="s">
         <v>62</v>
       </c>
@@ -2502,22 +2591,21 @@
       <c r="D3" s="134"/>
       <c r="E3" s="134"/>
       <c r="F3" s="134"/>
-      <c r="G3" s="134"/>
-    </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="131" t="s">
+      <c r="C4" s="131"/>
+      <c r="E4" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="131"/>
-      <c r="F4" s="131"/>
-      <c r="G4" s="131"/>
+      <c r="F4" s="197"/>
+      <c r="G4" s="197"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="84"/>
@@ -2540,22 +2628,22 @@
       <c r="G6" s="105"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="116" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="116"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="77"/>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="116"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="119"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="120"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="120"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="123"/>
       <c r="D8" s="76" t="s">
         <v>57</v>
       </c>
@@ -2568,21 +2656,21 @@
       <c r="G8" s="106"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="125"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="126"/>
       <c r="D9" s="72"/>
       <c r="E9" s="73"/>
       <c r="F9" s="72"/>
       <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="126" t="s">
+      <c r="A10" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="127"/>
+      <c r="B10" s="128"/>
       <c r="C10" s="71"/>
       <c r="D10" s="112"/>
       <c r="E10" s="30"/>
@@ -2590,10 +2678,10 @@
       <c r="G10" s="67"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="128" t="s">
+      <c r="A11" s="129" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="129"/>
+      <c r="B11" s="130"/>
       <c r="C11" s="69"/>
       <c r="D11" s="30"/>
       <c r="E11" s="30"/>
@@ -2601,21 +2689,21 @@
       <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="129"/>
+      <c r="B12" s="130"/>
       <c r="C12" s="69"/>
       <c r="D12" s="30"/>
       <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="F12"/>
       <c r="G12" s="67"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="128" t="s">
+      <c r="A13" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="129"/>
+      <c r="B13" s="130"/>
       <c r="C13" s="66"/>
       <c r="D13" s="30"/>
       <c r="E13" s="30"/>
@@ -2623,10 +2711,10 @@
       <c r="G13" s="67"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="128" t="s">
+      <c r="A14" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="129"/>
+      <c r="B14" s="130"/>
       <c r="C14" s="68"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
@@ -2634,10 +2722,10 @@
       <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="128" t="s">
+      <c r="A15" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="129"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="68"/>
       <c r="D15" s="31"/>
       <c r="E15" s="31"/>
@@ -2645,10 +2733,10 @@
       <c r="G15" s="64"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="113" t="s">
+      <c r="A16" s="114" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="114"/>
+      <c r="B16" s="115"/>
       <c r="C16" s="65" t="s">
         <v>39</v>
       </c>
@@ -2724,10 +2812,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="128" t="s">
+      <c r="A22" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="129"/>
+      <c r="B22" s="130"/>
       <c r="C22" s="86"/>
       <c r="D22" s="30"/>
       <c r="E22" s="54"/>
@@ -2737,10 +2825,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="128" t="s">
+      <c r="A23" s="129" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="129"/>
+      <c r="B23" s="130"/>
       <c r="C23" s="53"/>
       <c r="D23" s="30"/>
       <c r="E23" s="30"/>
@@ -2750,10 +2838,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="128" t="s">
+      <c r="A24" s="129" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="129"/>
+      <c r="B24" s="130"/>
       <c r="C24" s="53"/>
       <c r="D24" s="30"/>
       <c r="E24" s="30"/>
@@ -2763,10 +2851,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="128" t="s">
+      <c r="A25" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="129"/>
+      <c r="B25" s="130"/>
       <c r="C25" s="103"/>
       <c r="D25" s="30"/>
       <c r="E25" s="30"/>
@@ -2776,10 +2864,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="114" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="114"/>
+      <c r="B26" s="115"/>
       <c r="C26" s="52"/>
       <c r="D26" s="51"/>
       <c r="E26" s="51"/>
@@ -3304,8 +3392,54 @@
       <c r="F65" s="194"/>
       <c r="G65" s="193"/>
     </row>
+    <row r="66" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A66" s="201" t="str">
+        <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
+        <v>Generated by Autodesk Construction Cloud on: 03 March 2025</v>
+      </c>
+      <c r="B66" s="201"/>
+      <c r="C66" s="201"/>
+      <c r="D66" s="201"/>
+      <c r="E66" s="199"/>
+      <c r="F66" s="199"/>
+      <c r="G66" s="199"/>
+    </row>
+    <row r="67" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="202"/>
+      <c r="B67" s="202"/>
+      <c r="C67" s="202"/>
+      <c r="D67" s="202"/>
+      <c r="E67" s="200"/>
+      <c r="F67" s="200"/>
+      <c r="G67" s="200"/>
+    </row>
+    <row r="68" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A68" s="202"/>
+      <c r="B68" s="202"/>
+      <c r="C68" s="202"/>
+      <c r="D68" s="202"/>
+      <c r="E68" s="200"/>
+      <c r="F68" s="200"/>
+      <c r="G68" s="200"/>
+    </row>
+    <row r="69" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="202"/>
+      <c r="B69" s="202"/>
+      <c r="C69" s="202"/>
+      <c r="D69" s="202"/>
+      <c r="E69" s="200"/>
+      <c r="F69" s="200"/>
+      <c r="G69" s="200"/>
+    </row>
+    <row r="72" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E72"/>
+    </row>
+    <row r="73" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D73"/>
+    </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="A66:D69"/>
     <mergeCell ref="A63:A65"/>
     <mergeCell ref="B63:D63"/>
     <mergeCell ref="E63:G63"/>
@@ -3371,12 +3505,11 @@
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:G3"/>
+    <mergeCell ref="D2:F3"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="D7:E7"/>

</xml_diff>

<commit_message>
fix: update ExcelModifier.py to set cell font to Times New Roman when modifying cell values
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6E87E9-C9D8-4837-8FBC-4890918E8C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623BE7A2-05F7-4D87-A105-AE9652EE2632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="2" r:id="rId1"/>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -602,6 +602,9 @@
   </si>
   <si>
     <t xml:space="preserve">مستخلص جاري رقم (2) </t>
+  </si>
+  <si>
+    <t>تاريخ المستخلص:</t>
   </si>
 </sst>
 </file>
@@ -793,11 +796,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="16"/>
       <name val="Arial"/>
@@ -846,6 +844,12 @@
       <sz val="16"/>
       <name val="Traditional Arabic"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1672,9 +1676,6 @@
     <xf numFmtId="168" fontId="7" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="2"/>
     </xf>
@@ -1690,7 +1691,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="28" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="166" fontId="24" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1708,40 +1709,40 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1759,13 +1760,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1783,40 +1784,52 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1954,6 +1967,63 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="65" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
     </xf>
@@ -1966,83 +2036,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="65" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2075,8 +2079,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1023846</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>791</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>542247</xdr:rowOff>
     </xdr:to>
@@ -2528,8 +2532,8 @@
   </sheetPr>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A36" zoomScale="76" zoomScaleNormal="100" zoomScaleSheetLayoutView="76" zoomScalePageLayoutView="44" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2551,93 +2555,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="179" t="s">
+      <c r="B1" s="178" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
+      <c r="C1" s="178"/>
+      <c r="D1" s="179"/>
+      <c r="E1" s="179"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="178" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="181"/>
-      <c r="G2" s="112"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="180"/>
+      <c r="G2" s="111"/>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="178" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="179"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
+      <c r="C3" s="178"/>
+      <c r="D3" s="180"/>
+      <c r="E3" s="180"/>
+      <c r="F3" s="180"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="177" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="E4" s="110" t="s">
+      <c r="C4" s="177"/>
+      <c r="E4" s="109" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="111"/>
-      <c r="G4" s="111"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="81"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="101"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="100"/>
     </row>
     <row r="6" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="78"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="76" t="s">
+      <c r="A6" s="77"/>
+      <c r="B6" s="196" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="196" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="75"/>
-      <c r="G6" s="102"/>
+      <c r="G6" s="101"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="182" t="s">
+      <c r="A7" s="197" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="183"/>
+      <c r="B7" s="198"/>
       <c r="C7" s="74"/>
-      <c r="D7" s="184" t="s">
+      <c r="D7" s="199" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="183"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="186"/>
+      <c r="E7" s="198"/>
+      <c r="F7" s="182"/>
+      <c r="G7" s="183"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="187"/>
-      <c r="B8" s="188"/>
-      <c r="C8" s="189"/>
+      <c r="A8" s="184"/>
+      <c r="B8" s="185"/>
+      <c r="C8" s="186"/>
       <c r="D8" s="73" t="s">
         <v>57</v>
       </c>
@@ -2647,35 +2653,35 @@
       <c r="F8" s="71" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="103"/>
+      <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="190" t="s">
+      <c r="A9" s="187" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="191"/>
-      <c r="C9" s="192"/>
+      <c r="B9" s="188"/>
+      <c r="C9" s="189"/>
       <c r="D9" s="69"/>
       <c r="E9" s="70"/>
       <c r="F9" s="69"/>
       <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="193" t="s">
+      <c r="A10" s="190" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="194"/>
+      <c r="B10" s="191"/>
       <c r="C10" s="68"/>
-      <c r="D10" s="109"/>
+      <c r="D10" s="108"/>
       <c r="E10" s="27"/>
       <c r="F10" s="67"/>
       <c r="G10" s="64"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="174" t="s">
+      <c r="A11" s="173" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="175"/>
+      <c r="B11" s="174"/>
       <c r="C11" s="66"/>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -2683,10 +2689,10 @@
       <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="174" t="s">
+      <c r="A12" s="173" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="175"/>
+      <c r="B12" s="174"/>
       <c r="C12" s="66"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -2694,10 +2700,10 @@
       <c r="G12" s="64"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="173" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="175"/>
+      <c r="B13" s="174"/>
       <c r="C13" s="63"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -2705,10 +2711,10 @@
       <c r="G13" s="64"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="174" t="s">
+      <c r="A14" s="173" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="175"/>
+      <c r="B14" s="174"/>
       <c r="C14" s="65"/>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -2716,10 +2722,10 @@
       <c r="G14" s="64"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="173" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="175"/>
+      <c r="B15" s="174"/>
       <c r="C15" s="65"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
@@ -2727,10 +2733,10 @@
       <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="155" t="s">
+      <c r="A16" s="158" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="156"/>
+      <c r="B16" s="159"/>
       <c r="C16" s="62" t="s">
         <v>39</v>
       </c>
@@ -2740,13 +2746,13 @@
       <c r="G16" s="61"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="165" t="s">
+      <c r="A17" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="166"/>
+      <c r="B17" s="169"/>
       <c r="C17" s="60"/>
       <c r="D17" s="59">
-        <f>D16-D15-D14+D13+D12+D11+D10</f>
+        <f>D10+D13+D14+D15+D16</f>
         <v>0</v>
       </c>
       <c r="E17" s="59">
@@ -2766,118 +2772,118 @@
       <c r="D18" s="56"/>
       <c r="E18" s="56"/>
       <c r="F18" s="56"/>
-      <c r="G18" s="104"/>
+      <c r="G18" s="103"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="170" t="s">
+      <c r="A19" s="192" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="171"/>
-      <c r="C19" s="171"/>
+      <c r="B19" s="193"/>
+      <c r="C19" s="193"/>
       <c r="D19" s="54"/>
       <c r="E19" s="55"/>
       <c r="F19" s="54"/>
-      <c r="G19" s="88"/>
+      <c r="G19" s="87"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="172" t="s">
+      <c r="A20" s="194" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="173"/>
+      <c r="B20" s="195"/>
       <c r="C20" s="53"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
-      <c r="G20" s="89">
+      <c r="G20" s="88">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="176" t="s">
+      <c r="A21" s="175" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="177"/>
+      <c r="B21" s="176"/>
       <c r="C21" s="52"/>
       <c r="D21" s="27"/>
       <c r="E21" s="51"/>
       <c r="F21" s="51"/>
-      <c r="G21" s="90">
+      <c r="G21" s="89">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="173" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="175"/>
-      <c r="C22" s="83"/>
+      <c r="B22" s="174"/>
+      <c r="C22" s="82"/>
       <c r="D22" s="27"/>
       <c r="E22" s="51"/>
       <c r="F22" s="51"/>
-      <c r="G22" s="89">
+      <c r="G22" s="88">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="174" t="s">
+      <c r="A23" s="173" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="175"/>
+      <c r="B23" s="174"/>
       <c r="C23" s="50"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
-      <c r="G23" s="90">
+      <c r="G23" s="89">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="174" t="s">
+      <c r="A24" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="175"/>
+      <c r="B24" s="174"/>
       <c r="C24" s="50"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
-      <c r="G24" s="89">
+      <c r="G24" s="88">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="174" t="s">
+      <c r="A25" s="173" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="175"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="174"/>
+      <c r="C25" s="99"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
-      <c r="G25" s="90">
+      <c r="G25" s="89">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="155" t="s">
+      <c r="A26" s="158" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="156"/>
+      <c r="B26" s="159"/>
       <c r="C26" s="49"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
       <c r="F26" s="48"/>
-      <c r="G26" s="90">
+      <c r="G26" s="89">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="157" t="s">
+      <c r="A27" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="158"/>
+      <c r="B27" s="161"/>
       <c r="C27" s="36"/>
       <c r="D27" s="22">
-        <f>D20+D21+D22+D23+D24+D25+D26</f>
+        <f>D20+D24+D25+D26</f>
         <v>0</v>
       </c>
       <c r="E27" s="22">
@@ -2888,69 +2894,69 @@
         <f>F20+F21+F22+F23-F24+F25-F26</f>
         <v>0</v>
       </c>
-      <c r="G27" s="91">
+      <c r="G27" s="90">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="149" t="s">
+      <c r="A28" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="150"/>
+      <c r="B28" s="153"/>
       <c r="C28" s="47"/>
       <c r="D28" s="46"/>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
-      <c r="G28" s="92">
+      <c r="G28" s="91">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="159" t="s">
+      <c r="A29" s="162" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="160"/>
+      <c r="B29" s="163"/>
       <c r="C29" s="44"/>
       <c r="D29" s="43"/>
       <c r="E29" s="42"/>
       <c r="F29" s="42"/>
-      <c r="G29" s="93">
+      <c r="G29" s="92">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="161" t="s">
+      <c r="A30" s="164" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="162"/>
+      <c r="B30" s="165"/>
       <c r="C30" s="41"/>
       <c r="D30" s="40"/>
       <c r="E30" s="39"/>
       <c r="F30" s="39"/>
-      <c r="G30" s="94">
+      <c r="G30" s="93">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="163" t="s">
+      <c r="A31" s="166" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="164"/>
+      <c r="B31" s="167"/>
       <c r="C31" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D31" s="84"/>
-      <c r="E31" s="85"/>
+      <c r="D31" s="83"/>
+      <c r="E31" s="84"/>
       <c r="F31" s="37"/>
-      <c r="G31" s="95">
+      <c r="G31" s="94">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="165" t="s">
+      <c r="A32" s="168" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="166"/>
+      <c r="B32" s="169"/>
       <c r="C32" s="36"/>
       <c r="D32" s="22">
         <f>D27+D28+D29+D30+D31</f>
@@ -2964,7 +2970,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="91">
+      <c r="G32" s="90">
         <v>13</v>
       </c>
     </row>
@@ -2975,105 +2981,105 @@
       <c r="D33" s="34"/>
       <c r="E33" s="34"/>
       <c r="F33" s="34"/>
-      <c r="G33" s="105"/>
+      <c r="G33" s="104"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="167" t="s">
+      <c r="A34" s="170" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="168"/>
-      <c r="C34" s="169"/>
+      <c r="B34" s="171"/>
+      <c r="C34" s="172"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
       <c r="F34" s="31"/>
-      <c r="G34" s="96"/>
+      <c r="G34" s="95"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="141" t="s">
+      <c r="A35" s="144" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="142"/>
+      <c r="B35" s="145"/>
       <c r="C35" s="30"/>
       <c r="D35" s="28"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
-      <c r="G35" s="97">
+      <c r="G35" s="96">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="141" t="s">
+      <c r="A36" s="144" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="142"/>
+      <c r="B36" s="145"/>
       <c r="C36" s="30"/>
       <c r="D36" s="28"/>
       <c r="E36" s="27"/>
       <c r="F36" s="27"/>
-      <c r="G36" s="97">
+      <c r="G36" s="96">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="141" t="s">
+      <c r="A37" s="144" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="142"/>
+      <c r="B37" s="145"/>
       <c r="C37" s="30"/>
       <c r="D37" s="28"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="97">
+      <c r="G37" s="96">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="143" t="s">
+      <c r="A38" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="144"/>
+      <c r="B38" s="147"/>
       <c r="C38" s="29"/>
       <c r="D38" s="28"/>
       <c r="E38" s="27"/>
       <c r="F38" s="27"/>
-      <c r="G38" s="97">
+      <c r="G38" s="96">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="143" t="s">
+      <c r="A39" s="146" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="144"/>
+      <c r="B39" s="147"/>
       <c r="C39" s="29"/>
       <c r="D39" s="28"/>
       <c r="E39" s="27"/>
       <c r="F39" s="27"/>
-      <c r="G39" s="97">
+      <c r="G39" s="96">
         <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="145" t="s">
+      <c r="A40" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="146"/>
+      <c r="B40" s="149"/>
       <c r="C40" s="26"/>
       <c r="D40" s="25"/>
       <c r="E40" s="16"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="97">
+      <c r="G40" s="96">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="147" t="s">
+      <c r="A41" s="150" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="148"/>
+      <c r="B41" s="151"/>
       <c r="C41" s="24"/>
       <c r="D41" s="23">
-        <f>D34+D35+D36+D37+D38+D39+D40</f>
+        <f>D35+D37+D38+D36</f>
         <v>0</v>
       </c>
       <c r="E41" s="23">
@@ -3084,7 +3090,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G41" s="98">
+      <c r="G41" s="97">
         <v>20</v>
       </c>
     </row>
@@ -3095,24 +3101,24 @@
       <c r="D42" s="20"/>
       <c r="E42" s="20"/>
       <c r="F42" s="20"/>
-      <c r="G42" s="106"/>
+      <c r="G42" s="105"/>
     </row>
     <row r="43" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="86" t="s">
+      <c r="A43" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="87"/>
-      <c r="C43" s="87"/>
-      <c r="D43" s="87"/>
-      <c r="E43" s="87"/>
-      <c r="F43" s="87"/>
-      <c r="G43" s="107"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="86"/>
+      <c r="E43" s="86"/>
+      <c r="F43" s="86"/>
+      <c r="G43" s="106"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="149" t="s">
+      <c r="A44" s="152" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="150"/>
+      <c r="B44" s="153"/>
       <c r="C44" s="19">
         <v>2</v>
       </c>
@@ -3128,15 +3134,15 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G44" s="92">
+      <c r="G44" s="91">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="151" t="s">
+      <c r="A45" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="152"/>
+      <c r="B45" s="155"/>
       <c r="C45" s="17">
         <f>C44</f>
         <v>2</v>
@@ -3144,15 +3150,15 @@
       <c r="D45" s="16"/>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
-      <c r="G45" s="99">
+      <c r="G45" s="98">
         <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="153" t="s">
+      <c r="A46" s="156" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="154"/>
+      <c r="B46" s="157"/>
       <c r="C46" s="15"/>
       <c r="D46" s="14">
         <f>D44-D45</f>
@@ -3160,7 +3166,7 @@
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
-      <c r="G46" s="91">
+      <c r="G46" s="90">
         <v>23</v>
       </c>
     </row>
@@ -3171,55 +3177,55 @@
       <c r="D47" s="11"/>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
-      <c r="G47" s="108"/>
+      <c r="G47" s="107"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="138" t="s">
+      <c r="A48" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="139"/>
-      <c r="C48" s="139"/>
-      <c r="D48" s="139"/>
-      <c r="E48" s="139"/>
-      <c r="F48" s="139"/>
-      <c r="G48" s="140"/>
+      <c r="B48" s="142"/>
+      <c r="C48" s="142"/>
+      <c r="D48" s="142"/>
+      <c r="E48" s="142"/>
+      <c r="F48" s="142"/>
+      <c r="G48" s="143"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="115" t="s">
+      <c r="A49" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="118" t="s">
+      <c r="B49" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="120"/>
-      <c r="D49" s="129" t="s">
+      <c r="C49" s="116"/>
+      <c r="D49" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="131"/>
-      <c r="F49" s="130" t="s">
+      <c r="E49" s="134"/>
+      <c r="F49" s="133" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="131"/>
+      <c r="G49" s="134"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="116"/>
-      <c r="B50" s="133" t="s">
+      <c r="A50" s="125"/>
+      <c r="B50" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="135"/>
-      <c r="D50" s="133"/>
-      <c r="E50" s="135"/>
-      <c r="F50" s="134"/>
-      <c r="G50" s="135"/>
+      <c r="C50" s="138"/>
+      <c r="D50" s="136"/>
+      <c r="E50" s="138"/>
+      <c r="F50" s="137"/>
+      <c r="G50" s="138"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="117"/>
-      <c r="B51" s="127"/>
-      <c r="C51" s="128"/>
-      <c r="D51" s="127"/>
-      <c r="E51" s="128"/>
-      <c r="F51" s="136"/>
-      <c r="G51" s="137"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="130"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="130"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="139"/>
+      <c r="G51" s="140"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" s="122" t="s">
@@ -3233,37 +3239,37 @@
       <c r="G52" s="124"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="115" t="s">
+      <c r="A53" s="120" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="129" t="s">
+      <c r="B53" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="130"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="130" t="s">
+      <c r="C53" s="133"/>
+      <c r="D53" s="134"/>
+      <c r="E53" s="133" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="130"/>
-      <c r="G53" s="131"/>
+      <c r="F53" s="133"/>
+      <c r="G53" s="134"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="116"/>
-      <c r="B54" s="133"/>
-      <c r="C54" s="134"/>
-      <c r="D54" s="135"/>
-      <c r="E54" s="134"/>
-      <c r="F54" s="134"/>
-      <c r="G54" s="135"/>
+      <c r="A54" s="125"/>
+      <c r="B54" s="136"/>
+      <c r="C54" s="137"/>
+      <c r="D54" s="138"/>
+      <c r="E54" s="137"/>
+      <c r="F54" s="137"/>
+      <c r="G54" s="138"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="117"/>
-      <c r="B55" s="127"/>
-      <c r="C55" s="132"/>
-      <c r="D55" s="128"/>
-      <c r="E55" s="136"/>
-      <c r="F55" s="136"/>
-      <c r="G55" s="137"/>
+      <c r="A55" s="121"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="135"/>
+      <c r="D55" s="131"/>
+      <c r="E55" s="139"/>
+      <c r="F55" s="139"/>
+      <c r="G55" s="140"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A56" s="122" t="s">
@@ -3277,61 +3283,61 @@
       <c r="G56" s="124"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="115" t="s">
+      <c r="A57" s="120" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="198" t="s">
+      <c r="B57" s="126" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="199"/>
-      <c r="D57" s="198" t="s">
+      <c r="C57" s="127"/>
+      <c r="D57" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="199"/>
-      <c r="F57" s="198" t="s">
+      <c r="E57" s="127"/>
+      <c r="F57" s="126" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="199"/>
+      <c r="G57" s="127"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="116"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="10"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="125"/>
-      <c r="E58" s="126"/>
+      <c r="D58" s="128"/>
+      <c r="E58" s="129"/>
       <c r="F58" s="9"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="116"/>
-      <c r="B59" s="127" t="s">
+      <c r="A59" s="125"/>
+      <c r="B59" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="128"/>
-      <c r="D59" s="113" t="s">
+      <c r="C59" s="131"/>
+      <c r="D59" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="121"/>
-      <c r="F59" s="114" t="s">
+      <c r="E59" s="119"/>
+      <c r="F59" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="121"/>
+      <c r="G59" s="119"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="116"/>
-      <c r="B60" s="129" t="s">
+      <c r="A60" s="125"/>
+      <c r="B60" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="130"/>
-      <c r="D60" s="131"/>
-      <c r="E60" s="118" t="s">
+      <c r="C60" s="133"/>
+      <c r="D60" s="134"/>
+      <c r="E60" s="114" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="119"/>
-      <c r="G60" s="120"/>
+      <c r="F60" s="115"/>
+      <c r="G60" s="116"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="116"/>
+      <c r="A61" s="125"/>
       <c r="B61" s="7"/>
       <c r="C61" s="6"/>
       <c r="D61" s="3"/>
@@ -3340,71 +3346,71 @@
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="117"/>
-      <c r="B62" s="127" t="s">
+      <c r="A62" s="121"/>
+      <c r="B62" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="132"/>
-      <c r="D62" s="128"/>
-      <c r="E62" s="113" t="s">
+      <c r="C62" s="135"/>
+      <c r="D62" s="131"/>
+      <c r="E62" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="114"/>
-      <c r="G62" s="121"/>
+      <c r="F62" s="118"/>
+      <c r="G62" s="119"/>
     </row>
     <row r="63" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="115" t="s">
+      <c r="A63" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="118" t="s">
+      <c r="B63" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="119"/>
-      <c r="D63" s="120"/>
-      <c r="E63" s="118" t="s">
+      <c r="C63" s="115"/>
+      <c r="D63" s="116"/>
+      <c r="E63" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="119"/>
-      <c r="G63" s="120"/>
+      <c r="F63" s="115"/>
+      <c r="G63" s="116"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="117"/>
-      <c r="B64" s="113" t="s">
+      <c r="A64" s="121"/>
+      <c r="B64" s="117" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="114"/>
-      <c r="D64" s="121"/>
-      <c r="E64" s="113" t="s">
+      <c r="C64" s="118"/>
+      <c r="D64" s="119"/>
+      <c r="E64" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="F64" s="114"/>
-      <c r="G64" s="121"/>
+      <c r="F64" s="118"/>
+      <c r="G64" s="119"/>
     </row>
     <row r="65" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="196"/>
-      <c r="B65" s="196"/>
-      <c r="C65" s="196"/>
-      <c r="D65" s="196"/>
-      <c r="E65" s="196"/>
-      <c r="F65" s="196"/>
-      <c r="G65" s="196"/>
+      <c r="A65" s="113"/>
+      <c r="B65" s="113"/>
+      <c r="C65" s="113"/>
+      <c r="D65" s="113"/>
+      <c r="E65" s="113"/>
+      <c r="F65" s="113"/>
+      <c r="G65" s="113"/>
     </row>
     <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="197" t="str">
+      <c r="A66" s="181" t="str">
         <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
-        <v>Generated by Autodesk Construction Cloud on: 03 March 2025</v>
-      </c>
-      <c r="B66" s="197"/>
-      <c r="C66" s="197"/>
-      <c r="D66" s="197"/>
-      <c r="E66" s="197"/>
-      <c r="F66" s="197"/>
+        <v>Generated by Autodesk Construction Cloud on: 04 March 2025</v>
+      </c>
+      <c r="B66" s="181"/>
+      <c r="C66" s="181"/>
+      <c r="D66" s="181"/>
+      <c r="E66" s="181"/>
+      <c r="F66" s="181"/>
     </row>
     <row r="70" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D70"/>
     </row>
     <row r="71" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="E71" s="195"/>
+      <c r="E71" s="112"/>
     </row>
   </sheetData>
   <mergeCells count="83">
@@ -3421,15 +3427,15 @@
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="D2:F3"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A24:B24"/>
@@ -3485,12 +3491,12 @@
     <mergeCell ref="E60:G60"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A65:G65"/>
     <mergeCell ref="B63:D63"/>
     <mergeCell ref="E63:G63"/>
     <mergeCell ref="E64:G64"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:G65"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to set last_date to a fixed value and modify ExcelModifier.py to remove font setting for modified cells
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623BE7A2-05F7-4D87-A105-AE9652EE2632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED77E43-CF22-4627-BAD6-471A922A739A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
   <sheets>
     <sheet name="IPC" sheetId="2" r:id="rId1"/>
@@ -568,9 +568,6 @@
     <t>تاريخ بداية الأعمال :</t>
   </si>
   <si>
-    <t>عن الأعمال حتى:</t>
-  </si>
-  <si>
     <t xml:space="preserve">المقــــاول </t>
   </si>
   <si>
@@ -605,6 +602,9 @@
   </si>
   <si>
     <t>تاريخ المستخلص:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> الأعمال حتى تاريخ:</t>
   </si>
 </sst>
 </file>
@@ -1787,98 +1787,116 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="65" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1886,60 +1904,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1950,12 +1914,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1967,86 +1925,128 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="65" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2533,7 +2533,7 @@
   <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2556,51 +2556,51 @@
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="81" t="s">
-        <v>65</v>
-      </c>
-      <c r="B1" s="178" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="178"/>
-      <c r="D1" s="179"/>
-      <c r="E1" s="179"/>
+      <c r="B1" s="139" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="139"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="81" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="178" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="180"/>
-      <c r="E2" s="180"/>
-      <c r="F2" s="180"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
       <c r="G2" s="111"/>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="178" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="178"/>
-      <c r="D3" s="180"/>
-      <c r="E3" s="180"/>
-      <c r="F3" s="180"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
       <c r="G3"/>
     </row>
     <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="81" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="177" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="177"/>
+      <c r="C4" s="138"/>
       <c r="E4" s="109" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="110"/>
       <c r="G4" s="110"/>
@@ -2616,34 +2616,34 @@
     </row>
     <row r="6" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="77"/>
-      <c r="B6" s="196" t="s">
-        <v>72</v>
+      <c r="B6" s="113" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="76"/>
       <c r="D6" s="76"/>
-      <c r="E6" s="196" t="s">
-        <v>60</v>
+      <c r="E6" s="113" t="s">
+        <v>72</v>
       </c>
       <c r="F6" s="75"/>
       <c r="G6" s="101"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="197" t="s">
+      <c r="A7" s="117" t="s">
         <v>59</v>
       </c>
-      <c r="B7" s="198"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="74"/>
-      <c r="D7" s="199" t="s">
+      <c r="D7" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="198"/>
-      <c r="F7" s="182"/>
-      <c r="G7" s="183"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="121"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="184"/>
-      <c r="B8" s="185"/>
-      <c r="C8" s="186"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="73" t="s">
         <v>57</v>
       </c>
@@ -2656,21 +2656,21 @@
       <c r="G8" s="102"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="187" t="s">
+      <c r="A9" s="125" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="188"/>
-      <c r="C9" s="189"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="127"/>
       <c r="D9" s="69"/>
       <c r="E9" s="70"/>
       <c r="F9" s="69"/>
       <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="190" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="191"/>
+      <c r="A10" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="129"/>
       <c r="C10" s="68"/>
       <c r="D10" s="108"/>
       <c r="E10" s="27"/>
@@ -2678,10 +2678,10 @@
       <c r="G10" s="64"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="173" t="s">
+      <c r="A11" s="130" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="174"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="66"/>
       <c r="D11" s="27"/>
       <c r="E11" s="27"/>
@@ -2689,10 +2689,10 @@
       <c r="G11" s="64"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="173" t="s">
+      <c r="A12" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="174"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="66"/>
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
@@ -2700,10 +2700,10 @@
       <c r="G12" s="64"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="173" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="174"/>
+      <c r="A13" s="130" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="131"/>
       <c r="C13" s="63"/>
       <c r="D13" s="27"/>
       <c r="E13" s="27"/>
@@ -2711,10 +2711,10 @@
       <c r="G13" s="64"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="173" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" s="174"/>
+      <c r="A14" s="130" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="131"/>
       <c r="C14" s="65"/>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
@@ -2722,10 +2722,10 @@
       <c r="G14" s="64"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="173" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="174"/>
+      <c r="A15" s="130" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="131"/>
       <c r="C15" s="65"/>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
@@ -2733,10 +2733,10 @@
       <c r="G15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="158" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="159"/>
+      <c r="A16" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="116"/>
       <c r="C16" s="62" t="s">
         <v>39</v>
       </c>
@@ -2746,10 +2746,10 @@
       <c r="G16" s="61"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="168" t="s">
+      <c r="A17" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="169"/>
+      <c r="B17" s="133"/>
       <c r="C17" s="60"/>
       <c r="D17" s="59">
         <f>D10+D13+D14+D15+D16</f>
@@ -2775,21 +2775,21 @@
       <c r="G18" s="103"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="192" t="s">
+      <c r="A19" s="134" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="193"/>
-      <c r="C19" s="193"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="135"/>
       <c r="D19" s="54"/>
       <c r="E19" s="55"/>
       <c r="F19" s="54"/>
       <c r="G19" s="87"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="194" t="s">
+      <c r="A20" s="136" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="195"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="53"/>
       <c r="D20" s="27"/>
       <c r="E20" s="27"/>
@@ -2799,10 +2799,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="175" t="s">
+      <c r="A21" s="142" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="176"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="52"/>
       <c r="D21" s="27"/>
       <c r="E21" s="51"/>
@@ -2812,10 +2812,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="173" t="s">
+      <c r="A22" s="130" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="174"/>
+      <c r="B22" s="131"/>
       <c r="C22" s="82"/>
       <c r="D22" s="27"/>
       <c r="E22" s="51"/>
@@ -2825,10 +2825,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="173" t="s">
+      <c r="A23" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="174"/>
+      <c r="B23" s="131"/>
       <c r="C23" s="50"/>
       <c r="D23" s="27"/>
       <c r="E23" s="27"/>
@@ -2838,10 +2838,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="173" t="s">
+      <c r="A24" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="174"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="50"/>
       <c r="D24" s="27"/>
       <c r="E24" s="27"/>
@@ -2851,10 +2851,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="173" t="s">
+      <c r="A25" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="174"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="99"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
@@ -2864,10 +2864,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="158" t="s">
+      <c r="A26" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="159"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="49"/>
       <c r="D26" s="48"/>
       <c r="E26" s="48"/>
@@ -2877,10 +2877,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="160" t="s">
+      <c r="A27" s="144" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="161"/>
+      <c r="B27" s="145"/>
       <c r="C27" s="36"/>
       <c r="D27" s="22">
         <f>D20+D24+D25+D26</f>
@@ -2899,10 +2899,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="152" t="s">
+      <c r="A28" s="146" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="153"/>
+      <c r="B28" s="147"/>
       <c r="C28" s="47"/>
       <c r="D28" s="46"/>
       <c r="E28" s="45"/>
@@ -2912,10 +2912,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="162" t="s">
+      <c r="A29" s="148" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="163"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="44"/>
       <c r="D29" s="43"/>
       <c r="E29" s="42"/>
@@ -2925,10 +2925,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="164" t="s">
+      <c r="A30" s="152" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="165"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="41"/>
       <c r="D30" s="40"/>
       <c r="E30" s="39"/>
@@ -2938,10 +2938,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="166" t="s">
+      <c r="A31" s="154" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="167"/>
+      <c r="B31" s="155"/>
       <c r="C31" s="38" t="s">
         <v>39</v>
       </c>
@@ -2953,10 +2953,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A32" s="168" t="s">
+      <c r="A32" s="132" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="169"/>
+      <c r="B32" s="133"/>
       <c r="C32" s="36"/>
       <c r="D32" s="22">
         <f>D27+D28+D29+D30+D31</f>
@@ -2984,21 +2984,21 @@
       <c r="G33" s="104"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="170" t="s">
+      <c r="A34" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="171"/>
-      <c r="C34" s="172"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="158"/>
       <c r="D34" s="33"/>
       <c r="E34" s="32"/>
       <c r="F34" s="31"/>
       <c r="G34" s="95"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="144" t="s">
+      <c r="A35" s="150" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="145"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="30"/>
       <c r="D35" s="28"/>
       <c r="E35" s="27"/>
@@ -3008,10 +3008,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="144" t="s">
+      <c r="A36" s="150" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="145"/>
+      <c r="B36" s="151"/>
       <c r="C36" s="30"/>
       <c r="D36" s="28"/>
       <c r="E36" s="27"/>
@@ -3021,10 +3021,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="144" t="s">
+      <c r="A37" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="145"/>
+      <c r="B37" s="151"/>
       <c r="C37" s="30"/>
       <c r="D37" s="28"/>
       <c r="E37" s="27"/>
@@ -3034,10 +3034,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="146" t="s">
+      <c r="A38" s="162" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="147"/>
+      <c r="B38" s="163"/>
       <c r="C38" s="29"/>
       <c r="D38" s="28"/>
       <c r="E38" s="27"/>
@@ -3047,10 +3047,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="146" t="s">
+      <c r="A39" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="B39" s="147"/>
+      <c r="B39" s="163"/>
       <c r="C39" s="29"/>
       <c r="D39" s="28"/>
       <c r="E39" s="27"/>
@@ -3060,10 +3060,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="148" t="s">
+      <c r="A40" s="164" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="149"/>
+      <c r="B40" s="165"/>
       <c r="C40" s="26"/>
       <c r="D40" s="25"/>
       <c r="E40" s="16"/>
@@ -3073,10 +3073,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="150" t="s">
+      <c r="A41" s="166" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="151"/>
+      <c r="B41" s="167"/>
       <c r="C41" s="24"/>
       <c r="D41" s="23">
         <f>D35+D37+D38+D36</f>
@@ -3115,10 +3115,10 @@
       <c r="G43" s="106"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="152" t="s">
+      <c r="A44" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="B44" s="153"/>
+      <c r="B44" s="147"/>
       <c r="C44" s="19">
         <v>2</v>
       </c>
@@ -3139,10 +3139,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="154" t="s">
+      <c r="A45" s="168" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="155"/>
+      <c r="B45" s="169"/>
       <c r="C45" s="17">
         <f>C44</f>
         <v>2</v>
@@ -3155,10 +3155,10 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A46" s="156" t="s">
+      <c r="A46" s="170" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="157"/>
+      <c r="B46" s="171"/>
       <c r="C46" s="15"/>
       <c r="D46" s="14">
         <f>D44-D45</f>
@@ -3180,164 +3180,164 @@
       <c r="G47" s="107"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="141" t="s">
+      <c r="A48" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="142"/>
-      <c r="C48" s="142"/>
-      <c r="D48" s="142"/>
-      <c r="E48" s="142"/>
-      <c r="F48" s="142"/>
-      <c r="G48" s="143"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="161"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="120" t="s">
+      <c r="A49" s="172" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="116"/>
-      <c r="D49" s="132" t="s">
+      <c r="C49" s="176"/>
+      <c r="D49" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="134"/>
-      <c r="F49" s="133" t="s">
+      <c r="E49" s="178"/>
+      <c r="F49" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="134"/>
+      <c r="G49" s="178"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="125"/>
-      <c r="B50" s="136" t="s">
+      <c r="A50" s="173"/>
+      <c r="B50" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="138"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="138"/>
-      <c r="F50" s="137"/>
-      <c r="G50" s="138"/>
+      <c r="C50" s="181"/>
+      <c r="D50" s="180"/>
+      <c r="E50" s="181"/>
+      <c r="F50" s="182"/>
+      <c r="G50" s="181"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="121"/>
-      <c r="B51" s="130"/>
-      <c r="C51" s="131"/>
-      <c r="D51" s="130"/>
-      <c r="E51" s="131"/>
-      <c r="F51" s="139"/>
-      <c r="G51" s="140"/>
+      <c r="A51" s="174"/>
+      <c r="B51" s="183"/>
+      <c r="C51" s="184"/>
+      <c r="D51" s="183"/>
+      <c r="E51" s="184"/>
+      <c r="F51" s="185"/>
+      <c r="G51" s="186"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A52" s="122" t="s">
+      <c r="A52" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="123"/>
-      <c r="C52" s="123"/>
-      <c r="D52" s="123"/>
-      <c r="E52" s="123"/>
-      <c r="F52" s="123"/>
-      <c r="G52" s="124"/>
+      <c r="B52" s="188"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="188"/>
+      <c r="E52" s="188"/>
+      <c r="F52" s="188"/>
+      <c r="G52" s="189"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A53" s="120" t="s">
+      <c r="A53" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="132" t="s">
+      <c r="B53" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="133"/>
-      <c r="D53" s="134"/>
-      <c r="E53" s="133" t="s">
+      <c r="C53" s="179"/>
+      <c r="D53" s="178"/>
+      <c r="E53" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="133"/>
-      <c r="G53" s="134"/>
+      <c r="F53" s="179"/>
+      <c r="G53" s="178"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A54" s="125"/>
-      <c r="B54" s="136"/>
-      <c r="C54" s="137"/>
-      <c r="D54" s="138"/>
-      <c r="E54" s="137"/>
-      <c r="F54" s="137"/>
-      <c r="G54" s="138"/>
+      <c r="A54" s="173"/>
+      <c r="B54" s="180"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="181"/>
+      <c r="E54" s="182"/>
+      <c r="F54" s="182"/>
+      <c r="G54" s="181"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="121"/>
-      <c r="B55" s="130"/>
-      <c r="C55" s="135"/>
-      <c r="D55" s="131"/>
-      <c r="E55" s="139"/>
-      <c r="F55" s="139"/>
-      <c r="G55" s="140"/>
+      <c r="A55" s="174"/>
+      <c r="B55" s="183"/>
+      <c r="C55" s="190"/>
+      <c r="D55" s="184"/>
+      <c r="E55" s="185"/>
+      <c r="F55" s="185"/>
+      <c r="G55" s="186"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="122" t="s">
+      <c r="A56" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="123"/>
-      <c r="C56" s="123"/>
-      <c r="D56" s="123"/>
-      <c r="E56" s="123"/>
-      <c r="F56" s="123"/>
-      <c r="G56" s="124"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="188"/>
+      <c r="D56" s="188"/>
+      <c r="E56" s="188"/>
+      <c r="F56" s="188"/>
+      <c r="G56" s="189"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="120" t="s">
+      <c r="A57" s="172" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="126" t="s">
+      <c r="B57" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="127"/>
-      <c r="D57" s="126" t="s">
+      <c r="C57" s="192"/>
+      <c r="D57" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="127"/>
-      <c r="F57" s="126" t="s">
+      <c r="E57" s="192"/>
+      <c r="F57" s="191" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="127"/>
+      <c r="G57" s="192"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="125"/>
+      <c r="A58" s="173"/>
       <c r="B58" s="10"/>
       <c r="C58" s="3"/>
-      <c r="D58" s="128"/>
-      <c r="E58" s="129"/>
+      <c r="D58" s="193"/>
+      <c r="E58" s="194"/>
       <c r="F58" s="9"/>
       <c r="G58" s="8"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="125"/>
-      <c r="B59" s="130" t="s">
+      <c r="A59" s="173"/>
+      <c r="B59" s="183" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="131"/>
-      <c r="D59" s="117" t="s">
+      <c r="C59" s="184"/>
+      <c r="D59" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="119"/>
-      <c r="F59" s="118" t="s">
+      <c r="E59" s="196"/>
+      <c r="F59" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="119"/>
+      <c r="G59" s="196"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A60" s="125"/>
-      <c r="B60" s="132" t="s">
+      <c r="A60" s="173"/>
+      <c r="B60" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="133"/>
-      <c r="D60" s="134"/>
-      <c r="E60" s="114" t="s">
+      <c r="C60" s="179"/>
+      <c r="D60" s="178"/>
+      <c r="E60" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="115"/>
-      <c r="G60" s="116"/>
+      <c r="F60" s="198"/>
+      <c r="G60" s="176"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A61" s="125"/>
+      <c r="A61" s="173"/>
       <c r="B61" s="7"/>
       <c r="C61" s="6"/>
       <c r="D61" s="3"/>
@@ -3346,65 +3346,65 @@
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="121"/>
-      <c r="B62" s="130" t="s">
+      <c r="A62" s="174"/>
+      <c r="B62" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="135"/>
-      <c r="D62" s="131"/>
-      <c r="E62" s="117" t="s">
+      <c r="C62" s="190"/>
+      <c r="D62" s="184"/>
+      <c r="E62" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="118"/>
-      <c r="G62" s="119"/>
+      <c r="F62" s="197"/>
+      <c r="G62" s="196"/>
     </row>
     <row r="63" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="120" t="s">
+      <c r="A63" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="114" t="s">
+      <c r="B63" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="115"/>
-      <c r="D63" s="116"/>
-      <c r="E63" s="114" t="s">
+      <c r="C63" s="198"/>
+      <c r="D63" s="176"/>
+      <c r="E63" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="115"/>
-      <c r="G63" s="116"/>
+      <c r="F63" s="198"/>
+      <c r="G63" s="176"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="121"/>
-      <c r="B64" s="117" t="s">
+      <c r="A64" s="174"/>
+      <c r="B64" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="118"/>
-      <c r="D64" s="119"/>
-      <c r="E64" s="117" t="s">
+      <c r="C64" s="197"/>
+      <c r="D64" s="196"/>
+      <c r="E64" s="195" t="s">
         <v>0</v>
       </c>
-      <c r="F64" s="118"/>
-      <c r="G64" s="119"/>
+      <c r="F64" s="197"/>
+      <c r="G64" s="196"/>
     </row>
     <row r="65" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="113"/>
-      <c r="B65" s="113"/>
-      <c r="C65" s="113"/>
-      <c r="D65" s="113"/>
-      <c r="E65" s="113"/>
-      <c r="F65" s="113"/>
-      <c r="G65" s="113"/>
+      <c r="A65" s="199"/>
+      <c r="B65" s="199"/>
+      <c r="C65" s="199"/>
+      <c r="D65" s="199"/>
+      <c r="E65" s="199"/>
+      <c r="F65" s="199"/>
+      <c r="G65" s="199"/>
     </row>
     <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="181" t="str">
+      <c r="A66" s="114" t="str">
         <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
         <v>Generated by Autodesk Construction Cloud on: 04 March 2025</v>
       </c>
-      <c r="B66" s="181"/>
-      <c r="C66" s="181"/>
-      <c r="D66" s="181"/>
-      <c r="E66" s="181"/>
-      <c r="F66" s="181"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="114"/>
+      <c r="F66" s="114"/>
     </row>
     <row r="70" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
       <c r="D70"/>
@@ -3414,6 +3414,73 @@
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:F3"/>
     <mergeCell ref="A66:F66"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
@@ -3430,73 +3497,6 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: update cost.py to set locale for date formatting and modify last_date handling
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED77E43-CF22-4627-BAD6-471A922A739A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B64E95-9721-4B62-9C9D-BE7286450BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -2532,8 +2532,8 @@
   </sheetPr>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="B1" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="72" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2624,7 +2624,10 @@
       <c r="E6" s="113" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="75"/>
+      <c r="F6" s="75" t="str">
+        <f ca="1">TEXT(TODAY(), "[$-ar-SA]dd mmmm yyyy")</f>
+        <v>04 مارس 2025</v>
+      </c>
       <c r="G6" s="101"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
fix: update cost.py to change cell reference for first_date from C7 to C6
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D2A1C7-ED33-4CC9-AFE9-2C4150ED3DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1AA5B-914A-4495-B6E6-19CD4BBA9B7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -2005,11 +2005,11 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="65" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="71" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2495,8 +2495,8 @@
   </sheetPr>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="B4" zoomScale="78" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A50" zoomScale="78" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2517,7 +2517,7 @@
     <col min="22" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="5" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
@@ -2527,10 +2527,8 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
@@ -2543,7 +2541,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
@@ -2556,7 +2554,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
@@ -2564,14 +2562,13 @@
         <v>25</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="4"/>
       <c r="E4" s="10" t="s">
         <v>69</v>
       </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A5" s="12"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
@@ -2580,7 +2577,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>70</v>
@@ -2596,7 +2593,7 @@
       </c>
       <c r="G6" s="20"/>
     </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="21" t="s">
         <v>58</v>
       </c>
@@ -2609,7 +2606,7 @@
       <c r="F7" s="25"/>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="27"/>
       <c r="B8" s="28"/>
       <c r="C8" s="29"/>
@@ -2624,7 +2621,7 @@
       </c>
       <c r="G8" s="33"/>
     </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="34" t="s">
         <v>53</v>
       </c>
@@ -2635,7 +2632,7 @@
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
     </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="39" t="s">
         <v>64</v>
       </c>
@@ -2646,7 +2643,7 @@
       <c r="F10" s="44"/>
       <c r="G10" s="45"/>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="46" t="s">
         <v>48</v>
       </c>
@@ -2657,7 +2654,7 @@
       <c r="F11" s="43"/>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="46" t="s">
         <v>52</v>
       </c>
@@ -2668,7 +2665,7 @@
       <c r="F12" s="8"/>
       <c r="G12" s="45"/>
     </row>
-    <row r="13" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="46" t="s">
         <v>66</v>
       </c>
@@ -2679,7 +2676,7 @@
       <c r="F13" s="43"/>
       <c r="G13" s="45"/>
     </row>
-    <row r="14" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="46" t="s">
         <v>67</v>
       </c>
@@ -2690,7 +2687,7 @@
       <c r="F14" s="51"/>
       <c r="G14" s="45"/>
     </row>
-    <row r="15" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="46" t="s">
         <v>68</v>
       </c>
@@ -2701,7 +2698,7 @@
       <c r="F15" s="51"/>
       <c r="G15" s="52"/>
     </row>
-    <row r="16" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A16" s="53" t="s">
         <v>65</v>
       </c>
@@ -2714,7 +2711,7 @@
       <c r="F16" s="56"/>
       <c r="G16" s="52"/>
     </row>
-    <row r="17" spans="1:7" s="5" customFormat="1" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="57" t="s">
         <v>51</v>
       </c>
@@ -2734,7 +2731,7 @@
       </c>
       <c r="G17" s="61"/>
     </row>
-    <row r="18" spans="1:7" s="5" customFormat="1" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="62"/>
       <c r="B18" s="63"/>
       <c r="C18" s="63"/>
@@ -2743,7 +2740,7 @@
       <c r="F18" s="63"/>
       <c r="G18" s="64"/>
     </row>
-    <row r="19" spans="1:7" s="5" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="65" t="s">
         <v>50</v>
       </c>
@@ -2754,7 +2751,7 @@
       <c r="F19" s="67"/>
       <c r="G19" s="69"/>
     </row>
-    <row r="20" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="70" t="s">
         <v>49</v>
       </c>
@@ -2767,7 +2764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="74" t="s">
         <v>48</v>
       </c>
@@ -2780,7 +2777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="46" t="s">
         <v>52</v>
       </c>
@@ -2793,7 +2790,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="46" t="s">
         <v>47</v>
       </c>
@@ -2806,7 +2803,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="46" t="s">
         <v>45</v>
       </c>
@@ -2819,7 +2816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="46" t="s">
         <v>46</v>
       </c>
@@ -2832,7 +2829,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="53" t="s">
         <v>44</v>
       </c>
@@ -2845,7 +2842,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="5" customFormat="1" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="84" t="s">
         <v>43</v>
       </c>
@@ -2867,7 +2864,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="89" t="s">
         <v>42</v>
       </c>
@@ -2880,7 +2877,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="95" t="s">
         <v>41</v>
       </c>
@@ -2893,7 +2890,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A30" s="101" t="s">
         <v>40</v>
       </c>
@@ -2906,7 +2903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A31" s="107" t="s">
         <v>39</v>
       </c>
@@ -2921,7 +2918,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="5" customFormat="1" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A32" s="57" t="s">
         <v>37</v>
       </c>
@@ -2943,7 +2940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="5" customFormat="1" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A33" s="114"/>
       <c r="B33" s="115"/>
       <c r="C33" s="115"/>
@@ -2952,7 +2949,7 @@
       <c r="F33" s="115"/>
       <c r="G33" s="116"/>
     </row>
-    <row r="34" spans="1:7" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="117" t="s">
         <v>36</v>
       </c>
@@ -2963,7 +2960,7 @@
       <c r="F34" s="122"/>
       <c r="G34" s="123"/>
     </row>
-    <row r="35" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="124" t="s">
         <v>35</v>
       </c>
@@ -2976,7 +2973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="124" t="s">
         <v>34</v>
       </c>
@@ -2989,7 +2986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="124" t="s">
         <v>33</v>
       </c>
@@ -3002,7 +2999,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="128" t="s">
         <v>32</v>
       </c>
@@ -3015,7 +3012,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="128" t="s">
         <v>31</v>
       </c>
@@ -3028,7 +3025,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="5" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A40" s="131" t="s">
         <v>30</v>
       </c>
@@ -3041,7 +3038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:7" s="5" customFormat="1" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A41" s="135" t="s">
         <v>29</v>
       </c>
@@ -3063,7 +3060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:7" s="5" customFormat="1" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A42" s="140"/>
       <c r="B42" s="141"/>
       <c r="C42" s="141"/>
@@ -3072,7 +3069,7 @@
       <c r="F42" s="141"/>
       <c r="G42" s="116"/>
     </row>
-    <row r="43" spans="1:7" s="5" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A43" s="142" t="s">
         <v>28</v>
       </c>
@@ -3083,7 +3080,7 @@
       <c r="F43" s="143"/>
       <c r="G43" s="144"/>
     </row>
-    <row r="44" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="89" t="s">
         <v>27</v>
       </c>
@@ -3107,7 +3104,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="147" t="s">
         <v>72</v>
       </c>
@@ -3123,7 +3120,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:7" s="5" customFormat="1" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A46" s="151" t="s">
         <v>26</v>
       </c>
@@ -3139,7 +3136,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="5" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A47" s="155"/>
       <c r="B47" s="156"/>
       <c r="C47" s="157"/>
@@ -3148,7 +3145,7 @@
       <c r="F47" s="157"/>
       <c r="G47" s="158"/>
     </row>
-    <row r="48" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="159" t="s">
         <v>25</v>
       </c>
@@ -3159,7 +3156,7 @@
       <c r="F48" s="160"/>
       <c r="G48" s="161"/>
     </row>
-    <row r="49" spans="1:7" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="162" t="s">
         <v>24</v>
       </c>
@@ -3176,7 +3173,7 @@
       </c>
       <c r="G49" s="166"/>
     </row>
-    <row r="50" spans="1:7" s="5" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="168"/>
       <c r="B50" s="169" t="s">
         <v>20</v>
@@ -3187,7 +3184,7 @@
       <c r="F50" s="171"/>
       <c r="G50" s="170"/>
     </row>
-    <row r="51" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A51" s="172"/>
       <c r="B51" s="173"/>
       <c r="C51" s="174"/>
@@ -3196,7 +3193,7 @@
       <c r="F51" s="175"/>
       <c r="G51" s="176"/>
     </row>
-    <row r="52" spans="1:7" s="5" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A52" s="177" t="s">
         <v>19</v>
       </c>
@@ -3207,7 +3204,7 @@
       <c r="F52" s="178"/>
       <c r="G52" s="179"/>
     </row>
-    <row r="53" spans="1:7" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="162" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3219,7 @@
       <c r="F53" s="167"/>
       <c r="G53" s="166"/>
     </row>
-    <row r="54" spans="1:7" s="5" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="168"/>
       <c r="B54" s="169"/>
       <c r="C54" s="171"/>
@@ -3231,7 +3228,7 @@
       <c r="F54" s="171"/>
       <c r="G54" s="170"/>
     </row>
-    <row r="55" spans="1:7" s="5" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A55" s="172"/>
       <c r="B55" s="173"/>
       <c r="C55" s="180"/>
@@ -3240,7 +3237,7 @@
       <c r="F55" s="175"/>
       <c r="G55" s="176"/>
     </row>
-    <row r="56" spans="1:7" s="5" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A56" s="177" t="s">
         <v>15</v>
       </c>
@@ -3251,7 +3248,7 @@
       <c r="F56" s="178"/>
       <c r="G56" s="179"/>
     </row>
-    <row r="57" spans="1:7" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="162" t="s">
         <v>14</v>
       </c>
@@ -3268,7 +3265,7 @@
       </c>
       <c r="G57" s="182"/>
     </row>
-    <row r="58" spans="1:7" s="5" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="168"/>
       <c r="B58" s="183"/>
       <c r="C58" s="184"/>
@@ -3277,7 +3274,7 @@
       <c r="F58" s="187"/>
       <c r="G58" s="188"/>
     </row>
-    <row r="59" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A59" s="168"/>
       <c r="B59" s="173" t="s">
         <v>10</v>
@@ -3292,7 +3289,7 @@
       </c>
       <c r="G59" s="190"/>
     </row>
-    <row r="60" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="168"/>
       <c r="B60" s="165" t="s">
         <v>3</v>
@@ -3305,7 +3302,7 @@
       <c r="F60" s="192"/>
       <c r="G60" s="164"/>
     </row>
-    <row r="61" spans="1:7" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="168"/>
       <c r="B61" s="193"/>
       <c r="C61" s="194"/>
@@ -3314,7 +3311,7 @@
       <c r="F61" s="196"/>
       <c r="G61" s="184"/>
     </row>
-    <row r="62" spans="1:7" s="5" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A62" s="172"/>
       <c r="B62" s="173" t="s">
         <v>6</v>
@@ -3327,7 +3324,7 @@
       <c r="F62" s="191"/>
       <c r="G62" s="190"/>
     </row>
-    <row r="63" spans="1:7" s="5" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="162" t="s">
         <v>4</v>
       </c>
@@ -3342,7 +3339,7 @@
       <c r="F63" s="192"/>
       <c r="G63" s="164"/>
     </row>
-    <row r="64" spans="1:7" s="5" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A64" s="172"/>
       <c r="B64" s="189" t="s">
         <v>1</v>
@@ -3355,7 +3352,7 @@
       <c r="F64" s="191"/>
       <c r="G64" s="190"/>
     </row>
-    <row r="65" spans="1:7" s="5" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="197"/>
       <c r="B65" s="197"/>
       <c r="C65" s="197"/>
@@ -3364,35 +3361,22 @@
       <c r="F65" s="197"/>
       <c r="G65" s="197"/>
     </row>
-    <row r="66" spans="1:7" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="198" t="str">
+    <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A66" s="199" t="str">
         <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
         <v>Generated by Autodesk Construction Cloud on: 04 March 2025</v>
       </c>
-      <c r="B66" s="198"/>
-      <c r="C66" s="198"/>
-      <c r="D66" s="198"/>
-      <c r="E66" s="198"/>
-      <c r="F66" s="198"/>
-      <c r="G66" s="4"/>
-    </row>
-    <row r="70" spans="1:7" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
+      <c r="B66" s="199"/>
+      <c r="C66" s="199"/>
+      <c r="D66" s="199"/>
+      <c r="E66" s="199"/>
+      <c r="F66" s="199"/>
+    </row>
+    <row r="70" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D70" s="8"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-    </row>
-    <row r="71" spans="1:7" s="5" customFormat="1" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="4"/>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="199"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
+    </row>
+    <row r="71" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E71" s="198"/>
     </row>
   </sheetData>
   <mergeCells count="83">

</xml_diff>

<commit_message>
fix: optimize payment items calculation in cost.py
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925C3EB4-3554-47E9-8BCB-0EB29E7C9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53001889-BC85-4BF3-B323-0FF7BF2FB258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -374,7 +374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>م/ محمد عاطف</t>
   </si>
@@ -605,6 +605,9 @@
       </rPr>
       <t>(TMG)</t>
     </r>
+  </si>
+  <si>
+    <t>شركة سكوير للمشروعات الهندسية</t>
   </si>
 </sst>
 </file>
@@ -1421,58 +1424,544 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="0" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="14" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="19" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="12" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="23" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="168" fontId="8" fillId="0" borderId="44" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+      <alignment horizontal="right" vertical="center" indent="75" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
@@ -1480,9 +1969,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="42" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="2"/>
     </xf>
@@ -1501,18 +1987,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
     </xf>
@@ -1522,89 +1996,11 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="14" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="32" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="11" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
@@ -1612,404 +2008,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="29" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="36" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="35" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="19" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="31" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="12" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="27" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="28" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="16" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="4" fontId="11" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="20" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="18" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="75" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2495,958 +2498,891 @@
   </sheetPr>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A50" zoomScale="78" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="F69" sqref="F69"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="58" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.1796875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="39.453125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="4" customWidth="1"/>
-    <col min="4" max="6" width="46.7265625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.81640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="22.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.7265625" style="5" customWidth="1"/>
-    <col min="10" max="10" width="22.54296875" style="5" customWidth="1"/>
-    <col min="11" max="14" width="21.453125" style="5" customWidth="1"/>
-    <col min="15" max="15" width="25.81640625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="25.1796875" style="5" customWidth="1"/>
-    <col min="17" max="17" width="23.453125" style="5" customWidth="1"/>
-    <col min="18" max="21" width="9.54296875" style="5" customWidth="1"/>
-    <col min="22" max="16384" width="9.1796875" style="5"/>
+    <col min="1" max="1" width="23.1796875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="46.7265625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="22.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.7265625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="22.54296875" style="3" customWidth="1"/>
+    <col min="11" max="14" width="21.453125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="25.81640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="25.1796875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="23.453125" style="3" customWidth="1"/>
+    <col min="18" max="21" width="9.54296875" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="179"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="8"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="178" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="E4" s="10" t="s">
+      <c r="C4" s="178"/>
+      <c r="E4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="17" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="19" t="str">
+      <c r="F6" s="15" t="str">
         <f ca="1">TEXT(TODAY(), "[$-ar-SA]dd mmmm yyyy")</f>
-        <v>04 مارس 2025</v>
-      </c>
-      <c r="G6" s="20"/>
+        <v>06 مارس 2025</v>
+      </c>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="183" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="24" t="s">
+      <c r="B7" s="184"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="185" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="E7" s="184"/>
+      <c r="F7" s="186"/>
+      <c r="G7" s="187"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="27"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="30" t="s">
+      <c r="A8" s="188"/>
+      <c r="B8" s="189"/>
+      <c r="C8" s="190"/>
+      <c r="D8" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="33"/>
+      <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="191" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="B9" s="192"/>
+      <c r="C9" s="193"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="194" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="45"/>
+      <c r="B10" s="195"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="174" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="48"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="45"/>
+      <c r="B11" s="175"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="174" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="45"/>
+      <c r="B12" s="175"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="174" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="45"/>
+      <c r="B13" s="175"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="46" t="s">
+      <c r="A14" s="174" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="45"/>
+      <c r="B14" s="175"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="46" t="s">
+      <c r="A15" s="174" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="47"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="52"/>
+      <c r="B15" s="175"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="53" t="s">
+      <c r="A16" s="159" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="55" t="s">
+      <c r="B16" s="160"/>
+      <c r="C16" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="52"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="57" t="s">
+      <c r="A17" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="58"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60">
+      <c r="B17" s="170"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="38">
         <f>D10+D13+D14+D15+D16</f>
         <v>0</v>
       </c>
-      <c r="E17" s="60">
+      <c r="E17" s="38">
         <f t="shared" ref="E17:F17" si="0">E16+E15+E14+E13+E12+E11+E10</f>
         <v>0</v>
       </c>
-      <c r="F17" s="60">
+      <c r="F17" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G17" s="61"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="62"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="196" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="69"/>
+      <c r="B19" s="197"/>
+      <c r="C19" s="197"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="198" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="43"/>
-      <c r="G20" s="73">
+      <c r="B20" s="199"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="47">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="74" t="s">
+      <c r="A21" s="176" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="77"/>
-      <c r="F21" s="77"/>
-      <c r="G21" s="78">
+      <c r="B21" s="177"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="50">
         <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="46" t="s">
+      <c r="A22" s="174" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="73">
+      <c r="B22" s="175"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
+      <c r="G22" s="47">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="174" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="78">
+      <c r="B23" s="175"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="50">
         <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="46" t="s">
+      <c r="A24" s="174" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="73">
+      <c r="B24" s="175"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="47">
         <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="174" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="47"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="78">
+      <c r="B25" s="175"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="50">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="159" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="83"/>
-      <c r="F26" s="83"/>
-      <c r="G26" s="78">
+      <c r="B26" s="160"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="50">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="84" t="s">
+      <c r="A27" s="161" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="85"/>
-      <c r="C27" s="86"/>
-      <c r="D27" s="87">
+      <c r="B27" s="162"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="56">
         <f>D20+D24+D25+D26</f>
         <v>0</v>
       </c>
-      <c r="E27" s="87">
+      <c r="E27" s="56">
         <f>E20+E21+E22+E23-E24+E25-E26</f>
         <v>0</v>
       </c>
-      <c r="F27" s="87">
+      <c r="F27" s="56">
         <f>F20+F21+F22+F23-F24+F25-F26</f>
         <v>0</v>
       </c>
-      <c r="G27" s="88">
+      <c r="G27" s="57">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="89" t="s">
+      <c r="A28" s="153" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="90"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="93"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="94">
+      <c r="B28" s="154"/>
+      <c r="C28" s="58"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="60"/>
+      <c r="G28" s="61">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="95" t="s">
+      <c r="A29" s="163" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="96"/>
-      <c r="C29" s="97"/>
-      <c r="D29" s="98"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="99"/>
-      <c r="G29" s="100">
+      <c r="B29" s="164"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="65">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="101" t="s">
+      <c r="A30" s="165" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="102"/>
-      <c r="C30" s="103"/>
-      <c r="D30" s="104"/>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="106">
+      <c r="B30" s="166"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="69">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="107" t="s">
+      <c r="A31" s="167" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="108"/>
-      <c r="C31" s="109" t="s">
+      <c r="B31" s="168"/>
+      <c r="C31" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="D31" s="110"/>
-      <c r="E31" s="111"/>
-      <c r="F31" s="112"/>
-      <c r="G31" s="113">
+      <c r="D31" s="71"/>
+      <c r="E31" s="72"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="74">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="169" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="87">
+      <c r="B32" s="170"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="56">
         <f>D27+D28+D29+D30+D31</f>
         <v>0</v>
       </c>
-      <c r="E32" s="87">
+      <c r="E32" s="56">
         <f t="shared" ref="E32:F32" si="1">E27+E28+E29+E30+E31</f>
         <v>0</v>
       </c>
-      <c r="F32" s="87">
+      <c r="F32" s="56">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G32" s="88">
+      <c r="G32" s="57">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="114"/>
-      <c r="B33" s="115"/>
-      <c r="C33" s="115"/>
-      <c r="D33" s="115"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="116"/>
+      <c r="A33" s="75"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="76"/>
+      <c r="E33" s="76"/>
+      <c r="F33" s="76"/>
+      <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="117" t="s">
+      <c r="A34" s="171" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="118"/>
-      <c r="C34" s="119"/>
-      <c r="D34" s="120"/>
-      <c r="E34" s="121"/>
-      <c r="F34" s="122"/>
-      <c r="G34" s="123"/>
+      <c r="B34" s="172"/>
+      <c r="C34" s="173"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="81"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="124" t="s">
+      <c r="A35" s="145" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="125"/>
-      <c r="C35" s="126"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="127">
+      <c r="B35" s="146"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="83">
         <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="124" t="s">
+      <c r="A36" s="145" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="125"/>
-      <c r="C36" s="126"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="43"/>
-      <c r="G36" s="127">
+      <c r="B36" s="146"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="33"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="83">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="124" t="s">
+      <c r="A37" s="145" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="125"/>
-      <c r="C37" s="126"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="43"/>
-      <c r="F37" s="43"/>
-      <c r="G37" s="127">
+      <c r="B37" s="146"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="83">
         <v>16</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="128" t="s">
+      <c r="A38" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="129"/>
-      <c r="C38" s="130"/>
-      <c r="D38" s="51"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="127">
+      <c r="B38" s="148"/>
+      <c r="C38" s="84"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="83">
         <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="128" t="s">
+      <c r="A39" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="129"/>
-      <c r="C39" s="130"/>
-      <c r="D39" s="51"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="127">
+      <c r="B39" s="148"/>
+      <c r="C39" s="84"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="83">
         <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="131" t="s">
+      <c r="A40" s="149" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="132"/>
-      <c r="C40" s="133"/>
-      <c r="D40" s="134"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="56"/>
-      <c r="G40" s="127">
+      <c r="B40" s="150"/>
+      <c r="C40" s="85"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="83">
         <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="135" t="s">
+      <c r="A41" s="151" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="136"/>
-      <c r="C41" s="137"/>
-      <c r="D41" s="138">
+      <c r="B41" s="152"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="88">
         <f>D35+D37+D38+D36</f>
         <v>0</v>
       </c>
-      <c r="E41" s="138">
+      <c r="E41" s="88">
         <f t="shared" ref="E41:F41" si="2">E34+E35+E36+E37+E38+E39+E40</f>
         <v>0</v>
       </c>
-      <c r="F41" s="138">
+      <c r="F41" s="88">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G41" s="139">
+      <c r="G41" s="89">
         <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="8.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="140"/>
-      <c r="B42" s="141"/>
-      <c r="C42" s="141"/>
-      <c r="D42" s="141"/>
-      <c r="E42" s="141"/>
-      <c r="F42" s="141"/>
-      <c r="G42" s="116"/>
+      <c r="A42" s="90"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="91"/>
+      <c r="D42" s="91"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="77"/>
     </row>
     <row r="43" spans="1:7" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="142" t="s">
+      <c r="A43" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B43" s="143"/>
-      <c r="C43" s="143"/>
-      <c r="D43" s="143"/>
-      <c r="E43" s="143"/>
-      <c r="F43" s="143"/>
-      <c r="G43" s="144"/>
+      <c r="B43" s="93"/>
+      <c r="C43" s="93"/>
+      <c r="D43" s="93"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="93"/>
+      <c r="G43" s="94"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="89" t="s">
+      <c r="A44" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="145">
+      <c r="B44" s="154"/>
+      <c r="C44" s="95">
         <v>2</v>
       </c>
-      <c r="D44" s="146">
+      <c r="D44" s="96">
         <f>D32-D41</f>
         <v>0</v>
       </c>
-      <c r="E44" s="146">
+      <c r="E44" s="96">
         <f t="shared" ref="E44:F44" si="3">E32-E41</f>
         <v>0</v>
       </c>
-      <c r="F44" s="146">
+      <c r="F44" s="96">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G44" s="94">
+      <c r="G44" s="61">
         <v>21</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="147" t="s">
+      <c r="A45" s="155" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="148"/>
-      <c r="C45" s="149">
+      <c r="B45" s="156"/>
+      <c r="C45" s="97">
         <f>C44</f>
         <v>2</v>
       </c>
-      <c r="D45" s="56"/>
-      <c r="E45" s="56"/>
-      <c r="F45" s="56"/>
-      <c r="G45" s="150">
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="98">
         <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="151" t="s">
+      <c r="A46" s="157" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="152"/>
-      <c r="C46" s="153"/>
-      <c r="D46" s="154">
+      <c r="B46" s="158"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="100">
         <f>D44-D45</f>
         <v>0</v>
       </c>
-      <c r="E46" s="154"/>
-      <c r="F46" s="154"/>
-      <c r="G46" s="88">
+      <c r="E46" s="100"/>
+      <c r="F46" s="100"/>
+      <c r="G46" s="57">
         <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="155"/>
-      <c r="B47" s="156"/>
-      <c r="C47" s="157"/>
-      <c r="D47" s="157"/>
-      <c r="E47" s="157"/>
-      <c r="F47" s="157"/>
-      <c r="G47" s="158"/>
+      <c r="A47" s="101"/>
+      <c r="B47" s="102"/>
+      <c r="C47" s="103"/>
+      <c r="D47" s="103"/>
+      <c r="E47" s="103"/>
+      <c r="F47" s="103"/>
+      <c r="G47" s="104"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="159" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="160"/>
-      <c r="C48" s="160"/>
-      <c r="D48" s="160"/>
-      <c r="E48" s="160"/>
-      <c r="F48" s="160"/>
-      <c r="G48" s="161"/>
+      <c r="A48" s="142" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" s="143"/>
+      <c r="C48" s="143"/>
+      <c r="D48" s="143"/>
+      <c r="E48" s="143"/>
+      <c r="F48" s="143"/>
+      <c r="G48" s="144"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="162" t="s">
+      <c r="A49" s="121" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="163" t="s">
+      <c r="B49" s="115" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="164"/>
-      <c r="D49" s="165" t="s">
+      <c r="C49" s="117"/>
+      <c r="D49" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="166"/>
-      <c r="F49" s="167" t="s">
+      <c r="E49" s="135"/>
+      <c r="F49" s="134" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="166"/>
+      <c r="G49" s="135"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="168"/>
-      <c r="B50" s="169" t="s">
+      <c r="A50" s="126"/>
+      <c r="B50" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="170"/>
-      <c r="D50" s="169"/>
-      <c r="E50" s="170"/>
-      <c r="F50" s="171"/>
-      <c r="G50" s="170"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="137"/>
+      <c r="E50" s="139"/>
+      <c r="F50" s="138"/>
+      <c r="G50" s="139"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="172"/>
-      <c r="B51" s="173"/>
-      <c r="C51" s="174"/>
-      <c r="D51" s="173"/>
-      <c r="E51" s="174"/>
-      <c r="F51" s="175"/>
-      <c r="G51" s="176"/>
+      <c r="A51" s="122"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="132"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="132"/>
+      <c r="F51" s="140"/>
+      <c r="G51" s="141"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="177" t="s">
+      <c r="A52" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="178"/>
-      <c r="C52" s="178"/>
-      <c r="D52" s="178"/>
-      <c r="E52" s="178"/>
-      <c r="F52" s="178"/>
-      <c r="G52" s="179"/>
+      <c r="B52" s="124"/>
+      <c r="C52" s="124"/>
+      <c r="D52" s="124"/>
+      <c r="E52" s="124"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="125"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="162" t="s">
+      <c r="A53" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="165" t="s">
+      <c r="B53" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="167"/>
-      <c r="D53" s="166"/>
-      <c r="E53" s="167" t="s">
+      <c r="C53" s="134"/>
+      <c r="D53" s="135"/>
+      <c r="E53" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="167"/>
-      <c r="G53" s="166"/>
+      <c r="F53" s="134"/>
+      <c r="G53" s="135"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="168"/>
-      <c r="B54" s="169"/>
-      <c r="C54" s="171"/>
-      <c r="D54" s="170"/>
-      <c r="E54" s="171"/>
-      <c r="F54" s="171"/>
-      <c r="G54" s="170"/>
+      <c r="A54" s="126"/>
+      <c r="B54" s="137"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="139"/>
+      <c r="E54" s="138"/>
+      <c r="F54" s="138"/>
+      <c r="G54" s="139"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="172"/>
-      <c r="B55" s="173"/>
-      <c r="C55" s="180"/>
-      <c r="D55" s="174"/>
-      <c r="E55" s="175"/>
-      <c r="F55" s="175"/>
-      <c r="G55" s="176"/>
+      <c r="A55" s="122"/>
+      <c r="B55" s="131"/>
+      <c r="C55" s="136"/>
+      <c r="D55" s="132"/>
+      <c r="E55" s="140"/>
+      <c r="F55" s="140"/>
+      <c r="G55" s="141"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="177" t="s">
+      <c r="A56" s="123" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="178"/>
-      <c r="C56" s="178"/>
-      <c r="D56" s="178"/>
-      <c r="E56" s="178"/>
-      <c r="F56" s="178"/>
-      <c r="G56" s="179"/>
+      <c r="B56" s="124"/>
+      <c r="C56" s="124"/>
+      <c r="D56" s="124"/>
+      <c r="E56" s="124"/>
+      <c r="F56" s="124"/>
+      <c r="G56" s="125"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="162" t="s">
+      <c r="A57" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="181" t="s">
+      <c r="B57" s="127" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="182"/>
-      <c r="D57" s="181" t="s">
+      <c r="C57" s="128"/>
+      <c r="D57" s="127" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="182"/>
-      <c r="F57" s="181" t="s">
+      <c r="E57" s="128"/>
+      <c r="F57" s="127" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="182"/>
+      <c r="G57" s="128"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="168"/>
-      <c r="B58" s="183"/>
-      <c r="C58" s="184"/>
-      <c r="D58" s="185"/>
-      <c r="E58" s="186"/>
-      <c r="F58" s="187"/>
-      <c r="G58" s="188"/>
+      <c r="A58" s="126"/>
+      <c r="B58" s="105"/>
+      <c r="C58" s="106"/>
+      <c r="D58" s="129"/>
+      <c r="E58" s="130"/>
+      <c r="F58" s="108"/>
+      <c r="G58" s="107"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="168"/>
-      <c r="B59" s="173" t="s">
+      <c r="A59" s="126"/>
+      <c r="B59" s="131" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="174"/>
-      <c r="D59" s="189" t="s">
+      <c r="C59" s="132"/>
+      <c r="D59" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="190"/>
-      <c r="F59" s="191" t="s">
+      <c r="E59" s="120"/>
+      <c r="F59" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="190"/>
+      <c r="G59" s="120"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="168"/>
-      <c r="B60" s="165" t="s">
+      <c r="A60" s="126"/>
+      <c r="B60" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="167"/>
-      <c r="D60" s="166"/>
-      <c r="E60" s="163" t="s">
+      <c r="C60" s="134"/>
+      <c r="D60" s="135"/>
+      <c r="E60" s="115" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="192"/>
-      <c r="G60" s="164"/>
+      <c r="F60" s="116"/>
+      <c r="G60" s="117"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="168"/>
-      <c r="B61" s="193"/>
-      <c r="C61" s="194"/>
-      <c r="D61" s="184"/>
-      <c r="E61" s="195"/>
-      <c r="F61" s="196"/>
-      <c r="G61" s="184"/>
+      <c r="A61" s="126"/>
+      <c r="B61" s="109"/>
+      <c r="C61" s="110"/>
+      <c r="D61" s="106"/>
+      <c r="E61" s="111"/>
+      <c r="F61" s="112"/>
+      <c r="G61" s="106"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="172"/>
-      <c r="B62" s="173" t="s">
+      <c r="A62" s="122"/>
+      <c r="B62" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="180"/>
-      <c r="D62" s="174"/>
-      <c r="E62" s="189" t="s">
+      <c r="C62" s="136"/>
+      <c r="D62" s="132"/>
+      <c r="E62" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="191"/>
-      <c r="G62" s="190"/>
+      <c r="F62" s="119"/>
+      <c r="G62" s="120"/>
     </row>
     <row r="63" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="162" t="s">
+      <c r="A63" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="163" t="s">
+      <c r="B63" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="192"/>
-      <c r="D63" s="164"/>
-      <c r="E63" s="163" t="s">
+      <c r="C63" s="116"/>
+      <c r="D63" s="117"/>
+      <c r="E63" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="192"/>
-      <c r="G63" s="164"/>
+      <c r="F63" s="116"/>
+      <c r="G63" s="117"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="172"/>
-      <c r="B64" s="189" t="s">
+      <c r="A64" s="122"/>
+      <c r="B64" s="118" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="191"/>
-      <c r="D64" s="190"/>
-      <c r="E64" s="189" t="s">
+      <c r="C64" s="119"/>
+      <c r="D64" s="120"/>
+      <c r="E64" s="118" t="s">
         <v>0</v>
       </c>
-      <c r="F64" s="191"/>
-      <c r="G64" s="190"/>
+      <c r="F64" s="119"/>
+      <c r="G64" s="120"/>
     </row>
     <row r="65" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="197"/>
-      <c r="B65" s="197"/>
-      <c r="C65" s="197"/>
-      <c r="D65" s="197"/>
-      <c r="E65" s="197"/>
-      <c r="F65" s="197"/>
-      <c r="G65" s="197"/>
+      <c r="A65" s="114"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="114"/>
+      <c r="D65" s="114"/>
+      <c r="E65" s="114"/>
+      <c r="F65" s="114"/>
+      <c r="G65" s="114"/>
     </row>
     <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="199" t="str">
+      <c r="A66" s="182" t="str">
         <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
-        <v>Generated by Autodesk Construction Cloud on: 04 March 2025</v>
-      </c>
-      <c r="B66" s="199"/>
-      <c r="C66" s="199"/>
-      <c r="D66" s="199"/>
-      <c r="E66" s="199"/>
-      <c r="F66" s="199"/>
+        <v>Generated by Autodesk Construction Cloud on: 06 March 2025</v>
+      </c>
+      <c r="B66" s="182"/>
+      <c r="C66" s="182"/>
+      <c r="D66" s="182"/>
+      <c r="E66" s="182"/>
+      <c r="F66" s="182"/>
     </row>
     <row r="70" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D70" s="8"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E71" s="198"/>
+      <c r="E71" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="83">
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:F3"/>
     <mergeCell ref="A66:F66"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
@@ -3463,6 +3399,73 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:F3"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: reorganize file paths and enhance API token handling in ACCAPI
</commit_message>
<xml_diff>
--- a/templates/cost_cover_template.xlsx
+++ b/templates/cost_cover_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Work\Square\PDF Automater\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53001889-BC85-4BF3-B323-0FF7BF2FB258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCC3612-70DD-45A6-9515-3B6DE071649F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{489EC8E5-F2B0-4D62-96BA-77282DF98E55}"/>
   </bookViews>
@@ -1756,98 +1756,113 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="2" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="75" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -1855,60 +1870,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="38" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="37" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1919,12 +1880,6 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1936,83 +1891,128 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="4" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="75" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="40" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="39" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="5" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2498,8 +2498,8 @@
   </sheetPr>
   <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScale="58" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H57" sqref="H57"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" topLeftCell="A43" zoomScale="58" zoomScaleNormal="100" zoomScaleSheetLayoutView="72" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46:F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2524,47 +2524,47 @@
       <c r="A1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="179" t="s">
+      <c r="B1" s="139" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="179"/>
-      <c r="D1" s="180"/>
-      <c r="E1" s="180"/>
+      <c r="C1" s="139"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
     </row>
     <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="139" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="179"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-      <c r="F2" s="181"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="141"/>
+      <c r="E2" s="141"/>
+      <c r="F2" s="141"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="179" t="s">
+      <c r="B3" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="179"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="141"/>
+      <c r="E3" s="141"/>
+      <c r="F3" s="141"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="138" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="178"/>
+      <c r="C4" s="138"/>
       <c r="E4" s="6" t="s">
         <v>69</v>
       </c>
@@ -2592,27 +2592,27 @@
       </c>
       <c r="F6" s="15" t="str">
         <f ca="1">TEXT(TODAY(), "[$-ar-SA]dd mmmm yyyy")</f>
-        <v>06 مارس 2025</v>
+        <v>19 مارس 2025</v>
       </c>
       <c r="G6" s="16"/>
     </row>
     <row r="7" spans="1:7" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="183" t="s">
+      <c r="A7" s="117" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="184"/>
+      <c r="B7" s="118"/>
       <c r="C7" s="17"/>
-      <c r="D7" s="185" t="s">
+      <c r="D7" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="184"/>
-      <c r="F7" s="186"/>
-      <c r="G7" s="187"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="121"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="188"/>
-      <c r="B8" s="189"/>
-      <c r="C8" s="190"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="18" t="s">
         <v>56</v>
       </c>
@@ -2625,21 +2625,21 @@
       <c r="G8" s="21"/>
     </row>
     <row r="9" spans="1:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="191" t="s">
+      <c r="A9" s="125" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="192"/>
-      <c r="C9" s="193"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="127"/>
       <c r="D9" s="22"/>
       <c r="E9" s="23"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="194" t="s">
+      <c r="A10" s="128" t="s">
         <v>64</v>
       </c>
-      <c r="B10" s="195"/>
+      <c r="B10" s="129"/>
       <c r="C10" s="24"/>
       <c r="D10" s="25"/>
       <c r="E10" s="26"/>
@@ -2647,10 +2647,10 @@
       <c r="G10" s="28"/>
     </row>
     <row r="11" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="174" t="s">
+      <c r="A11" s="130" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="175"/>
+      <c r="B11" s="131"/>
       <c r="C11" s="30"/>
       <c r="D11" s="26"/>
       <c r="E11" s="26"/>
@@ -2658,10 +2658,10 @@
       <c r="G11" s="28"/>
     </row>
     <row r="12" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="174" t="s">
+      <c r="A12" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="175"/>
+      <c r="B12" s="131"/>
       <c r="C12" s="30"/>
       <c r="D12" s="26"/>
       <c r="E12" s="26"/>
@@ -2669,10 +2669,10 @@
       <c r="G12" s="28"/>
     </row>
     <row r="13" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="174" t="s">
+      <c r="A13" s="130" t="s">
         <v>66</v>
       </c>
-      <c r="B13" s="175"/>
+      <c r="B13" s="131"/>
       <c r="C13" s="31"/>
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
@@ -2680,10 +2680,10 @@
       <c r="G13" s="28"/>
     </row>
     <row r="14" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="174" t="s">
+      <c r="A14" s="130" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="175"/>
+      <c r="B14" s="131"/>
       <c r="C14" s="32"/>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
@@ -2691,10 +2691,10 @@
       <c r="G14" s="28"/>
     </row>
     <row r="15" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="174" t="s">
+      <c r="A15" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="175"/>
+      <c r="B15" s="131"/>
       <c r="C15" s="32"/>
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
@@ -2702,10 +2702,10 @@
       <c r="G15" s="34"/>
     </row>
     <row r="16" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="115" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="160"/>
+      <c r="B16" s="116"/>
       <c r="C16" s="35" t="s">
         <v>38</v>
       </c>
@@ -2715,10 +2715,10 @@
       <c r="G16" s="34"/>
     </row>
     <row r="17" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="169" t="s">
+      <c r="A17" s="132" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="170"/>
+      <c r="B17" s="133"/>
       <c r="C17" s="37"/>
       <c r="D17" s="38">
         <f>D10+D13+D14+D15+D16</f>
@@ -2744,21 +2744,21 @@
       <c r="G18" s="42"/>
     </row>
     <row r="19" spans="1:7" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="196" t="s">
+      <c r="A19" s="134" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="197"/>
-      <c r="C19" s="197"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="135"/>
       <c r="D19" s="43"/>
       <c r="E19" s="44"/>
       <c r="F19" s="43"/>
       <c r="G19" s="45"/>
     </row>
     <row r="20" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="198" t="s">
+      <c r="A20" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="199"/>
+      <c r="B20" s="137"/>
       <c r="C20" s="46"/>
       <c r="D20" s="26"/>
       <c r="E20" s="26"/>
@@ -2768,10 +2768,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="176" t="s">
+      <c r="A21" s="142" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="177"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="48"/>
       <c r="D21" s="26"/>
       <c r="E21" s="49"/>
@@ -2781,10 +2781,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="174" t="s">
+      <c r="A22" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="175"/>
+      <c r="B22" s="131"/>
       <c r="C22" s="51"/>
       <c r="D22" s="26"/>
       <c r="E22" s="49"/>
@@ -2794,10 +2794,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="174" t="s">
+      <c r="A23" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="B23" s="175"/>
+      <c r="B23" s="131"/>
       <c r="C23" s="29"/>
       <c r="D23" s="26"/>
       <c r="E23" s="26"/>
@@ -2807,10 +2807,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="174" t="s">
+      <c r="A24" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="175"/>
+      <c r="B24" s="131"/>
       <c r="C24" s="29"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
@@ -2820,10 +2820,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="174" t="s">
+      <c r="A25" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="175"/>
+      <c r="B25" s="131"/>
       <c r="C25" s="52"/>
       <c r="D25" s="26"/>
       <c r="E25" s="26"/>
@@ -2833,10 +2833,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="159" t="s">
+      <c r="A26" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="160"/>
+      <c r="B26" s="116"/>
       <c r="C26" s="53"/>
       <c r="D26" s="54"/>
       <c r="E26" s="54"/>
@@ -2846,10 +2846,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="161" t="s">
+      <c r="A27" s="144" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="162"/>
+      <c r="B27" s="145"/>
       <c r="C27" s="55"/>
       <c r="D27" s="56">
         <f>D20+D24+D25+D26</f>
@@ -2868,10 +2868,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="153" t="s">
+      <c r="A28" s="146" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="154"/>
+      <c r="B28" s="147"/>
       <c r="C28" s="58"/>
       <c r="D28" s="59"/>
       <c r="E28" s="60"/>
@@ -2881,10 +2881,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="163" t="s">
+      <c r="A29" s="148" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="164"/>
+      <c r="B29" s="149"/>
       <c r="C29" s="62"/>
       <c r="D29" s="63"/>
       <c r="E29" s="64"/>
@@ -2894,10 +2894,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="165" t="s">
+      <c r="A30" s="152" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="166"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="66"/>
       <c r="D30" s="67"/>
       <c r="E30" s="68"/>
@@ -2907,10 +2907,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="167" t="s">
+      <c r="A31" s="154" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="168"/>
+      <c r="B31" s="155"/>
       <c r="C31" s="70" t="s">
         <v>38</v>
       </c>
@@ -2922,10 +2922,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="169" t="s">
+      <c r="A32" s="132" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="170"/>
+      <c r="B32" s="133"/>
       <c r="C32" s="55"/>
       <c r="D32" s="56">
         <f>D27+D28+D29+D30+D31</f>
@@ -2953,21 +2953,21 @@
       <c r="G33" s="77"/>
     </row>
     <row r="34" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="171" t="s">
+      <c r="A34" s="156" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="172"/>
-      <c r="C34" s="173"/>
+      <c r="B34" s="157"/>
+      <c r="C34" s="158"/>
       <c r="D34" s="78"/>
       <c r="E34" s="79"/>
       <c r="F34" s="80"/>
       <c r="G34" s="81"/>
     </row>
     <row r="35" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="145" t="s">
+      <c r="A35" s="150" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="146"/>
+      <c r="B35" s="151"/>
       <c r="C35" s="82"/>
       <c r="D35" s="33"/>
       <c r="E35" s="26"/>
@@ -2977,10 +2977,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="145" t="s">
+      <c r="A36" s="150" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="146"/>
+      <c r="B36" s="151"/>
       <c r="C36" s="82"/>
       <c r="D36" s="33"/>
       <c r="E36" s="26"/>
@@ -2990,10 +2990,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="145" t="s">
+      <c r="A37" s="150" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="146"/>
+      <c r="B37" s="151"/>
       <c r="C37" s="82"/>
       <c r="D37" s="33"/>
       <c r="E37" s="26"/>
@@ -3003,10 +3003,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A38" s="147" t="s">
+      <c r="A38" s="162" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="148"/>
+      <c r="B38" s="163"/>
       <c r="C38" s="84"/>
       <c r="D38" s="33"/>
       <c r="E38" s="26"/>
@@ -3016,10 +3016,10 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="147" t="s">
+      <c r="A39" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="148"/>
+      <c r="B39" s="163"/>
       <c r="C39" s="84"/>
       <c r="D39" s="33"/>
       <c r="E39" s="26"/>
@@ -3029,10 +3029,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A40" s="149" t="s">
+      <c r="A40" s="164" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="150"/>
+      <c r="B40" s="165"/>
       <c r="C40" s="85"/>
       <c r="D40" s="86"/>
       <c r="E40" s="36"/>
@@ -3042,10 +3042,10 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="151" t="s">
+      <c r="A41" s="166" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="152"/>
+      <c r="B41" s="167"/>
       <c r="C41" s="87"/>
       <c r="D41" s="88">
         <f>D35+D37+D38+D36</f>
@@ -3084,10 +3084,10 @@
       <c r="G43" s="94"/>
     </row>
     <row r="44" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="153" t="s">
+      <c r="A44" s="146" t="s">
         <v>27</v>
       </c>
-      <c r="B44" s="154"/>
+      <c r="B44" s="147"/>
       <c r="C44" s="95">
         <v>2</v>
       </c>
@@ -3108,10 +3108,10 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="155" t="s">
+      <c r="A45" s="168" t="s">
         <v>72</v>
       </c>
-      <c r="B45" s="156"/>
+      <c r="B45" s="169"/>
       <c r="C45" s="97">
         <f>C44</f>
         <v>2</v>
@@ -3124,17 +3124,23 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="35.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="157" t="s">
+      <c r="A46" s="170" t="s">
         <v>26</v>
       </c>
-      <c r="B46" s="158"/>
+      <c r="B46" s="171"/>
       <c r="C46" s="99"/>
       <c r="D46" s="100">
         <f>D44-D45</f>
         <v>0</v>
       </c>
-      <c r="E46" s="100"/>
-      <c r="F46" s="100"/>
+      <c r="E46" s="100">
+        <f t="shared" ref="E46:F46" si="4">E44-E45</f>
+        <v>0</v>
+      </c>
+      <c r="F46" s="100">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G46" s="57">
         <v>23</v>
       </c>
@@ -3149,164 +3155,164 @@
       <c r="G47" s="104"/>
     </row>
     <row r="48" spans="1:7" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="142" t="s">
+      <c r="A48" s="159" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="143"/>
-      <c r="C48" s="143"/>
-      <c r="D48" s="143"/>
-      <c r="E48" s="143"/>
-      <c r="F48" s="143"/>
-      <c r="G48" s="144"/>
+      <c r="B48" s="160"/>
+      <c r="C48" s="160"/>
+      <c r="D48" s="160"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="160"/>
+      <c r="G48" s="161"/>
     </row>
     <row r="49" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="172" t="s">
         <v>24</v>
       </c>
-      <c r="B49" s="115" t="s">
+      <c r="B49" s="175" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="117"/>
-      <c r="D49" s="133" t="s">
+      <c r="C49" s="176"/>
+      <c r="D49" s="177" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="135"/>
-      <c r="F49" s="134" t="s">
+      <c r="E49" s="178"/>
+      <c r="F49" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="G49" s="135"/>
+      <c r="G49" s="178"/>
     </row>
     <row r="50" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="126"/>
-      <c r="B50" s="137" t="s">
+      <c r="A50" s="173"/>
+      <c r="B50" s="180" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="139"/>
-      <c r="D50" s="137"/>
-      <c r="E50" s="139"/>
-      <c r="F50" s="138"/>
-      <c r="G50" s="139"/>
+      <c r="C50" s="181"/>
+      <c r="D50" s="180"/>
+      <c r="E50" s="181"/>
+      <c r="F50" s="182"/>
+      <c r="G50" s="181"/>
     </row>
     <row r="51" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A51" s="122"/>
-      <c r="B51" s="131"/>
-      <c r="C51" s="132"/>
-      <c r="D51" s="131"/>
-      <c r="E51" s="132"/>
-      <c r="F51" s="140"/>
-      <c r="G51" s="141"/>
+      <c r="A51" s="174"/>
+      <c r="B51" s="183"/>
+      <c r="C51" s="184"/>
+      <c r="D51" s="183"/>
+      <c r="E51" s="184"/>
+      <c r="F51" s="185"/>
+      <c r="G51" s="186"/>
     </row>
     <row r="52" spans="1:7" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A52" s="123" t="s">
+      <c r="A52" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="B52" s="124"/>
-      <c r="C52" s="124"/>
-      <c r="D52" s="124"/>
-      <c r="E52" s="124"/>
-      <c r="F52" s="124"/>
-      <c r="G52" s="125"/>
+      <c r="B52" s="188"/>
+      <c r="C52" s="188"/>
+      <c r="D52" s="188"/>
+      <c r="E52" s="188"/>
+      <c r="F52" s="188"/>
+      <c r="G52" s="189"/>
     </row>
     <row r="53" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="121" t="s">
+      <c r="A53" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="B53" s="133" t="s">
+      <c r="B53" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="134"/>
-      <c r="D53" s="135"/>
-      <c r="E53" s="134" t="s">
+      <c r="C53" s="179"/>
+      <c r="D53" s="178"/>
+      <c r="E53" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="134"/>
-      <c r="G53" s="135"/>
+      <c r="F53" s="179"/>
+      <c r="G53" s="178"/>
     </row>
     <row r="54" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="126"/>
-      <c r="B54" s="137"/>
-      <c r="C54" s="138"/>
-      <c r="D54" s="139"/>
-      <c r="E54" s="138"/>
-      <c r="F54" s="138"/>
-      <c r="G54" s="139"/>
+      <c r="A54" s="173"/>
+      <c r="B54" s="180"/>
+      <c r="C54" s="182"/>
+      <c r="D54" s="181"/>
+      <c r="E54" s="182"/>
+      <c r="F54" s="182"/>
+      <c r="G54" s="181"/>
     </row>
     <row r="55" spans="1:7" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="122"/>
-      <c r="B55" s="131"/>
-      <c r="C55" s="136"/>
-      <c r="D55" s="132"/>
-      <c r="E55" s="140"/>
-      <c r="F55" s="140"/>
-      <c r="G55" s="141"/>
+      <c r="A55" s="174"/>
+      <c r="B55" s="183"/>
+      <c r="C55" s="190"/>
+      <c r="D55" s="184"/>
+      <c r="E55" s="185"/>
+      <c r="F55" s="185"/>
+      <c r="G55" s="186"/>
     </row>
     <row r="56" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="123" t="s">
+      <c r="A56" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="B56" s="124"/>
-      <c r="C56" s="124"/>
-      <c r="D56" s="124"/>
-      <c r="E56" s="124"/>
-      <c r="F56" s="124"/>
-      <c r="G56" s="125"/>
+      <c r="B56" s="188"/>
+      <c r="C56" s="188"/>
+      <c r="D56" s="188"/>
+      <c r="E56" s="188"/>
+      <c r="F56" s="188"/>
+      <c r="G56" s="189"/>
     </row>
     <row r="57" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="121" t="s">
+      <c r="A57" s="172" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="127" t="s">
+      <c r="B57" s="191" t="s">
         <v>13</v>
       </c>
-      <c r="C57" s="128"/>
-      <c r="D57" s="127" t="s">
+      <c r="C57" s="192"/>
+      <c r="D57" s="191" t="s">
         <v>12</v>
       </c>
-      <c r="E57" s="128"/>
-      <c r="F57" s="127" t="s">
+      <c r="E57" s="192"/>
+      <c r="F57" s="191" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="128"/>
+      <c r="G57" s="192"/>
     </row>
     <row r="58" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="126"/>
+      <c r="A58" s="173"/>
       <c r="B58" s="105"/>
       <c r="C58" s="106"/>
-      <c r="D58" s="129"/>
-      <c r="E58" s="130"/>
+      <c r="D58" s="193"/>
+      <c r="E58" s="194"/>
       <c r="F58" s="108"/>
       <c r="G58" s="107"/>
     </row>
     <row r="59" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="126"/>
-      <c r="B59" s="131" t="s">
+      <c r="A59" s="173"/>
+      <c r="B59" s="183" t="s">
         <v>10</v>
       </c>
-      <c r="C59" s="132"/>
-      <c r="D59" s="118" t="s">
+      <c r="C59" s="184"/>
+      <c r="D59" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="120"/>
-      <c r="F59" s="119" t="s">
+      <c r="E59" s="196"/>
+      <c r="F59" s="197" t="s">
         <v>8</v>
       </c>
-      <c r="G59" s="120"/>
+      <c r="G59" s="196"/>
     </row>
     <row r="60" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="126"/>
-      <c r="B60" s="133" t="s">
+      <c r="A60" s="173"/>
+      <c r="B60" s="177" t="s">
         <v>3</v>
       </c>
-      <c r="C60" s="134"/>
-      <c r="D60" s="135"/>
-      <c r="E60" s="115" t="s">
+      <c r="C60" s="179"/>
+      <c r="D60" s="178"/>
+      <c r="E60" s="175" t="s">
         <v>7</v>
       </c>
-      <c r="F60" s="116"/>
-      <c r="G60" s="117"/>
+      <c r="F60" s="198"/>
+      <c r="G60" s="176"/>
     </row>
     <row r="61" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="126"/>
+      <c r="A61" s="173"/>
       <c r="B61" s="109"/>
       <c r="C61" s="110"/>
       <c r="D61" s="106"/>
@@ -3315,65 +3321,65 @@
       <c r="G61" s="106"/>
     </row>
     <row r="62" spans="1:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A62" s="122"/>
-      <c r="B62" s="131" t="s">
+      <c r="A62" s="174"/>
+      <c r="B62" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="C62" s="136"/>
-      <c r="D62" s="132"/>
-      <c r="E62" s="118" t="s">
+      <c r="C62" s="190"/>
+      <c r="D62" s="184"/>
+      <c r="E62" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="119"/>
-      <c r="G62" s="120"/>
+      <c r="F62" s="197"/>
+      <c r="G62" s="196"/>
     </row>
     <row r="63" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="121" t="s">
+      <c r="A63" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="115" t="s">
+      <c r="B63" s="175" t="s">
         <v>3</v>
       </c>
-      <c r="C63" s="116"/>
-      <c r="D63" s="117"/>
-      <c r="E63" s="115" t="s">
+      <c r="C63" s="198"/>
+      <c r="D63" s="176"/>
+      <c r="E63" s="175" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="116"/>
-      <c r="G63" s="117"/>
+      <c r="F63" s="198"/>
+      <c r="G63" s="176"/>
     </row>
     <row r="64" spans="1:7" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A64" s="122"/>
-      <c r="B64" s="118" t="s">
+      <c r="A64" s="174"/>
+      <c r="B64" s="195" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="119"/>
-      <c r="D64" s="120"/>
-      <c r="E64" s="118" t="s">
+      <c r="C64" s="197"/>
+      <c r="D64" s="196"/>
+      <c r="E64" s="195" t="s">
         <v>0</v>
       </c>
-      <c r="F64" s="119"/>
-      <c r="G64" s="120"/>
+      <c r="F64" s="197"/>
+      <c r="G64" s="196"/>
     </row>
     <row r="65" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="114"/>
-      <c r="B65" s="114"/>
-      <c r="C65" s="114"/>
-      <c r="D65" s="114"/>
-      <c r="E65" s="114"/>
-      <c r="F65" s="114"/>
-      <c r="G65" s="114"/>
+      <c r="A65" s="199"/>
+      <c r="B65" s="199"/>
+      <c r="C65" s="199"/>
+      <c r="D65" s="199"/>
+      <c r="E65" s="199"/>
+      <c r="F65" s="199"/>
+      <c r="G65" s="199"/>
     </row>
     <row r="66" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="182" t="str">
+      <c r="A66" s="114" t="str">
         <f ca="1">"Generated by Autodesk Construction Cloud on: " &amp; TEXT(TODAY(), "dd mmmm yyyy")</f>
-        <v>Generated by Autodesk Construction Cloud on: 06 March 2025</v>
-      </c>
-      <c r="B66" s="182"/>
-      <c r="C66" s="182"/>
-      <c r="D66" s="182"/>
-      <c r="E66" s="182"/>
-      <c r="F66" s="182"/>
+        <v>Generated by Autodesk Construction Cloud on: 19 March 2025</v>
+      </c>
+      <c r="B66" s="114"/>
+      <c r="C66" s="114"/>
+      <c r="D66" s="114"/>
+      <c r="E66" s="114"/>
+      <c r="F66" s="114"/>
     </row>
     <row r="70" spans="1:7" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D70" s="5"/>
@@ -3383,6 +3389,73 @@
     </row>
   </sheetData>
   <mergeCells count="83">
+    <mergeCell ref="A65:G65"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A56:G56"/>
+    <mergeCell ref="A57:A62"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="E60:G60"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="E62:G62"/>
+    <mergeCell ref="A52:G52"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="E53:G53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="E54:G54"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="E55:G55"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:F3"/>
     <mergeCell ref="A66:F66"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A7:B7"/>
@@ -3399,73 +3472,6 @@
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:B20"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:F3"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A48:G48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="A52:G52"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="E53:G53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="E54:G54"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="E55:G55"/>
-    <mergeCell ref="A56:G56"/>
-    <mergeCell ref="A57:A62"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="E60:G60"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="E62:G62"/>
-    <mergeCell ref="A65:G65"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="A63:A64"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>